<commit_message>
updated excel files, included pubs version
</commit_message>
<xml_diff>
--- a/chart-styles.xlsx
+++ b/chart-styles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="33700" windowHeight="23860" tabRatio="913"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="33700" windowHeight="23860" tabRatio="913" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="17" r:id="rId1"/>
@@ -1808,71 +1808,12 @@
     <xf numFmtId="0" fontId="52" fillId="3" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1882,47 +1823,20 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1949,6 +1863,92 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -2118,11 +2118,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1831758232"/>
-        <c:axId val="1881938552"/>
+        <c:axId val="1897263912"/>
+        <c:axId val="1896478232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1831758232"/>
+        <c:axId val="1897263912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2139,7 +2139,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1881938552"/>
+        <c:crossAx val="1896478232"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2147,7 +2147,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1881938552"/>
+        <c:axId val="1896478232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2174,7 +2174,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1831758232"/>
+        <c:crossAx val="1897263912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -4270,11 +4270,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1898653304"/>
-        <c:axId val="1898656424"/>
+        <c:axId val="1895213656"/>
+        <c:axId val="1824249864"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1898653304"/>
+        <c:axId val="1895213656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4284,7 +4284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1898656424"/>
+        <c:crossAx val="1824249864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4293,7 +4293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1898656424"/>
+        <c:axId val="1824249864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4304,7 +4304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1898653304"/>
+        <c:crossAx val="1895213656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4338,8 +4338,8 @@
     <a:p>
       <a:pPr>
         <a:defRPr sz="1200">
-          <a:latin typeface="Avenir Medium"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -4929,11 +4929,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="1881384808"/>
-        <c:axId val="1902897768"/>
+        <c:axId val="1823956712"/>
+        <c:axId val="1823488856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1881384808"/>
+        <c:axId val="1823956712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4956,19 +4956,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Avenir Medium"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Avenir Medium"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1902897768"/>
+        <c:crossAx val="1823488856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4976,7 +4969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1902897768"/>
+        <c:axId val="1823488856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5008,19 +5001,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Avenir Medium"/>
-                <a:ea typeface="Calibri"/>
-                <a:cs typeface="Avenir Medium"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1881384808"/>
+        <c:crossAx val="1823956712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5052,23 +5038,6 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Avenir Medium"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Avenir Medium"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -5091,9 +5060,9 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:latin typeface="Calibri"/>
+          <a:latin typeface="Lato Regular"/>
           <a:ea typeface="Calibri"/>
-          <a:cs typeface="Calibri"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -5664,11 +5633,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1814915800"/>
-        <c:axId val="1901461368"/>
+        <c:axId val="1819706200"/>
+        <c:axId val="1819358504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1814915800"/>
+        <c:axId val="1819706200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5678,7 +5647,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1901461368"/>
+        <c:crossAx val="1819358504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5686,7 +5655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1901461368"/>
+        <c:axId val="1819358504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5712,7 +5681,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1814915800"/>
+        <c:crossAx val="1819706200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5746,8 +5715,8 @@
     <a:p>
       <a:pPr>
         <a:defRPr sz="1200">
-          <a:latin typeface="Avenir Medium"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -7030,11 +6999,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1901074904"/>
-        <c:axId val="1901981480"/>
+        <c:axId val="1900559816"/>
+        <c:axId val="1900723800"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1901074904"/>
+        <c:axId val="1900559816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7044,7 +7013,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1901981480"/>
+        <c:crossAx val="1900723800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7052,7 +7021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1901981480"/>
+        <c:axId val="1900723800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7062,9 +7031,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -7083,15 +7050,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200">
-                <a:latin typeface="Avenir Medium"/>
-                <a:cs typeface="Avenir Medium"/>
-              </a:defRPr>
+              <a:defRPr sz="1100"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1901074904"/>
+        <c:crossAx val="1900559816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7114,10 +7078,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200">
-              <a:latin typeface="Avenir Medium"/>
-              <a:cs typeface="Avenir Medium"/>
-            </a:defRPr>
+            <a:defRPr sz="1200"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -7132,6 +7093,19 @@
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Lato Regular"/>
+          <a:cs typeface="Lato Regular"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -7162,9 +7136,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.122779370530307"/>
+          <c:x val="0.10306110679827"/>
           <c:y val="0.227054907905972"/>
-          <c:w val="0.843727562339859"/>
+          <c:w val="0.863445824553621"/>
           <c:h val="0.566776748809846"/>
         </c:manualLayout>
       </c:layout>
@@ -7194,20 +7168,6 @@
                   <c:y val="0.0431159873104896"/>
                 </c:manualLayout>
               </c:layout>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="1">
-                      <a:latin typeface="Lato Regular"/>
-                      <a:cs typeface="Lato Regular"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -7221,10 +7181,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr>
-                    <a:latin typeface="Lato Regular"/>
-                    <a:cs typeface="Lato Regular"/>
-                  </a:defRPr>
+                  <a:defRPr sz="1200" b="1"/>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -7385,20 +7342,6 @@
                   <c:y val="-0.0431159873104896"/>
                 </c:manualLayout>
               </c:layout>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="1">
-                      <a:latin typeface="Lato Regular"/>
-                      <a:cs typeface="Lato Regular"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -7412,10 +7355,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr>
-                    <a:latin typeface="Lato Regular"/>
-                    <a:cs typeface="Lato Regular"/>
-                  </a:defRPr>
+                  <a:defRPr sz="1200" b="1"/>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -7502,11 +7442,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1898744328"/>
-        <c:axId val="1898747672"/>
+        <c:axId val="1833119096"/>
+        <c:axId val="2070831176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1898744328"/>
+        <c:axId val="1833119096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7529,12 +7469,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1100"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1898747672"/>
+        <c:crossAx val="2070831176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7542,7 +7482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1898747672"/>
+        <c:axId val="2070831176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.3E7"/>
@@ -7576,12 +7516,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1100"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1898744328"/>
+        <c:crossAx val="1833119096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7612,8 +7552,8 @@
     <a:p>
       <a:pPr>
         <a:defRPr>
-          <a:latin typeface="Avenir Medium"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -7650,9 +7590,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0584645669291338"/>
+          <c:x val="0.0441788526434196"/>
           <c:y val="0.212962962962963"/>
-          <c:w val="0.897631496062992"/>
+          <c:w val="0.911917210348707"/>
           <c:h val="0.585702151404303"/>
         </c:manualLayout>
       </c:layout>
@@ -7955,11 +7895,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1898357256"/>
-        <c:axId val="2070888936"/>
+        <c:axId val="1880038616"/>
+        <c:axId val="1879650088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1898357256"/>
+        <c:axId val="1880038616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7969,7 +7909,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070888936"/>
+        <c:crossAx val="1879650088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7977,7 +7917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2070888936"/>
+        <c:axId val="1879650088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7994,7 +7934,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8003,9 +7943,9 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1898357256"/>
+        <c:crossAx val="1880038616"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -8023,8 +7963,8 @@
     <a:p>
       <a:pPr>
         <a:defRPr sz="1200">
-          <a:latin typeface="Avenir Medium"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -8223,9 +8163,9 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:latin typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
           <a:ea typeface="Calibri"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -8371,11 +8311,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2079713800"/>
-        <c:axId val="2079658216"/>
+        <c:axId val="1835568040"/>
+        <c:axId val="1817440600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2079713800"/>
+        <c:axId val="1835568040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8385,7 +8325,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079658216"/>
+        <c:crossAx val="1817440600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8393,7 +8333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079658216"/>
+        <c:axId val="1817440600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8403,7 +8343,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079713800"/>
+        <c:crossAx val="1835568040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8436,9 +8376,9 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:latin typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
           <a:ea typeface="Calibri"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -8699,8 +8639,8 @@
     <a:p>
       <a:pPr>
         <a:defRPr sz="1200">
-          <a:latin typeface="Avenir Medium"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -8828,11 +8768,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1893995272"/>
-        <c:axId val="1898309944"/>
+        <c:axId val="2130063576"/>
+        <c:axId val="2130430024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1893995272"/>
+        <c:axId val="2130063576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8841,7 +8781,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1898309944"/>
+        <c:crossAx val="2130430024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8849,7 +8789,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1898309944"/>
+        <c:axId val="2130430024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8875,7 +8815,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1893995272"/>
+        <c:crossAx val="2130063576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8895,8 +8835,8 @@
     <a:p>
       <a:pPr>
         <a:defRPr sz="1200">
-          <a:latin typeface="Avenir Medium"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -9029,11 +8969,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1831024312"/>
-        <c:axId val="1902803304"/>
+        <c:axId val="1860342952"/>
+        <c:axId val="1860336312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1831024312"/>
+        <c:axId val="1860342952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9050,7 +8990,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1902803304"/>
+        <c:crossAx val="1860336312"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9058,7 +8998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1902803304"/>
+        <c:axId val="1860336312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -9070,7 +9010,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1831024312"/>
+        <c:crossAx val="1860342952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -9301,11 +9241,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1898559720"/>
-        <c:axId val="1898563032"/>
+        <c:axId val="1902775992"/>
+        <c:axId val="1884616040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1898559720"/>
+        <c:axId val="1902775992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9322,7 +9262,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1898563032"/>
+        <c:crossAx val="1884616040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9330,7 +9270,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1898563032"/>
+        <c:axId val="1884616040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-20.0"/>
@@ -9357,7 +9297,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1898559720"/>
+        <c:crossAx val="1902775992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -9656,11 +9596,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1898513640"/>
-        <c:axId val="1898516648"/>
+        <c:axId val="1861801064"/>
+        <c:axId val="1860415768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1898513640"/>
+        <c:axId val="1861801064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9679,7 +9619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1898516648"/>
+        <c:crossAx val="1860415768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9687,7 +9627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1898516648"/>
+        <c:axId val="1860415768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9713,7 +9653,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1898513640"/>
+        <c:crossAx val="1861801064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10138,11 +10078,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="30"/>
-        <c:axId val="1898460856"/>
-        <c:axId val="1894506232"/>
+        <c:axId val="1884997192"/>
+        <c:axId val="1885021784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1898460856"/>
+        <c:axId val="1884997192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10170,7 +10110,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1894506232"/>
+        <c:crossAx val="1885021784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10180,7 +10120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1894506232"/>
+        <c:axId val="1885021784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -10192,7 +10132,7 @@
           <c:spPr>
             <a:ln w="3175">
               <a:solidFill>
-                <a:srgbClr val="C0C0C0"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -10217,7 +10157,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1898460856"/>
+        <c:crossAx val="1884997192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -10478,7 +10418,7 @@
                   <c:v>5.0718</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.154199999999994</c:v>
+                  <c:v>6.154199999999993</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7.2366</c:v>
@@ -11215,11 +11155,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1897968424"/>
-        <c:axId val="1897971736"/>
+        <c:axId val="1896365352"/>
+        <c:axId val="1885524136"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1897968424"/>
+        <c:axId val="1896365352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11247,7 +11187,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1897971736"/>
+        <c:crossAx val="1885524136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11257,7 +11197,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1897971736"/>
+        <c:axId val="1885524136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11337,7 +11277,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1897968424"/>
+        <c:crossAx val="1896365352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
@@ -12386,11 +12326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1894740664"/>
-        <c:axId val="1898071816"/>
+        <c:axId val="1879802344"/>
+        <c:axId val="1879494760"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1894740664"/>
+        <c:axId val="1879802344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12418,7 +12358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1898071816"/>
+        <c:crossAx val="1879494760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12428,7 +12368,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1898071816"/>
+        <c:axId val="1879494760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12438,9 +12378,7 @@
           <c:spPr>
             <a:ln w="3175">
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="65000"/>
-                </a:schemeClr>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -12466,7 +12404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1894740664"/>
+        <c:crossAx val="1879802344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -12500,9 +12438,9 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:latin typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
           <a:ea typeface="Arial"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -13435,8 +13373,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1898869640"/>
-        <c:axId val="1898873032"/>
+        <c:axId val="1833138168"/>
+        <c:axId val="1832925048"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13709,11 +13647,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1898869640"/>
-        <c:axId val="1898873032"/>
+        <c:axId val="1833138168"/>
+        <c:axId val="1832925048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1898869640"/>
+        <c:axId val="1833138168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13741,7 +13679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1898873032"/>
+        <c:crossAx val="1832925048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13751,7 +13689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1898873032"/>
+        <c:axId val="1832925048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13789,7 +13727,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1898869640"/>
+        <c:crossAx val="1833138168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -13823,9 +13761,9 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:latin typeface="Avenir Medium"/>
+          <a:latin typeface="Lato Regular"/>
           <a:ea typeface="Arial"/>
-          <a:cs typeface="Avenir Medium"/>
+          <a:cs typeface="Lato Regular"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -14765,8 +14703,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115815448"/>
-        <c:axId val="1895078792"/>
+        <c:axId val="1823767208"/>
+        <c:axId val="1824068296"/>
       </c:areaChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -14838,11 +14776,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2115815448"/>
-        <c:axId val="1895078792"/>
+        <c:axId val="1823767208"/>
+        <c:axId val="1824068296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115815448"/>
+        <c:axId val="1823767208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14852,7 +14790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1895078792"/>
+        <c:crossAx val="1824068296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14862,7 +14800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1895078792"/>
+        <c:axId val="1824068296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -14889,7 +14827,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2115815448"/>
+        <c:crossAx val="1823767208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -28763,7 +28701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -34617,8 +34555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX276"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="11" customHeight="1" x14ac:dyDescent="0"/>
@@ -40760,8 +40698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="V88" sqref="V88"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="V68" sqref="V68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -40897,7 +40835,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="S71" sqref="S71"/>
+      <selection activeCell="X80" sqref="X80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -40966,20 +40904,20 @@
     </row>
     <row r="4" spans="1:11" s="60" customFormat="1" ht="13"/>
     <row r="5" spans="1:11" s="60" customFormat="1" ht="13">
-      <c r="A5" s="143" t="s">
+      <c r="A5" s="176" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="143"/>
-      <c r="C5" s="143"/>
-      <c r="D5" s="143"/>
-      <c r="E5" s="143"/>
+      <c r="B5" s="176"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
     </row>
     <row r="6" spans="1:11" s="60" customFormat="1" ht="13">
-      <c r="A6" s="144"/>
-      <c r="B6" s="144"/>
-      <c r="C6" s="144"/>
-      <c r="D6" s="144"/>
-      <c r="E6" s="144"/>
+      <c r="A6" s="177"/>
+      <c r="B6" s="177"/>
+      <c r="C6" s="177"/>
+      <c r="D6" s="177"/>
+      <c r="E6" s="177"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -40999,7 +40937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
@@ -41531,132 +41469,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" s="14" customFormat="1" ht="23">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="U1" s="145"/>
-      <c r="V1" s="177" t="s">
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="U1" s="126"/>
+      <c r="V1" s="147" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="146"/>
-      <c r="X1" s="146"/>
-      <c r="Y1" s="146"/>
-      <c r="Z1" s="146"/>
-      <c r="AA1" s="146"/>
-      <c r="AB1" s="146"/>
-      <c r="AC1" s="146"/>
-      <c r="AD1" s="146"/>
-      <c r="AE1" s="146"/>
-      <c r="AF1" s="146"/>
-      <c r="AG1" s="146"/>
-      <c r="AH1" s="146"/>
-      <c r="AI1" s="146"/>
-      <c r="AJ1" s="146"/>
-      <c r="AK1" s="146"/>
-      <c r="AL1" s="146"/>
-      <c r="AM1" s="146"/>
-      <c r="AN1" s="146"/>
-      <c r="AO1" s="145"/>
-      <c r="AP1" s="147"/>
-      <c r="AQ1" s="147"/>
-      <c r="AR1" s="147"/>
-      <c r="AS1" s="147"/>
-      <c r="AT1" s="147"/>
-      <c r="AU1" s="147"/>
-      <c r="AV1" s="147"/>
-      <c r="AW1" s="147"/>
-      <c r="AX1" s="147"/>
-      <c r="AY1" s="147"/>
-      <c r="AZ1" s="147"/>
-      <c r="BA1" s="147"/>
-      <c r="BB1" s="147"/>
-      <c r="BC1" s="147"/>
-      <c r="BD1" s="147"/>
-      <c r="BE1" s="147"/>
-      <c r="BF1" s="147"/>
-      <c r="BG1" s="147"/>
-      <c r="BH1" s="147"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="127"/>
+      <c r="Z1" s="127"/>
+      <c r="AA1" s="127"/>
+      <c r="AB1" s="127"/>
+      <c r="AC1" s="127"/>
+      <c r="AD1" s="127"/>
+      <c r="AE1" s="127"/>
+      <c r="AF1" s="127"/>
+      <c r="AG1" s="127"/>
+      <c r="AH1" s="127"/>
+      <c r="AI1" s="127"/>
+      <c r="AJ1" s="127"/>
+      <c r="AK1" s="127"/>
+      <c r="AL1" s="127"/>
+      <c r="AM1" s="127"/>
+      <c r="AN1" s="127"/>
+      <c r="AO1" s="126"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
+      <c r="AS1" s="164"/>
+      <c r="AT1" s="164"/>
+      <c r="AU1" s="164"/>
+      <c r="AV1" s="164"/>
+      <c r="AW1" s="164"/>
+      <c r="AX1" s="164"/>
+      <c r="AY1" s="164"/>
+      <c r="AZ1" s="164"/>
+      <c r="BA1" s="164"/>
+      <c r="BB1" s="164"/>
+      <c r="BC1" s="164"/>
+      <c r="BD1" s="164"/>
+      <c r="BE1" s="164"/>
+      <c r="BF1" s="164"/>
+      <c r="BG1" s="164"/>
+      <c r="BH1" s="164"/>
     </row>
     <row r="2" spans="1:60" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="167" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
-      <c r="O2" s="126"/>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="U2" s="148"/>
-      <c r="V2" s="149"/>
-      <c r="W2" s="149"/>
-      <c r="X2" s="149"/>
-      <c r="Y2" s="149"/>
-      <c r="Z2" s="149"/>
-      <c r="AA2" s="149"/>
-      <c r="AB2" s="149"/>
-      <c r="AC2" s="149"/>
-      <c r="AD2" s="149"/>
-      <c r="AE2" s="149"/>
-      <c r="AF2" s="149"/>
-      <c r="AG2" s="149"/>
-      <c r="AH2" s="149"/>
-      <c r="AI2" s="149"/>
-      <c r="AJ2" s="149"/>
-      <c r="AK2" s="149"/>
-      <c r="AL2" s="149"/>
-      <c r="AM2" s="149"/>
-      <c r="AN2" s="149"/>
-      <c r="AO2" s="149"/>
-      <c r="AP2" s="149"/>
-      <c r="AQ2" s="149"/>
-      <c r="AR2" s="149"/>
-      <c r="AS2" s="149"/>
-      <c r="AT2" s="149"/>
-      <c r="AU2" s="149"/>
-      <c r="AV2" s="149"/>
-      <c r="AW2" s="149"/>
-      <c r="AX2" s="149"/>
-      <c r="AY2" s="149"/>
-      <c r="AZ2" s="149"/>
-      <c r="BA2" s="149"/>
-      <c r="BB2" s="149"/>
-      <c r="BC2" s="149"/>
-      <c r="BD2" s="149"/>
-      <c r="BE2" s="149"/>
-      <c r="BF2" s="149"/>
-      <c r="BG2" s="149"/>
-      <c r="BH2" s="149"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
+      <c r="P2" s="167"/>
+      <c r="Q2" s="167"/>
+      <c r="R2" s="167"/>
+      <c r="S2" s="167"/>
+      <c r="U2" s="128"/>
+      <c r="V2" s="129"/>
+      <c r="W2" s="129"/>
+      <c r="X2" s="129"/>
+      <c r="Y2" s="129"/>
+      <c r="Z2" s="129"/>
+      <c r="AA2" s="129"/>
+      <c r="AB2" s="129"/>
+      <c r="AC2" s="129"/>
+      <c r="AD2" s="129"/>
+      <c r="AE2" s="129"/>
+      <c r="AF2" s="129"/>
+      <c r="AG2" s="129"/>
+      <c r="AH2" s="129"/>
+      <c r="AI2" s="129"/>
+      <c r="AJ2" s="129"/>
+      <c r="AK2" s="129"/>
+      <c r="AL2" s="129"/>
+      <c r="AM2" s="129"/>
+      <c r="AN2" s="129"/>
+      <c r="AO2" s="129"/>
+      <c r="AP2" s="129"/>
+      <c r="AQ2" s="129"/>
+      <c r="AR2" s="129"/>
+      <c r="AS2" s="129"/>
+      <c r="AT2" s="129"/>
+      <c r="AU2" s="129"/>
+      <c r="AV2" s="129"/>
+      <c r="AW2" s="129"/>
+      <c r="AX2" s="129"/>
+      <c r="AY2" s="129"/>
+      <c r="AZ2" s="129"/>
+      <c r="BA2" s="129"/>
+      <c r="BB2" s="129"/>
+      <c r="BC2" s="129"/>
+      <c r="BD2" s="129"/>
+      <c r="BE2" s="129"/>
+      <c r="BF2" s="129"/>
+      <c r="BG2" s="129"/>
+      <c r="BH2" s="129"/>
     </row>
     <row r="3" spans="1:60" ht="15" thickTop="1" thickBot="1">
       <c r="A3" s="16"/>
@@ -41678,326 +41616,326 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
-      <c r="U3" s="150"/>
-      <c r="V3" s="150"/>
-      <c r="W3" s="150" t="s">
+      <c r="U3" s="153"/>
+      <c r="V3" s="153"/>
+      <c r="W3" s="153" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="150"/>
-      <c r="Y3" s="151"/>
-      <c r="Z3" s="150" t="s">
+      <c r="X3" s="153"/>
+      <c r="Y3" s="130"/>
+      <c r="Z3" s="153" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="150"/>
-      <c r="AB3" s="152"/>
-      <c r="AC3" s="150" t="s">
+      <c r="AA3" s="153"/>
+      <c r="AB3" s="131"/>
+      <c r="AC3" s="153" t="s">
         <v>45</v>
       </c>
-      <c r="AD3" s="150"/>
-      <c r="AE3" s="151"/>
-      <c r="AF3" s="150" t="s">
+      <c r="AD3" s="153"/>
+      <c r="AE3" s="130"/>
+      <c r="AF3" s="153" t="s">
         <v>46</v>
       </c>
-      <c r="AG3" s="153"/>
-      <c r="AH3" s="153"/>
-      <c r="AI3" s="153"/>
-      <c r="AJ3" s="153"/>
-      <c r="AK3" s="154"/>
-      <c r="AL3" s="150" t="s">
+      <c r="AG3" s="169"/>
+      <c r="AH3" s="169"/>
+      <c r="AI3" s="169"/>
+      <c r="AJ3" s="169"/>
+      <c r="AK3" s="132"/>
+      <c r="AL3" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="AM3" s="155"/>
-      <c r="AN3" s="155"/>
-      <c r="AO3" s="155"/>
-      <c r="AP3" s="150"/>
-      <c r="AQ3" s="155"/>
-      <c r="AR3" s="155"/>
-      <c r="AS3" s="155"/>
-      <c r="AT3" s="148"/>
-      <c r="AU3" s="148"/>
-      <c r="AV3" s="148"/>
-      <c r="AW3" s="148"/>
-      <c r="AX3" s="148"/>
-      <c r="AY3" s="148"/>
-      <c r="AZ3" s="148"/>
-      <c r="BA3" s="148"/>
-      <c r="BB3" s="148"/>
-      <c r="BC3" s="148"/>
-      <c r="BD3" s="148"/>
-      <c r="BE3" s="148"/>
-      <c r="BF3" s="148"/>
-      <c r="BG3" s="148"/>
-      <c r="BH3" s="148"/>
+      <c r="AM3" s="165"/>
+      <c r="AN3" s="165"/>
+      <c r="AO3" s="165"/>
+      <c r="AP3" s="153"/>
+      <c r="AQ3" s="165"/>
+      <c r="AR3" s="165"/>
+      <c r="AS3" s="165"/>
+      <c r="AT3" s="128"/>
+      <c r="AU3" s="128"/>
+      <c r="AV3" s="128"/>
+      <c r="AW3" s="128"/>
+      <c r="AX3" s="128"/>
+      <c r="AY3" s="128"/>
+      <c r="AZ3" s="128"/>
+      <c r="BA3" s="128"/>
+      <c r="BB3" s="128"/>
+      <c r="BC3" s="128"/>
+      <c r="BD3" s="128"/>
+      <c r="BE3" s="128"/>
+      <c r="BF3" s="128"/>
+      <c r="BG3" s="128"/>
+      <c r="BH3" s="128"/>
     </row>
     <row r="4" spans="1:60" ht="13.5" customHeight="1" thickTop="1">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="127"/>
+      <c r="B4" s="161"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="127" t="s">
+      <c r="D4" s="161" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="127"/>
+      <c r="E4" s="161"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="127" t="s">
+      <c r="G4" s="161" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="127"/>
+      <c r="H4" s="161"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="127" t="s">
+      <c r="J4" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="130"/>
-      <c r="L4" s="130"/>
-      <c r="M4" s="130"/>
-      <c r="N4" s="130"/>
+      <c r="K4" s="168"/>
+      <c r="L4" s="168"/>
+      <c r="M4" s="168"/>
+      <c r="N4" s="168"/>
       <c r="O4" s="19"/>
-      <c r="P4" s="127" t="s">
+      <c r="P4" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="Q4" s="132"/>
-      <c r="R4" s="132"/>
-      <c r="S4" s="132"/>
-      <c r="U4" s="156"/>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
-      <c r="Z4" s="156"/>
-      <c r="AA4" s="156"/>
-      <c r="AB4" s="158"/>
-      <c r="AC4" s="156"/>
-      <c r="AD4" s="156"/>
-      <c r="AE4" s="157"/>
+      <c r="Q4" s="162"/>
+      <c r="R4" s="162"/>
+      <c r="S4" s="162"/>
+      <c r="U4" s="154"/>
+      <c r="V4" s="154"/>
+      <c r="W4" s="154"/>
+      <c r="X4" s="154"/>
+      <c r="Y4" s="133"/>
+      <c r="Z4" s="154"/>
+      <c r="AA4" s="154"/>
+      <c r="AB4" s="134"/>
+      <c r="AC4" s="154"/>
+      <c r="AD4" s="154"/>
+      <c r="AE4" s="133"/>
       <c r="AF4" s="159"/>
       <c r="AG4" s="159"/>
       <c r="AH4" s="159"/>
       <c r="AI4" s="159"/>
       <c r="AJ4" s="159"/>
-      <c r="AK4" s="160"/>
-      <c r="AL4" s="161"/>
-      <c r="AM4" s="161"/>
-      <c r="AN4" s="161"/>
-      <c r="AO4" s="161"/>
-      <c r="AP4" s="161"/>
-      <c r="AQ4" s="161"/>
-      <c r="AR4" s="161"/>
-      <c r="AS4" s="161"/>
-      <c r="AT4" s="148"/>
-      <c r="AU4" s="148"/>
-      <c r="AV4" s="148"/>
-      <c r="AW4" s="148"/>
-      <c r="AX4" s="148"/>
-      <c r="AY4" s="148"/>
-      <c r="AZ4" s="148"/>
-      <c r="BA4" s="148"/>
-      <c r="BB4" s="148"/>
-      <c r="BC4" s="148"/>
-      <c r="BD4" s="148"/>
-      <c r="BE4" s="148"/>
-      <c r="BF4" s="148"/>
-      <c r="BG4" s="148"/>
-      <c r="BH4" s="148"/>
+      <c r="AK4" s="135"/>
+      <c r="AL4" s="166"/>
+      <c r="AM4" s="166"/>
+      <c r="AN4" s="166"/>
+      <c r="AO4" s="166"/>
+      <c r="AP4" s="166"/>
+      <c r="AQ4" s="166"/>
+      <c r="AR4" s="166"/>
+      <c r="AS4" s="166"/>
+      <c r="AT4" s="128"/>
+      <c r="AU4" s="128"/>
+      <c r="AV4" s="128"/>
+      <c r="AW4" s="128"/>
+      <c r="AX4" s="128"/>
+      <c r="AY4" s="128"/>
+      <c r="AZ4" s="128"/>
+      <c r="BA4" s="128"/>
+      <c r="BB4" s="128"/>
+      <c r="BC4" s="128"/>
+      <c r="BD4" s="128"/>
+      <c r="BE4" s="128"/>
+      <c r="BF4" s="128"/>
+      <c r="BG4" s="128"/>
+      <c r="BH4" s="128"/>
     </row>
     <row r="5" spans="1:60" ht="13.5" customHeight="1">
-      <c r="A5" s="128"/>
-      <c r="B5" s="128"/>
+      <c r="A5" s="151"/>
+      <c r="B5" s="151"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
+      <c r="D5" s="151"/>
+      <c r="E5" s="151"/>
       <c r="F5" s="21"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
+      <c r="G5" s="151"/>
+      <c r="H5" s="151"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
-      <c r="N5" s="131"/>
+      <c r="J5" s="150"/>
+      <c r="K5" s="150"/>
+      <c r="L5" s="150"/>
+      <c r="M5" s="150"/>
+      <c r="N5" s="150"/>
       <c r="O5" s="22"/>
-      <c r="P5" s="133"/>
-      <c r="Q5" s="133"/>
-      <c r="R5" s="133"/>
-      <c r="S5" s="133"/>
-      <c r="U5" s="156"/>
-      <c r="V5" s="156"/>
-      <c r="W5" s="156"/>
-      <c r="X5" s="156"/>
-      <c r="Y5" s="157"/>
-      <c r="Z5" s="156"/>
-      <c r="AA5" s="156"/>
-      <c r="AB5" s="158"/>
-      <c r="AC5" s="156"/>
-      <c r="AD5" s="156"/>
-      <c r="AE5" s="157"/>
-      <c r="AF5" s="162" t="s">
+      <c r="P5" s="163"/>
+      <c r="Q5" s="163"/>
+      <c r="R5" s="163"/>
+      <c r="S5" s="163"/>
+      <c r="U5" s="154"/>
+      <c r="V5" s="154"/>
+      <c r="W5" s="154"/>
+      <c r="X5" s="154"/>
+      <c r="Y5" s="133"/>
+      <c r="Z5" s="154"/>
+      <c r="AA5" s="154"/>
+      <c r="AB5" s="134"/>
+      <c r="AC5" s="154"/>
+      <c r="AD5" s="154"/>
+      <c r="AE5" s="133"/>
+      <c r="AF5" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="AG5" s="163"/>
-      <c r="AH5" s="164"/>
-      <c r="AI5" s="162" t="s">
+      <c r="AG5" s="158"/>
+      <c r="AH5" s="136"/>
+      <c r="AI5" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="AJ5" s="163"/>
-      <c r="AK5" s="164"/>
-      <c r="AL5" s="156" t="s">
+      <c r="AJ5" s="158"/>
+      <c r="AK5" s="136"/>
+      <c r="AL5" s="154" t="s">
         <v>50</v>
       </c>
-      <c r="AM5" s="156"/>
-      <c r="AN5" s="164"/>
-      <c r="AO5" s="156" t="s">
+      <c r="AM5" s="154"/>
+      <c r="AN5" s="136"/>
+      <c r="AO5" s="154" t="s">
         <v>51</v>
       </c>
-      <c r="AP5" s="156"/>
-      <c r="AQ5" s="156"/>
-      <c r="AR5" s="164"/>
-      <c r="AS5" s="156"/>
-      <c r="AT5" s="148"/>
-      <c r="AU5" s="148"/>
-      <c r="AV5" s="148"/>
-      <c r="AW5" s="148"/>
-      <c r="AX5" s="148"/>
-      <c r="AY5" s="148"/>
-      <c r="AZ5" s="148"/>
-      <c r="BA5" s="148"/>
-      <c r="BB5" s="148"/>
-      <c r="BC5" s="148"/>
-      <c r="BD5" s="148"/>
-      <c r="BE5" s="148"/>
-      <c r="BF5" s="148"/>
-      <c r="BG5" s="148"/>
-      <c r="BH5" s="148"/>
+      <c r="AP5" s="154"/>
+      <c r="AQ5" s="154"/>
+      <c r="AR5" s="136"/>
+      <c r="AS5" s="154"/>
+      <c r="AT5" s="128"/>
+      <c r="AU5" s="128"/>
+      <c r="AV5" s="128"/>
+      <c r="AW5" s="128"/>
+      <c r="AX5" s="128"/>
+      <c r="AY5" s="128"/>
+      <c r="AZ5" s="128"/>
+      <c r="BA5" s="128"/>
+      <c r="BB5" s="128"/>
+      <c r="BC5" s="128"/>
+      <c r="BD5" s="128"/>
+      <c r="BE5" s="128"/>
+      <c r="BF5" s="128"/>
+      <c r="BG5" s="128"/>
+      <c r="BH5" s="128"/>
     </row>
     <row r="6" spans="1:60" ht="12.75" customHeight="1">
-      <c r="A6" s="128"/>
-      <c r="B6" s="128"/>
+      <c r="A6" s="151"/>
+      <c r="B6" s="151"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
       <c r="I6" s="20"/>
-      <c r="J6" s="134" t="s">
+      <c r="J6" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="135"/>
+      <c r="K6" s="149"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="134" t="s">
+      <c r="M6" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="N6" s="135"/>
+      <c r="N6" s="149"/>
       <c r="O6" s="23"/>
-      <c r="P6" s="128" t="s">
+      <c r="P6" s="151" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="128"/>
+      <c r="Q6" s="151"/>
       <c r="R6" s="23"/>
-      <c r="S6" s="128" t="s">
+      <c r="S6" s="151" t="s">
         <v>51</v>
       </c>
-      <c r="U6" s="165"/>
-      <c r="V6" s="165"/>
-      <c r="W6" s="165"/>
-      <c r="X6" s="165"/>
-      <c r="Y6" s="157"/>
-      <c r="Z6" s="165"/>
-      <c r="AA6" s="165"/>
-      <c r="AB6" s="158"/>
-      <c r="AC6" s="165"/>
-      <c r="AD6" s="165"/>
-      <c r="AE6" s="157"/>
+      <c r="U6" s="155"/>
+      <c r="V6" s="155"/>
+      <c r="W6" s="155"/>
+      <c r="X6" s="155"/>
+      <c r="Y6" s="133"/>
+      <c r="Z6" s="155"/>
+      <c r="AA6" s="155"/>
+      <c r="AB6" s="134"/>
+      <c r="AC6" s="155"/>
+      <c r="AD6" s="155"/>
+      <c r="AE6" s="133"/>
       <c r="AF6" s="159"/>
       <c r="AG6" s="159"/>
-      <c r="AH6" s="166"/>
+      <c r="AH6" s="137"/>
       <c r="AI6" s="159"/>
       <c r="AJ6" s="159"/>
-      <c r="AK6" s="164"/>
-      <c r="AL6" s="165"/>
-      <c r="AM6" s="165"/>
-      <c r="AN6" s="166"/>
-      <c r="AO6" s="167"/>
-      <c r="AP6" s="165"/>
-      <c r="AQ6" s="165"/>
-      <c r="AR6" s="166"/>
-      <c r="AS6" s="167"/>
-      <c r="AT6" s="148"/>
-      <c r="AU6" s="148"/>
-      <c r="AV6" s="148"/>
-      <c r="AW6" s="148"/>
-      <c r="AX6" s="148"/>
-      <c r="AY6" s="148"/>
-      <c r="AZ6" s="148"/>
-      <c r="BA6" s="148"/>
-      <c r="BB6" s="148"/>
-      <c r="BC6" s="148"/>
-      <c r="BD6" s="148"/>
-      <c r="BE6" s="148"/>
-      <c r="BF6" s="148"/>
-      <c r="BG6" s="148"/>
-      <c r="BH6" s="148"/>
+      <c r="AK6" s="136"/>
+      <c r="AL6" s="155"/>
+      <c r="AM6" s="155"/>
+      <c r="AN6" s="137"/>
+      <c r="AO6" s="160"/>
+      <c r="AP6" s="155"/>
+      <c r="AQ6" s="155"/>
+      <c r="AR6" s="137"/>
+      <c r="AS6" s="160"/>
+      <c r="AT6" s="128"/>
+      <c r="AU6" s="128"/>
+      <c r="AV6" s="128"/>
+      <c r="AW6" s="128"/>
+      <c r="AX6" s="128"/>
+      <c r="AY6" s="128"/>
+      <c r="AZ6" s="128"/>
+      <c r="BA6" s="128"/>
+      <c r="BB6" s="128"/>
+      <c r="BC6" s="128"/>
+      <c r="BD6" s="128"/>
+      <c r="BE6" s="128"/>
+      <c r="BF6" s="128"/>
+      <c r="BG6" s="128"/>
+      <c r="BH6" s="128"/>
     </row>
     <row r="7" spans="1:60" ht="12.75" customHeight="1">
-      <c r="A7" s="129"/>
-      <c r="B7" s="129"/>
+      <c r="A7" s="152"/>
+      <c r="B7" s="152"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="152"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
+      <c r="G7" s="152"/>
+      <c r="H7" s="152"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="131"/>
-      <c r="K7" s="131"/>
+      <c r="J7" s="150"/>
+      <c r="K7" s="150"/>
       <c r="L7" s="24"/>
-      <c r="M7" s="131"/>
-      <c r="N7" s="131"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="150"/>
       <c r="O7" s="23"/>
-      <c r="P7" s="129"/>
-      <c r="Q7" s="129"/>
+      <c r="P7" s="152"/>
+      <c r="Q7" s="152"/>
       <c r="R7" s="24"/>
-      <c r="S7" s="136"/>
-      <c r="U7" s="148"/>
-      <c r="V7" s="148"/>
-      <c r="W7" s="148"/>
-      <c r="X7" s="148"/>
-      <c r="Y7" s="148"/>
-      <c r="Z7" s="148"/>
-      <c r="AA7" s="148"/>
-      <c r="AB7" s="148"/>
-      <c r="AC7" s="148"/>
-      <c r="AD7" s="148"/>
-      <c r="AE7" s="148"/>
-      <c r="AF7" s="148"/>
-      <c r="AG7" s="148"/>
-      <c r="AH7" s="148"/>
-      <c r="AI7" s="148"/>
-      <c r="AJ7" s="148"/>
-      <c r="AK7" s="148"/>
-      <c r="AL7" s="148"/>
-      <c r="AM7" s="148"/>
-      <c r="AN7" s="148"/>
-      <c r="AO7" s="148"/>
-      <c r="AP7" s="148"/>
-      <c r="AQ7" s="148"/>
-      <c r="AR7" s="148"/>
-      <c r="AS7" s="148"/>
-      <c r="AT7" s="148"/>
-      <c r="AU7" s="148"/>
-      <c r="AV7" s="148"/>
-      <c r="AW7" s="148"/>
-      <c r="AX7" s="148"/>
-      <c r="AY7" s="148"/>
-      <c r="AZ7" s="148"/>
-      <c r="BA7" s="148"/>
-      <c r="BB7" s="148"/>
-      <c r="BC7" s="148"/>
-      <c r="BD7" s="148"/>
-      <c r="BE7" s="148"/>
-      <c r="BF7" s="148"/>
-      <c r="BG7" s="148"/>
-      <c r="BH7" s="148"/>
+      <c r="S7" s="156"/>
+      <c r="U7" s="128"/>
+      <c r="V7" s="128"/>
+      <c r="W7" s="128"/>
+      <c r="X7" s="128"/>
+      <c r="Y7" s="128"/>
+      <c r="Z7" s="128"/>
+      <c r="AA7" s="128"/>
+      <c r="AB7" s="128"/>
+      <c r="AC7" s="128"/>
+      <c r="AD7" s="128"/>
+      <c r="AE7" s="128"/>
+      <c r="AF7" s="128"/>
+      <c r="AG7" s="128"/>
+      <c r="AH7" s="128"/>
+      <c r="AI7" s="128"/>
+      <c r="AJ7" s="128"/>
+      <c r="AK7" s="128"/>
+      <c r="AL7" s="128"/>
+      <c r="AM7" s="128"/>
+      <c r="AN7" s="128"/>
+      <c r="AO7" s="128"/>
+      <c r="AP7" s="128"/>
+      <c r="AQ7" s="128"/>
+      <c r="AR7" s="128"/>
+      <c r="AS7" s="128"/>
+      <c r="AT7" s="128"/>
+      <c r="AU7" s="128"/>
+      <c r="AV7" s="128"/>
+      <c r="AW7" s="128"/>
+      <c r="AX7" s="128"/>
+      <c r="AY7" s="128"/>
+      <c r="AZ7" s="128"/>
+      <c r="BA7" s="128"/>
+      <c r="BB7" s="128"/>
+      <c r="BC7" s="128"/>
+      <c r="BD7" s="128"/>
+      <c r="BE7" s="128"/>
+      <c r="BF7" s="128"/>
+      <c r="BG7" s="128"/>
+      <c r="BH7" s="128"/>
     </row>
     <row r="8" spans="1:60" ht="13">
       <c r="A8" s="25"/>
@@ -42019,78 +41957,78 @@
       <c r="Q8" s="25"/>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
-      <c r="U8" s="148"/>
-      <c r="V8" s="148"/>
-      <c r="W8" s="168" t="s">
+      <c r="U8" s="128"/>
+      <c r="V8" s="128"/>
+      <c r="W8" s="138" t="s">
         <v>190</v>
       </c>
-      <c r="X8" s="168"/>
-      <c r="Y8" s="148"/>
-      <c r="Z8" s="169">
+      <c r="X8" s="138"/>
+      <c r="Y8" s="128"/>
+      <c r="Z8" s="139">
         <v>0.41</v>
       </c>
-      <c r="AA8" s="170">
+      <c r="AA8" s="140">
         <f>Z8</f>
         <v>0.41</v>
       </c>
-      <c r="AB8" s="171"/>
-      <c r="AC8" s="169">
+      <c r="AB8" s="141"/>
+      <c r="AC8" s="139">
         <v>0.43</v>
       </c>
-      <c r="AD8" s="170">
+      <c r="AD8" s="140">
         <f>AC8</f>
         <v>0.43</v>
       </c>
-      <c r="AE8" s="172"/>
-      <c r="AF8" s="172">
+      <c r="AE8" s="142"/>
+      <c r="AF8" s="142">
         <v>-37</v>
       </c>
-      <c r="AG8" s="170">
+      <c r="AG8" s="140">
         <f>AF8</f>
         <v>-37</v>
       </c>
-      <c r="AH8" s="148"/>
-      <c r="AI8" s="169">
+      <c r="AH8" s="128"/>
+      <c r="AI8" s="139">
         <v>-9.75</v>
       </c>
-      <c r="AJ8" s="170">
+      <c r="AJ8" s="140">
         <f>AI8</f>
         <v>-9.75</v>
       </c>
-      <c r="AK8" s="172"/>
-      <c r="AL8" s="169">
+      <c r="AK8" s="142"/>
+      <c r="AL8" s="139">
         <v>0</v>
       </c>
-      <c r="AM8" s="170">
+      <c r="AM8" s="140">
         <f>AL8</f>
         <v>0</v>
       </c>
-      <c r="AN8" s="171"/>
-      <c r="AO8" s="169">
+      <c r="AN8" s="141"/>
+      <c r="AO8" s="139">
         <v>0.41</v>
       </c>
-      <c r="AP8" s="170">
+      <c r="AP8" s="140">
         <f>AO8</f>
         <v>0.41</v>
       </c>
-      <c r="AQ8" s="148"/>
-      <c r="AR8" s="148"/>
-      <c r="AS8" s="148"/>
-      <c r="AT8" s="148"/>
-      <c r="AU8" s="148"/>
-      <c r="AV8" s="148"/>
-      <c r="AW8" s="148"/>
-      <c r="AX8" s="148"/>
-      <c r="AY8" s="148"/>
-      <c r="AZ8" s="148"/>
-      <c r="BA8" s="148"/>
-      <c r="BB8" s="148"/>
-      <c r="BC8" s="148"/>
-      <c r="BD8" s="148"/>
-      <c r="BE8" s="148"/>
-      <c r="BF8" s="148"/>
-      <c r="BG8" s="148"/>
-      <c r="BH8" s="148"/>
+      <c r="AQ8" s="128"/>
+      <c r="AR8" s="128"/>
+      <c r="AS8" s="128"/>
+      <c r="AT8" s="128"/>
+      <c r="AU8" s="128"/>
+      <c r="AV8" s="128"/>
+      <c r="AW8" s="128"/>
+      <c r="AX8" s="128"/>
+      <c r="AY8" s="128"/>
+      <c r="AZ8" s="128"/>
+      <c r="BA8" s="128"/>
+      <c r="BB8" s="128"/>
+      <c r="BC8" s="128"/>
+      <c r="BD8" s="128"/>
+      <c r="BE8" s="128"/>
+      <c r="BF8" s="128"/>
+      <c r="BG8" s="128"/>
+      <c r="BH8" s="128"/>
     </row>
     <row r="9" spans="1:60" ht="13">
       <c r="A9" s="26" t="s">
@@ -42127,78 +42065,78 @@
         <v>0.41</v>
       </c>
       <c r="T9" s="27"/>
-      <c r="U9" s="148"/>
-      <c r="V9" s="148"/>
-      <c r="W9" s="173" t="s">
+      <c r="U9" s="128"/>
+      <c r="V9" s="128"/>
+      <c r="W9" s="143" t="s">
         <v>191</v>
       </c>
-      <c r="X9" s="173"/>
-      <c r="Y9" s="148"/>
-      <c r="Z9" s="169">
+      <c r="X9" s="143"/>
+      <c r="Y9" s="128"/>
+      <c r="Z9" s="139">
         <v>2.06</v>
       </c>
-      <c r="AA9" s="170">
+      <c r="AA9" s="140">
         <f t="shared" ref="AA9:AA20" si="0">Z9</f>
         <v>2.06</v>
       </c>
-      <c r="AB9" s="171"/>
-      <c r="AC9" s="169">
+      <c r="AB9" s="141"/>
+      <c r="AC9" s="139">
         <v>5.18</v>
       </c>
-      <c r="AD9" s="170">
+      <c r="AD9" s="140">
         <f t="shared" ref="AD9:AD20" si="1">AC9</f>
         <v>5.18</v>
       </c>
-      <c r="AE9" s="172"/>
-      <c r="AF9" s="172">
+      <c r="AE9" s="142"/>
+      <c r="AF9" s="142">
         <v>-437</v>
       </c>
-      <c r="AG9" s="170">
+      <c r="AG9" s="140">
         <f t="shared" ref="AG9:AG20" si="2">AF9</f>
         <v>-437</v>
       </c>
-      <c r="AH9" s="148"/>
-      <c r="AI9" s="169">
+      <c r="AH9" s="128"/>
+      <c r="AI9" s="139">
         <v>-19.07</v>
       </c>
-      <c r="AJ9" s="170">
+      <c r="AJ9" s="140">
         <f t="shared" ref="AJ9:AJ20" si="3">AI9</f>
         <v>-19.07</v>
       </c>
-      <c r="AK9" s="172"/>
-      <c r="AL9" s="169">
+      <c r="AK9" s="142"/>
+      <c r="AL9" s="139">
         <v>-0.27</v>
       </c>
-      <c r="AM9" s="170">
+      <c r="AM9" s="140">
         <f t="shared" ref="AM9:AM20" si="4">AL9</f>
         <v>-0.27</v>
       </c>
-      <c r="AN9" s="171"/>
-      <c r="AO9" s="169">
+      <c r="AN9" s="141"/>
+      <c r="AO9" s="139">
         <v>2.29</v>
       </c>
-      <c r="AP9" s="170">
+      <c r="AP9" s="140">
         <f t="shared" ref="AP9:AP20" si="5">AO9</f>
         <v>2.29</v>
       </c>
-      <c r="AQ9" s="148"/>
-      <c r="AR9" s="148"/>
-      <c r="AS9" s="148"/>
-      <c r="AT9" s="148"/>
-      <c r="AU9" s="148"/>
-      <c r="AV9" s="148"/>
-      <c r="AW9" s="148"/>
-      <c r="AX9" s="148"/>
-      <c r="AY9" s="148"/>
-      <c r="AZ9" s="148"/>
-      <c r="BA9" s="148"/>
-      <c r="BB9" s="148"/>
-      <c r="BC9" s="148"/>
-      <c r="BD9" s="148"/>
-      <c r="BE9" s="148"/>
-      <c r="BF9" s="148"/>
-      <c r="BG9" s="148"/>
-      <c r="BH9" s="148"/>
+      <c r="AQ9" s="128"/>
+      <c r="AR9" s="128"/>
+      <c r="AS9" s="128"/>
+      <c r="AT9" s="128"/>
+      <c r="AU9" s="128"/>
+      <c r="AV9" s="128"/>
+      <c r="AW9" s="128"/>
+      <c r="AX9" s="128"/>
+      <c r="AY9" s="128"/>
+      <c r="AZ9" s="128"/>
+      <c r="BA9" s="128"/>
+      <c r="BB9" s="128"/>
+      <c r="BC9" s="128"/>
+      <c r="BD9" s="128"/>
+      <c r="BE9" s="128"/>
+      <c r="BF9" s="128"/>
+      <c r="BG9" s="128"/>
+      <c r="BH9" s="128"/>
     </row>
     <row r="10" spans="1:60" ht="13">
       <c r="A10" s="30" t="s">
@@ -42235,78 +42173,78 @@
         <v>2.29</v>
       </c>
       <c r="T10" s="27"/>
-      <c r="U10" s="148"/>
-      <c r="V10" s="148"/>
-      <c r="W10" s="168" t="s">
+      <c r="U10" s="128"/>
+      <c r="V10" s="128"/>
+      <c r="W10" s="138" t="s">
         <v>192</v>
       </c>
-      <c r="X10" s="168"/>
-      <c r="Y10" s="148"/>
-      <c r="Z10" s="169">
+      <c r="X10" s="138"/>
+      <c r="Y10" s="128"/>
+      <c r="Z10" s="139">
         <v>2.34</v>
       </c>
-      <c r="AA10" s="170">
+      <c r="AA10" s="140">
         <f t="shared" si="0"/>
         <v>2.34</v>
       </c>
-      <c r="AB10" s="171"/>
-      <c r="AC10" s="169">
+      <c r="AB10" s="141"/>
+      <c r="AC10" s="139">
         <v>9.66</v>
       </c>
-      <c r="AD10" s="170">
+      <c r="AD10" s="140">
         <f t="shared" si="1"/>
         <v>9.66</v>
       </c>
-      <c r="AE10" s="172"/>
-      <c r="AF10" s="172">
+      <c r="AE10" s="142"/>
+      <c r="AF10" s="142">
         <v>-814</v>
       </c>
-      <c r="AG10" s="170">
+      <c r="AG10" s="140">
         <f t="shared" si="2"/>
         <v>-814</v>
       </c>
-      <c r="AH10" s="148"/>
-      <c r="AI10" s="169">
+      <c r="AH10" s="128"/>
+      <c r="AI10" s="139">
         <v>-11.58</v>
       </c>
-      <c r="AJ10" s="170">
+      <c r="AJ10" s="140">
         <f t="shared" si="3"/>
         <v>-11.58</v>
       </c>
-      <c r="AK10" s="172"/>
-      <c r="AL10" s="169">
+      <c r="AK10" s="142"/>
+      <c r="AL10" s="139">
         <v>-0.19</v>
       </c>
-      <c r="AM10" s="170">
+      <c r="AM10" s="140">
         <f t="shared" si="4"/>
         <v>-0.19</v>
       </c>
-      <c r="AN10" s="171"/>
-      <c r="AO10" s="169">
+      <c r="AN10" s="141"/>
+      <c r="AO10" s="139">
         <v>7.68</v>
       </c>
-      <c r="AP10" s="170">
+      <c r="AP10" s="140">
         <f t="shared" si="5"/>
         <v>7.68</v>
       </c>
-      <c r="AQ10" s="148"/>
-      <c r="AR10" s="148"/>
-      <c r="AS10" s="148"/>
-      <c r="AT10" s="148"/>
-      <c r="AU10" s="148"/>
-      <c r="AV10" s="148"/>
-      <c r="AW10" s="148"/>
-      <c r="AX10" s="148"/>
-      <c r="AY10" s="148"/>
-      <c r="AZ10" s="148"/>
-      <c r="BA10" s="148"/>
-      <c r="BB10" s="148"/>
-      <c r="BC10" s="148"/>
-      <c r="BD10" s="148"/>
-      <c r="BE10" s="148"/>
-      <c r="BF10" s="148"/>
-      <c r="BG10" s="148"/>
-      <c r="BH10" s="148"/>
+      <c r="AQ10" s="128"/>
+      <c r="AR10" s="128"/>
+      <c r="AS10" s="128"/>
+      <c r="AT10" s="128"/>
+      <c r="AU10" s="128"/>
+      <c r="AV10" s="128"/>
+      <c r="AW10" s="128"/>
+      <c r="AX10" s="128"/>
+      <c r="AY10" s="128"/>
+      <c r="AZ10" s="128"/>
+      <c r="BA10" s="128"/>
+      <c r="BB10" s="128"/>
+      <c r="BC10" s="128"/>
+      <c r="BD10" s="128"/>
+      <c r="BE10" s="128"/>
+      <c r="BF10" s="128"/>
+      <c r="BG10" s="128"/>
+      <c r="BH10" s="128"/>
     </row>
     <row r="11" spans="1:60" ht="13">
       <c r="A11" s="26" t="s">
@@ -42343,78 +42281,78 @@
         <v>7.68</v>
       </c>
       <c r="T11" s="27"/>
-      <c r="U11" s="148"/>
-      <c r="V11" s="148"/>
-      <c r="W11" s="168" t="s">
+      <c r="U11" s="128"/>
+      <c r="V11" s="128"/>
+      <c r="W11" s="138" t="s">
         <v>193</v>
       </c>
-      <c r="X11" s="168"/>
-      <c r="Y11" s="148"/>
-      <c r="Z11" s="169">
+      <c r="X11" s="138"/>
+      <c r="Y11" s="128"/>
+      <c r="Z11" s="139">
         <v>2.27</v>
       </c>
-      <c r="AA11" s="170">
+      <c r="AA11" s="140">
         <f t="shared" si="0"/>
         <v>2.27</v>
       </c>
-      <c r="AB11" s="171"/>
-      <c r="AC11" s="169">
+      <c r="AB11" s="141"/>
+      <c r="AC11" s="139">
         <v>15.48</v>
       </c>
-      <c r="AD11" s="170">
+      <c r="AD11" s="140">
         <f t="shared" si="1"/>
         <v>15.48</v>
       </c>
-      <c r="AE11" s="172"/>
-      <c r="AF11" s="172">
+      <c r="AE11" s="142"/>
+      <c r="AF11" s="142">
         <v>-1305</v>
       </c>
-      <c r="AG11" s="170">
+      <c r="AG11" s="140">
         <f t="shared" si="2"/>
         <v>-1305</v>
       </c>
-      <c r="AH11" s="148"/>
-      <c r="AI11" s="169">
+      <c r="AH11" s="128"/>
+      <c r="AI11" s="139">
         <v>-8.41</v>
       </c>
-      <c r="AJ11" s="170">
+      <c r="AJ11" s="140">
         <f t="shared" si="3"/>
         <v>-8.41</v>
       </c>
-      <c r="AK11" s="172"/>
-      <c r="AL11" s="169">
+      <c r="AK11" s="142"/>
+      <c r="AL11" s="139">
         <v>0.2</v>
       </c>
-      <c r="AM11" s="170">
+      <c r="AM11" s="140">
         <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
-      <c r="AN11" s="171"/>
-      <c r="AO11" s="169">
+      <c r="AN11" s="141"/>
+      <c r="AO11" s="139">
         <v>17.559999999999999</v>
       </c>
-      <c r="AP11" s="170">
+      <c r="AP11" s="140">
         <f t="shared" si="5"/>
         <v>17.559999999999999</v>
       </c>
-      <c r="AQ11" s="148"/>
-      <c r="AR11" s="148"/>
-      <c r="AS11" s="148"/>
-      <c r="AT11" s="148"/>
-      <c r="AU11" s="148"/>
-      <c r="AV11" s="148"/>
-      <c r="AW11" s="148"/>
-      <c r="AX11" s="148"/>
-      <c r="AY11" s="148"/>
-      <c r="AZ11" s="148"/>
-      <c r="BA11" s="148"/>
-      <c r="BB11" s="148"/>
-      <c r="BC11" s="148"/>
-      <c r="BD11" s="148"/>
-      <c r="BE11" s="148"/>
-      <c r="BF11" s="148"/>
-      <c r="BG11" s="148"/>
-      <c r="BH11" s="148"/>
+      <c r="AQ11" s="128"/>
+      <c r="AR11" s="128"/>
+      <c r="AS11" s="128"/>
+      <c r="AT11" s="128"/>
+      <c r="AU11" s="128"/>
+      <c r="AV11" s="128"/>
+      <c r="AW11" s="128"/>
+      <c r="AX11" s="128"/>
+      <c r="AY11" s="128"/>
+      <c r="AZ11" s="128"/>
+      <c r="BA11" s="128"/>
+      <c r="BB11" s="128"/>
+      <c r="BC11" s="128"/>
+      <c r="BD11" s="128"/>
+      <c r="BE11" s="128"/>
+      <c r="BF11" s="128"/>
+      <c r="BG11" s="128"/>
+      <c r="BH11" s="128"/>
     </row>
     <row r="12" spans="1:60" ht="13">
       <c r="A12" s="26" t="s">
@@ -42451,78 +42389,78 @@
         <v>17.559999999999999</v>
       </c>
       <c r="T12" s="27"/>
-      <c r="U12" s="148"/>
-      <c r="V12" s="148"/>
-      <c r="W12" s="168" t="s">
+      <c r="U12" s="128"/>
+      <c r="V12" s="128"/>
+      <c r="W12" s="138" t="s">
         <v>194</v>
       </c>
-      <c r="X12" s="168"/>
-      <c r="Y12" s="148"/>
-      <c r="Z12" s="169">
+      <c r="X12" s="138"/>
+      <c r="Y12" s="128"/>
+      <c r="Z12" s="139">
         <v>3.6</v>
       </c>
-      <c r="AA12" s="170">
+      <c r="AA12" s="140">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="AB12" s="171"/>
-      <c r="AC12" s="169">
+      <c r="AB12" s="141"/>
+      <c r="AC12" s="139">
         <v>68.91</v>
       </c>
-      <c r="AD12" s="170">
+      <c r="AD12" s="140">
         <f t="shared" si="1"/>
         <v>68.91</v>
       </c>
-      <c r="AE12" s="172"/>
-      <c r="AF12" s="172">
+      <c r="AE12" s="142"/>
+      <c r="AF12" s="142">
         <v>-5809</v>
       </c>
-      <c r="AG12" s="170">
+      <c r="AG12" s="140">
         <f t="shared" si="2"/>
         <v>-5809</v>
       </c>
-      <c r="AH12" s="148"/>
-      <c r="AI12" s="169">
+      <c r="AH12" s="128"/>
+      <c r="AI12" s="139">
         <v>-9.07</v>
       </c>
-      <c r="AJ12" s="170">
+      <c r="AJ12" s="140">
         <f t="shared" si="3"/>
         <v>-9.07</v>
       </c>
-      <c r="AK12" s="172"/>
-      <c r="AL12" s="169">
+      <c r="AK12" s="142"/>
+      <c r="AL12" s="139">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AM12" s="170">
+      <c r="AM12" s="140">
         <f t="shared" si="4"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="AN12" s="171"/>
-      <c r="AO12" s="169">
+      <c r="AN12" s="141"/>
+      <c r="AO12" s="139">
         <v>71.91</v>
       </c>
-      <c r="AP12" s="170">
+      <c r="AP12" s="140">
         <f t="shared" si="5"/>
         <v>71.91</v>
       </c>
-      <c r="AQ12" s="148"/>
-      <c r="AR12" s="148"/>
-      <c r="AS12" s="148"/>
-      <c r="AT12" s="148"/>
-      <c r="AU12" s="148"/>
-      <c r="AV12" s="148"/>
-      <c r="AW12" s="148"/>
-      <c r="AX12" s="148"/>
-      <c r="AY12" s="148"/>
-      <c r="AZ12" s="148"/>
-      <c r="BA12" s="148"/>
-      <c r="BB12" s="148"/>
-      <c r="BC12" s="148"/>
-      <c r="BD12" s="148"/>
-      <c r="BE12" s="148"/>
-      <c r="BF12" s="148"/>
-      <c r="BG12" s="148"/>
-      <c r="BH12" s="148"/>
+      <c r="AQ12" s="128"/>
+      <c r="AR12" s="128"/>
+      <c r="AS12" s="128"/>
+      <c r="AT12" s="128"/>
+      <c r="AU12" s="128"/>
+      <c r="AV12" s="128"/>
+      <c r="AW12" s="128"/>
+      <c r="AX12" s="128"/>
+      <c r="AY12" s="128"/>
+      <c r="AZ12" s="128"/>
+      <c r="BA12" s="128"/>
+      <c r="BB12" s="128"/>
+      <c r="BC12" s="128"/>
+      <c r="BD12" s="128"/>
+      <c r="BE12" s="128"/>
+      <c r="BF12" s="128"/>
+      <c r="BG12" s="128"/>
+      <c r="BH12" s="128"/>
     </row>
     <row r="13" spans="1:60" ht="13">
       <c r="A13" s="26" t="s">
@@ -42559,78 +42497,78 @@
         <v>71.91</v>
       </c>
       <c r="T13" s="27"/>
-      <c r="U13" s="148"/>
-      <c r="V13" s="148"/>
-      <c r="W13" s="168" t="s">
+      <c r="U13" s="128"/>
+      <c r="V13" s="128"/>
+      <c r="W13" s="138" t="s">
         <v>57</v>
       </c>
-      <c r="X13" s="168"/>
-      <c r="Y13" s="148"/>
-      <c r="Z13" s="169">
+      <c r="X13" s="138"/>
+      <c r="Y13" s="128"/>
+      <c r="Z13" s="139">
         <v>2.99</v>
       </c>
-      <c r="AA13" s="170">
+      <c r="AA13" s="140">
         <f t="shared" si="0"/>
         <v>2.99</v>
       </c>
-      <c r="AB13" s="171"/>
-      <c r="AC13" s="169">
+      <c r="AB13" s="141"/>
+      <c r="AC13" s="139">
         <v>100</v>
       </c>
-      <c r="AD13" s="170">
+      <c r="AD13" s="140">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="AE13" s="172"/>
-      <c r="AF13" s="172">
+      <c r="AE13" s="142"/>
+      <c r="AF13" s="142">
         <v>-1686</v>
       </c>
-      <c r="AG13" s="170">
+      <c r="AG13" s="140">
         <f t="shared" si="2"/>
         <v>-1686</v>
       </c>
-      <c r="AH13" s="148"/>
-      <c r="AI13" s="169">
+      <c r="AH13" s="128"/>
+      <c r="AI13" s="139">
         <v>-9.43</v>
       </c>
-      <c r="AJ13" s="170">
+      <c r="AJ13" s="140">
         <f t="shared" si="3"/>
         <v>-9.43</v>
       </c>
-      <c r="AK13" s="172"/>
-      <c r="AL13" s="169">
+      <c r="AK13" s="142"/>
+      <c r="AL13" s="139">
         <v>0</v>
       </c>
-      <c r="AM13" s="170">
+      <c r="AM13" s="140">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AN13" s="171"/>
-      <c r="AO13" s="169">
+      <c r="AN13" s="141"/>
+      <c r="AO13" s="139">
         <v>100</v>
       </c>
-      <c r="AP13" s="170">
+      <c r="AP13" s="140">
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="AQ13" s="148"/>
-      <c r="AR13" s="148"/>
-      <c r="AS13" s="148"/>
-      <c r="AT13" s="148"/>
-      <c r="AU13" s="148"/>
-      <c r="AV13" s="148"/>
-      <c r="AW13" s="148"/>
-      <c r="AX13" s="148"/>
-      <c r="AY13" s="148"/>
-      <c r="AZ13" s="148"/>
-      <c r="BA13" s="148"/>
-      <c r="BB13" s="148"/>
-      <c r="BC13" s="148"/>
-      <c r="BD13" s="148"/>
-      <c r="BE13" s="148"/>
-      <c r="BF13" s="148"/>
-      <c r="BG13" s="148"/>
-      <c r="BH13" s="148"/>
+      <c r="AQ13" s="128"/>
+      <c r="AR13" s="128"/>
+      <c r="AS13" s="128"/>
+      <c r="AT13" s="128"/>
+      <c r="AU13" s="128"/>
+      <c r="AV13" s="128"/>
+      <c r="AW13" s="128"/>
+      <c r="AX13" s="128"/>
+      <c r="AY13" s="128"/>
+      <c r="AZ13" s="128"/>
+      <c r="BA13" s="128"/>
+      <c r="BB13" s="128"/>
+      <c r="BC13" s="128"/>
+      <c r="BD13" s="128"/>
+      <c r="BE13" s="128"/>
+      <c r="BF13" s="128"/>
+      <c r="BG13" s="128"/>
+      <c r="BH13" s="128"/>
     </row>
     <row r="14" spans="1:60" ht="13">
       <c r="A14" s="26" t="s">
@@ -42667,46 +42605,46 @@
         <v>100</v>
       </c>
       <c r="T14" s="27"/>
-      <c r="U14" s="148"/>
-      <c r="V14" s="148"/>
-      <c r="W14" s="168"/>
-      <c r="X14" s="168"/>
-      <c r="Y14" s="148"/>
-      <c r="Z14" s="169"/>
-      <c r="AA14" s="170"/>
-      <c r="AB14" s="171"/>
-      <c r="AC14" s="169"/>
-      <c r="AD14" s="170"/>
-      <c r="AE14" s="172"/>
-      <c r="AF14" s="172"/>
-      <c r="AG14" s="170"/>
-      <c r="AH14" s="148"/>
-      <c r="AI14" s="169"/>
-      <c r="AJ14" s="170"/>
-      <c r="AK14" s="172"/>
-      <c r="AL14" s="169"/>
-      <c r="AM14" s="170"/>
-      <c r="AN14" s="171"/>
-      <c r="AO14" s="169"/>
-      <c r="AP14" s="170"/>
-      <c r="AQ14" s="148"/>
-      <c r="AR14" s="148"/>
-      <c r="AS14" s="148"/>
-      <c r="AT14" s="148"/>
-      <c r="AU14" s="148"/>
-      <c r="AV14" s="148"/>
-      <c r="AW14" s="148"/>
-      <c r="AX14" s="148"/>
-      <c r="AY14" s="148"/>
-      <c r="AZ14" s="148"/>
-      <c r="BA14" s="148"/>
-      <c r="BB14" s="148"/>
-      <c r="BC14" s="148"/>
-      <c r="BD14" s="148"/>
-      <c r="BE14" s="148"/>
-      <c r="BF14" s="148"/>
-      <c r="BG14" s="148"/>
-      <c r="BH14" s="148"/>
+      <c r="U14" s="128"/>
+      <c r="V14" s="128"/>
+      <c r="W14" s="138"/>
+      <c r="X14" s="138"/>
+      <c r="Y14" s="128"/>
+      <c r="Z14" s="139"/>
+      <c r="AA14" s="140"/>
+      <c r="AB14" s="141"/>
+      <c r="AC14" s="139"/>
+      <c r="AD14" s="140"/>
+      <c r="AE14" s="142"/>
+      <c r="AF14" s="142"/>
+      <c r="AG14" s="140"/>
+      <c r="AH14" s="128"/>
+      <c r="AI14" s="139"/>
+      <c r="AJ14" s="140"/>
+      <c r="AK14" s="142"/>
+      <c r="AL14" s="139"/>
+      <c r="AM14" s="140"/>
+      <c r="AN14" s="141"/>
+      <c r="AO14" s="139"/>
+      <c r="AP14" s="140"/>
+      <c r="AQ14" s="128"/>
+      <c r="AR14" s="128"/>
+      <c r="AS14" s="128"/>
+      <c r="AT14" s="128"/>
+      <c r="AU14" s="128"/>
+      <c r="AV14" s="128"/>
+      <c r="AW14" s="128"/>
+      <c r="AX14" s="128"/>
+      <c r="AY14" s="128"/>
+      <c r="AZ14" s="128"/>
+      <c r="BA14" s="128"/>
+      <c r="BB14" s="128"/>
+      <c r="BC14" s="128"/>
+      <c r="BD14" s="128"/>
+      <c r="BE14" s="128"/>
+      <c r="BF14" s="128"/>
+      <c r="BG14" s="128"/>
+      <c r="BH14" s="128"/>
     </row>
     <row r="15" spans="1:60" ht="13">
       <c r="A15" s="26"/>
@@ -42729,48 +42667,48 @@
       <c r="R15" s="29"/>
       <c r="S15" s="27"/>
       <c r="T15" s="27"/>
-      <c r="U15" s="148"/>
-      <c r="V15" s="148"/>
-      <c r="W15" s="174" t="s">
+      <c r="U15" s="128"/>
+      <c r="V15" s="128"/>
+      <c r="W15" s="144" t="s">
         <v>58</v>
       </c>
-      <c r="X15" s="168"/>
-      <c r="Y15" s="148"/>
-      <c r="Z15" s="148"/>
-      <c r="AA15" s="170"/>
-      <c r="AB15" s="148"/>
-      <c r="AC15" s="148"/>
-      <c r="AD15" s="170"/>
-      <c r="AE15" s="148"/>
-      <c r="AF15" s="148"/>
-      <c r="AG15" s="170"/>
-      <c r="AH15" s="148"/>
-      <c r="AI15" s="148"/>
-      <c r="AJ15" s="170"/>
-      <c r="AK15" s="148"/>
-      <c r="AL15" s="148"/>
-      <c r="AM15" s="170"/>
-      <c r="AN15" s="171"/>
-      <c r="AO15" s="148"/>
-      <c r="AP15" s="170"/>
-      <c r="AQ15" s="148"/>
-      <c r="AR15" s="148"/>
-      <c r="AS15" s="148"/>
-      <c r="AT15" s="148"/>
-      <c r="AU15" s="148"/>
-      <c r="AV15" s="148"/>
-      <c r="AW15" s="148"/>
-      <c r="AX15" s="148"/>
-      <c r="AY15" s="148"/>
-      <c r="AZ15" s="148"/>
-      <c r="BA15" s="148"/>
-      <c r="BB15" s="148"/>
-      <c r="BC15" s="148"/>
-      <c r="BD15" s="148"/>
-      <c r="BE15" s="148"/>
-      <c r="BF15" s="148"/>
-      <c r="BG15" s="148"/>
-      <c r="BH15" s="148"/>
+      <c r="X15" s="138"/>
+      <c r="Y15" s="128"/>
+      <c r="Z15" s="128"/>
+      <c r="AA15" s="140"/>
+      <c r="AB15" s="128"/>
+      <c r="AC15" s="128"/>
+      <c r="AD15" s="140"/>
+      <c r="AE15" s="128"/>
+      <c r="AF15" s="128"/>
+      <c r="AG15" s="140"/>
+      <c r="AH15" s="128"/>
+      <c r="AI15" s="128"/>
+      <c r="AJ15" s="140"/>
+      <c r="AK15" s="128"/>
+      <c r="AL15" s="128"/>
+      <c r="AM15" s="140"/>
+      <c r="AN15" s="141"/>
+      <c r="AO15" s="128"/>
+      <c r="AP15" s="140"/>
+      <c r="AQ15" s="128"/>
+      <c r="AR15" s="128"/>
+      <c r="AS15" s="128"/>
+      <c r="AT15" s="128"/>
+      <c r="AU15" s="128"/>
+      <c r="AV15" s="128"/>
+      <c r="AW15" s="128"/>
+      <c r="AX15" s="128"/>
+      <c r="AY15" s="128"/>
+      <c r="AZ15" s="128"/>
+      <c r="BA15" s="128"/>
+      <c r="BB15" s="128"/>
+      <c r="BC15" s="128"/>
+      <c r="BD15" s="128"/>
+      <c r="BE15" s="128"/>
+      <c r="BF15" s="128"/>
+      <c r="BG15" s="128"/>
+      <c r="BH15" s="128"/>
     </row>
     <row r="16" spans="1:60" ht="13">
       <c r="A16" s="31" t="s">
@@ -42780,78 +42718,78 @@
       <c r="C16" s="25"/>
       <c r="Q16" s="27"/>
       <c r="R16" s="29"/>
-      <c r="U16" s="148"/>
-      <c r="V16" s="148"/>
-      <c r="W16" s="168" t="s">
+      <c r="U16" s="128"/>
+      <c r="V16" s="128"/>
+      <c r="W16" s="138" t="s">
         <v>195</v>
       </c>
-      <c r="X16" s="168"/>
-      <c r="Y16" s="148"/>
-      <c r="Z16" s="169">
+      <c r="X16" s="138"/>
+      <c r="Y16" s="128"/>
+      <c r="Z16" s="139">
         <v>4.03</v>
       </c>
-      <c r="AA16" s="170">
+      <c r="AA16" s="140">
         <f t="shared" si="0"/>
         <v>4.03</v>
       </c>
-      <c r="AB16" s="171"/>
-      <c r="AC16" s="169">
+      <c r="AB16" s="141"/>
+      <c r="AC16" s="139">
         <v>56.09</v>
       </c>
-      <c r="AD16" s="170">
+      <c r="AD16" s="140">
         <f t="shared" si="1"/>
         <v>56.09</v>
       </c>
-      <c r="AE16" s="172"/>
-      <c r="AF16" s="172">
+      <c r="AE16" s="142"/>
+      <c r="AF16" s="142">
         <v>-9457</v>
       </c>
-      <c r="AG16" s="170">
+      <c r="AG16" s="140">
         <f t="shared" si="2"/>
         <v>-9457</v>
       </c>
-      <c r="AH16" s="148"/>
-      <c r="AI16" s="169">
+      <c r="AH16" s="128"/>
+      <c r="AI16" s="139">
         <v>-9.4600000000000009</v>
       </c>
-      <c r="AJ16" s="170">
+      <c r="AJ16" s="140">
         <f t="shared" si="3"/>
         <v>-9.4600000000000009</v>
       </c>
-      <c r="AK16" s="172"/>
-      <c r="AL16" s="169">
+      <c r="AK16" s="142"/>
+      <c r="AL16" s="139">
         <v>-0.02</v>
       </c>
-      <c r="AM16" s="170">
+      <c r="AM16" s="140">
         <f t="shared" si="4"/>
         <v>-0.02</v>
       </c>
-      <c r="AN16" s="171"/>
-      <c r="AO16" s="169">
+      <c r="AN16" s="141"/>
+      <c r="AO16" s="139">
         <v>55.87</v>
       </c>
-      <c r="AP16" s="170">
+      <c r="AP16" s="140">
         <f t="shared" si="5"/>
         <v>55.87</v>
       </c>
-      <c r="AQ16" s="148"/>
-      <c r="AR16" s="148"/>
-      <c r="AS16" s="148"/>
-      <c r="AT16" s="148"/>
-      <c r="AU16" s="148"/>
-      <c r="AV16" s="148"/>
-      <c r="AW16" s="148"/>
-      <c r="AX16" s="148"/>
-      <c r="AY16" s="148"/>
-      <c r="AZ16" s="148"/>
-      <c r="BA16" s="148"/>
-      <c r="BB16" s="148"/>
-      <c r="BC16" s="148"/>
-      <c r="BD16" s="148"/>
-      <c r="BE16" s="148"/>
-      <c r="BF16" s="148"/>
-      <c r="BG16" s="148"/>
-      <c r="BH16" s="148"/>
+      <c r="AQ16" s="128"/>
+      <c r="AR16" s="128"/>
+      <c r="AS16" s="128"/>
+      <c r="AT16" s="128"/>
+      <c r="AU16" s="128"/>
+      <c r="AV16" s="128"/>
+      <c r="AW16" s="128"/>
+      <c r="AX16" s="128"/>
+      <c r="AY16" s="128"/>
+      <c r="AZ16" s="128"/>
+      <c r="BA16" s="128"/>
+      <c r="BB16" s="128"/>
+      <c r="BC16" s="128"/>
+      <c r="BD16" s="128"/>
+      <c r="BE16" s="128"/>
+      <c r="BF16" s="128"/>
+      <c r="BG16" s="128"/>
+      <c r="BH16" s="128"/>
     </row>
     <row r="17" spans="1:60" ht="13">
       <c r="A17" s="26" t="s">
@@ -42888,78 +42826,78 @@
         <v>55.87</v>
       </c>
       <c r="T17" s="27"/>
-      <c r="U17" s="148"/>
-      <c r="V17" s="148"/>
-      <c r="W17" s="168" t="s">
+      <c r="U17" s="128"/>
+      <c r="V17" s="128"/>
+      <c r="W17" s="138" t="s">
         <v>196</v>
       </c>
-      <c r="X17" s="168"/>
-      <c r="Y17" s="148"/>
-      <c r="Z17" s="169">
+      <c r="X17" s="138"/>
+      <c r="Y17" s="128"/>
+      <c r="Z17" s="139">
         <v>4.68</v>
       </c>
-      <c r="AA17" s="170">
+      <c r="AA17" s="140">
         <f t="shared" si="0"/>
         <v>4.68</v>
       </c>
-      <c r="AB17" s="171"/>
-      <c r="AC17" s="169">
+      <c r="AB17" s="141"/>
+      <c r="AC17" s="139">
         <v>48.1</v>
       </c>
-      <c r="AD17" s="170">
+      <c r="AD17" s="140">
         <f t="shared" si="1"/>
         <v>48.1</v>
       </c>
-      <c r="AE17" s="172"/>
-      <c r="AF17" s="172">
+      <c r="AE17" s="142"/>
+      <c r="AF17" s="142">
         <v>-16223</v>
       </c>
-      <c r="AG17" s="170">
+      <c r="AG17" s="140">
         <f t="shared" si="2"/>
         <v>-16223</v>
       </c>
-      <c r="AH17" s="148"/>
-      <c r="AI17" s="169">
+      <c r="AH17" s="128"/>
+      <c r="AI17" s="139">
         <v>-10.39</v>
       </c>
-      <c r="AJ17" s="170">
+      <c r="AJ17" s="140">
         <f t="shared" si="3"/>
         <v>-10.39</v>
       </c>
-      <c r="AK17" s="172"/>
-      <c r="AL17" s="169">
+      <c r="AK17" s="142"/>
+      <c r="AL17" s="139">
         <v>-0.46</v>
       </c>
-      <c r="AM17" s="170">
+      <c r="AM17" s="140">
         <f t="shared" si="4"/>
         <v>-0.46</v>
       </c>
-      <c r="AN17" s="171"/>
-      <c r="AO17" s="169">
+      <c r="AN17" s="141"/>
+      <c r="AO17" s="139">
         <v>43.22</v>
       </c>
-      <c r="AP17" s="170">
+      <c r="AP17" s="140">
         <f t="shared" si="5"/>
         <v>43.22</v>
       </c>
-      <c r="AQ17" s="148"/>
-      <c r="AR17" s="148"/>
-      <c r="AS17" s="148"/>
-      <c r="AT17" s="148"/>
-      <c r="AU17" s="148"/>
-      <c r="AV17" s="148"/>
-      <c r="AW17" s="148"/>
-      <c r="AX17" s="148"/>
-      <c r="AY17" s="148"/>
-      <c r="AZ17" s="148"/>
-      <c r="BA17" s="148"/>
-      <c r="BB17" s="148"/>
-      <c r="BC17" s="148"/>
-      <c r="BD17" s="148"/>
-      <c r="BE17" s="148"/>
-      <c r="BF17" s="148"/>
-      <c r="BG17" s="148"/>
-      <c r="BH17" s="148"/>
+      <c r="AQ17" s="128"/>
+      <c r="AR17" s="128"/>
+      <c r="AS17" s="128"/>
+      <c r="AT17" s="128"/>
+      <c r="AU17" s="128"/>
+      <c r="AV17" s="128"/>
+      <c r="AW17" s="128"/>
+      <c r="AX17" s="128"/>
+      <c r="AY17" s="128"/>
+      <c r="AZ17" s="128"/>
+      <c r="BA17" s="128"/>
+      <c r="BB17" s="128"/>
+      <c r="BC17" s="128"/>
+      <c r="BD17" s="128"/>
+      <c r="BE17" s="128"/>
+      <c r="BF17" s="128"/>
+      <c r="BG17" s="128"/>
+      <c r="BH17" s="128"/>
     </row>
     <row r="18" spans="1:60" ht="13">
       <c r="A18" s="26" t="s">
@@ -42996,78 +42934,78 @@
         <v>43.22</v>
       </c>
       <c r="T18" s="27"/>
-      <c r="U18" s="148"/>
-      <c r="V18" s="148"/>
-      <c r="W18" s="168" t="s">
+      <c r="U18" s="128"/>
+      <c r="V18" s="128"/>
+      <c r="W18" s="138" t="s">
         <v>197</v>
       </c>
-      <c r="X18" s="168"/>
-      <c r="Y18" s="148"/>
-      <c r="Z18" s="169">
+      <c r="X18" s="138"/>
+      <c r="Y18" s="128"/>
+      <c r="Z18" s="139">
         <v>6.74</v>
       </c>
-      <c r="AA18" s="170">
+      <c r="AA18" s="140">
         <f t="shared" si="0"/>
         <v>6.74</v>
       </c>
-      <c r="AB18" s="171"/>
-      <c r="AC18" s="169">
+      <c r="AB18" s="141"/>
+      <c r="AC18" s="139">
         <v>36.78</v>
       </c>
-      <c r="AD18" s="170">
+      <c r="AD18" s="140">
         <f t="shared" si="1"/>
         <v>36.78</v>
       </c>
-      <c r="AE18" s="172"/>
-      <c r="AF18" s="172">
+      <c r="AE18" s="142"/>
+      <c r="AF18" s="142">
         <v>-62007</v>
       </c>
-      <c r="AG18" s="170">
+      <c r="AG18" s="140">
         <f t="shared" si="2"/>
         <v>-62007</v>
       </c>
-      <c r="AH18" s="148"/>
-      <c r="AI18" s="169">
+      <c r="AH18" s="128"/>
+      <c r="AI18" s="139">
         <v>-13.37</v>
       </c>
-      <c r="AJ18" s="170">
+      <c r="AJ18" s="140">
         <f t="shared" si="3"/>
         <v>-13.37</v>
       </c>
-      <c r="AK18" s="172"/>
-      <c r="AL18" s="169">
+      <c r="AK18" s="142"/>
+      <c r="AL18" s="139">
         <v>-1.1299999999999999</v>
       </c>
-      <c r="AM18" s="170">
+      <c r="AM18" s="140">
         <f t="shared" si="4"/>
         <v>-1.1299999999999999</v>
       </c>
-      <c r="AN18" s="171"/>
-      <c r="AO18" s="169">
+      <c r="AN18" s="141"/>
+      <c r="AO18" s="139">
         <v>24.83</v>
       </c>
-      <c r="AP18" s="170">
+      <c r="AP18" s="140">
         <f t="shared" si="5"/>
         <v>24.83</v>
       </c>
-      <c r="AQ18" s="148"/>
-      <c r="AR18" s="148"/>
-      <c r="AS18" s="148"/>
-      <c r="AT18" s="148"/>
-      <c r="AU18" s="148"/>
-      <c r="AV18" s="148"/>
-      <c r="AW18" s="148"/>
-      <c r="AX18" s="148"/>
-      <c r="AY18" s="148"/>
-      <c r="AZ18" s="148"/>
-      <c r="BA18" s="148"/>
-      <c r="BB18" s="148"/>
-      <c r="BC18" s="148"/>
-      <c r="BD18" s="148"/>
-      <c r="BE18" s="148"/>
-      <c r="BF18" s="148"/>
-      <c r="BG18" s="148"/>
-      <c r="BH18" s="148"/>
+      <c r="AQ18" s="128"/>
+      <c r="AR18" s="128"/>
+      <c r="AS18" s="128"/>
+      <c r="AT18" s="128"/>
+      <c r="AU18" s="128"/>
+      <c r="AV18" s="128"/>
+      <c r="AW18" s="128"/>
+      <c r="AX18" s="128"/>
+      <c r="AY18" s="128"/>
+      <c r="AZ18" s="128"/>
+      <c r="BA18" s="128"/>
+      <c r="BB18" s="128"/>
+      <c r="BC18" s="128"/>
+      <c r="BD18" s="128"/>
+      <c r="BE18" s="128"/>
+      <c r="BF18" s="128"/>
+      <c r="BG18" s="128"/>
+      <c r="BH18" s="128"/>
     </row>
     <row r="19" spans="1:60" ht="13">
       <c r="A19" s="26" t="s">
@@ -43104,78 +43042,78 @@
         <v>24.83</v>
       </c>
       <c r="T19" s="27"/>
-      <c r="U19" s="148"/>
-      <c r="V19" s="148"/>
-      <c r="W19" s="168" t="s">
+      <c r="U19" s="128"/>
+      <c r="V19" s="128"/>
+      <c r="W19" s="138" t="s">
         <v>198</v>
       </c>
-      <c r="X19" s="168"/>
-      <c r="Y19" s="148"/>
-      <c r="Z19" s="169">
+      <c r="X19" s="138"/>
+      <c r="Y19" s="128"/>
+      <c r="Z19" s="139">
         <v>7.33</v>
       </c>
-      <c r="AA19" s="170">
+      <c r="AA19" s="140">
         <f t="shared" si="0"/>
         <v>7.33</v>
       </c>
-      <c r="AB19" s="171"/>
-      <c r="AC19" s="169">
+      <c r="AB19" s="141"/>
+      <c r="AC19" s="139">
         <v>31.05</v>
       </c>
-      <c r="AD19" s="170">
+      <c r="AD19" s="140">
         <f t="shared" si="1"/>
         <v>31.05</v>
       </c>
-      <c r="AE19" s="172"/>
-      <c r="AF19" s="172">
+      <c r="AE19" s="142"/>
+      <c r="AF19" s="142">
         <v>-104678</v>
       </c>
-      <c r="AG19" s="170">
+      <c r="AG19" s="140">
         <f t="shared" si="2"/>
         <v>-104678</v>
       </c>
-      <c r="AH19" s="148"/>
-      <c r="AI19" s="169">
+      <c r="AH19" s="128"/>
+      <c r="AI19" s="139">
         <v>-13.91</v>
       </c>
-      <c r="AJ19" s="170">
+      <c r="AJ19" s="140">
         <f t="shared" si="3"/>
         <v>-13.91</v>
       </c>
-      <c r="AK19" s="172"/>
-      <c r="AL19" s="169">
+      <c r="AK19" s="142"/>
+      <c r="AL19" s="139">
         <v>-1.04</v>
       </c>
-      <c r="AM19" s="170">
+      <c r="AM19" s="140">
         <f t="shared" si="4"/>
         <v>-1.04</v>
       </c>
-      <c r="AN19" s="171"/>
-      <c r="AO19" s="169">
+      <c r="AN19" s="141"/>
+      <c r="AO19" s="139">
         <v>20.010000000000002</v>
       </c>
-      <c r="AP19" s="170">
+      <c r="AP19" s="140">
         <f t="shared" si="5"/>
         <v>20.010000000000002</v>
       </c>
-      <c r="AQ19" s="148"/>
-      <c r="AR19" s="148"/>
-      <c r="AS19" s="148"/>
-      <c r="AT19" s="148"/>
-      <c r="AU19" s="148"/>
-      <c r="AV19" s="148"/>
-      <c r="AW19" s="148"/>
-      <c r="AX19" s="148"/>
-      <c r="AY19" s="148"/>
-      <c r="AZ19" s="148"/>
-      <c r="BA19" s="148"/>
-      <c r="BB19" s="148"/>
-      <c r="BC19" s="148"/>
-      <c r="BD19" s="148"/>
-      <c r="BE19" s="148"/>
-      <c r="BF19" s="148"/>
-      <c r="BG19" s="148"/>
-      <c r="BH19" s="148"/>
+      <c r="AQ19" s="128"/>
+      <c r="AR19" s="128"/>
+      <c r="AS19" s="128"/>
+      <c r="AT19" s="128"/>
+      <c r="AU19" s="128"/>
+      <c r="AV19" s="128"/>
+      <c r="AW19" s="128"/>
+      <c r="AX19" s="128"/>
+      <c r="AY19" s="128"/>
+      <c r="AZ19" s="128"/>
+      <c r="BA19" s="128"/>
+      <c r="BB19" s="128"/>
+      <c r="BC19" s="128"/>
+      <c r="BD19" s="128"/>
+      <c r="BE19" s="128"/>
+      <c r="BF19" s="128"/>
+      <c r="BG19" s="128"/>
+      <c r="BH19" s="128"/>
     </row>
     <row r="20" spans="1:60" ht="13">
       <c r="A20" s="26" t="s">
@@ -43212,78 +43150,78 @@
         <v>20.010000000000002</v>
       </c>
       <c r="T20" s="27"/>
-      <c r="U20" s="148"/>
-      <c r="V20" s="148"/>
-      <c r="W20" s="168" t="s">
+      <c r="U20" s="128"/>
+      <c r="V20" s="128"/>
+      <c r="W20" s="138" t="s">
         <v>199</v>
       </c>
-      <c r="X20" s="168"/>
-      <c r="Y20" s="148"/>
-      <c r="Z20" s="169">
+      <c r="X20" s="138"/>
+      <c r="Y20" s="128"/>
+      <c r="Z20" s="139">
         <v>7.81</v>
       </c>
-      <c r="AA20" s="170">
+      <c r="AA20" s="140">
         <f t="shared" si="0"/>
         <v>7.81</v>
       </c>
-      <c r="AB20" s="171"/>
-      <c r="AC20" s="169">
+      <c r="AB20" s="141"/>
+      <c r="AC20" s="139">
         <v>18.63</v>
       </c>
-      <c r="AD20" s="170">
+      <c r="AD20" s="140">
         <f t="shared" si="1"/>
         <v>18.63</v>
       </c>
-      <c r="AE20" s="172"/>
-      <c r="AF20" s="172">
+      <c r="AE20" s="142"/>
+      <c r="AF20" s="142">
         <v>-314150</v>
       </c>
-      <c r="AG20" s="170">
+      <c r="AG20" s="140">
         <f t="shared" si="2"/>
         <v>-314150</v>
       </c>
-      <c r="AH20" s="148"/>
-      <c r="AI20" s="169">
+      <c r="AH20" s="128"/>
+      <c r="AI20" s="139">
         <v>-13.68</v>
       </c>
-      <c r="AJ20" s="170">
+      <c r="AJ20" s="140">
         <f t="shared" si="3"/>
         <v>-13.68</v>
       </c>
-      <c r="AK20" s="172"/>
-      <c r="AL20" s="169">
+      <c r="AK20" s="142"/>
+      <c r="AL20" s="139">
         <v>-0.6</v>
       </c>
-      <c r="AM20" s="170">
+      <c r="AM20" s="140">
         <f t="shared" si="4"/>
         <v>-0.6</v>
       </c>
-      <c r="AN20" s="171"/>
-      <c r="AO20" s="169">
+      <c r="AN20" s="141"/>
+      <c r="AO20" s="139">
         <v>12.25</v>
       </c>
-      <c r="AP20" s="170">
+      <c r="AP20" s="140">
         <f t="shared" si="5"/>
         <v>12.25</v>
       </c>
-      <c r="AQ20" s="148"/>
-      <c r="AR20" s="148"/>
-      <c r="AS20" s="148"/>
-      <c r="AT20" s="148"/>
-      <c r="AU20" s="148"/>
-      <c r="AV20" s="148"/>
-      <c r="AW20" s="148"/>
-      <c r="AX20" s="148"/>
-      <c r="AY20" s="148"/>
-      <c r="AZ20" s="148"/>
-      <c r="BA20" s="148"/>
-      <c r="BB20" s="148"/>
-      <c r="BC20" s="148"/>
-      <c r="BD20" s="148"/>
-      <c r="BE20" s="148"/>
-      <c r="BF20" s="148"/>
-      <c r="BG20" s="148"/>
-      <c r="BH20" s="148"/>
+      <c r="AQ20" s="128"/>
+      <c r="AR20" s="128"/>
+      <c r="AS20" s="128"/>
+      <c r="AT20" s="128"/>
+      <c r="AU20" s="128"/>
+      <c r="AV20" s="128"/>
+      <c r="AW20" s="128"/>
+      <c r="AX20" s="128"/>
+      <c r="AY20" s="128"/>
+      <c r="AZ20" s="128"/>
+      <c r="BA20" s="128"/>
+      <c r="BB20" s="128"/>
+      <c r="BC20" s="128"/>
+      <c r="BD20" s="128"/>
+      <c r="BE20" s="128"/>
+      <c r="BF20" s="128"/>
+      <c r="BG20" s="128"/>
+      <c r="BH20" s="128"/>
     </row>
     <row r="21" spans="1:60" ht="13">
       <c r="A21" s="26" t="s">
@@ -43320,46 +43258,46 @@
         <v>12.25</v>
       </c>
       <c r="T21" s="27"/>
-      <c r="U21" s="148"/>
-      <c r="V21" s="175"/>
-      <c r="W21" s="175"/>
-      <c r="X21" s="175"/>
-      <c r="Y21" s="175"/>
-      <c r="Z21" s="175"/>
-      <c r="AA21" s="175"/>
-      <c r="AB21" s="175"/>
-      <c r="AC21" s="175"/>
-      <c r="AD21" s="175"/>
-      <c r="AE21" s="175"/>
-      <c r="AF21" s="175"/>
-      <c r="AG21" s="175"/>
-      <c r="AH21" s="175"/>
-      <c r="AI21" s="175"/>
-      <c r="AJ21" s="175"/>
-      <c r="AK21" s="175"/>
-      <c r="AL21" s="175"/>
-      <c r="AM21" s="175"/>
-      <c r="AN21" s="175"/>
-      <c r="AO21" s="175"/>
-      <c r="AP21" s="175"/>
-      <c r="AQ21" s="148"/>
-      <c r="AR21" s="148"/>
-      <c r="AS21" s="148"/>
-      <c r="AT21" s="148"/>
-      <c r="AU21" s="148"/>
-      <c r="AV21" s="148"/>
-      <c r="AW21" s="148"/>
-      <c r="AX21" s="148"/>
-      <c r="AY21" s="148"/>
-      <c r="AZ21" s="148"/>
-      <c r="BA21" s="148"/>
-      <c r="BB21" s="148"/>
-      <c r="BC21" s="148"/>
-      <c r="BD21" s="148"/>
-      <c r="BE21" s="148"/>
-      <c r="BF21" s="148"/>
-      <c r="BG21" s="148"/>
-      <c r="BH21" s="148"/>
+      <c r="U21" s="128"/>
+      <c r="V21" s="145"/>
+      <c r="W21" s="145"/>
+      <c r="X21" s="145"/>
+      <c r="Y21" s="145"/>
+      <c r="Z21" s="145"/>
+      <c r="AA21" s="145"/>
+      <c r="AB21" s="145"/>
+      <c r="AC21" s="145"/>
+      <c r="AD21" s="145"/>
+      <c r="AE21" s="145"/>
+      <c r="AF21" s="145"/>
+      <c r="AG21" s="145"/>
+      <c r="AH21" s="145"/>
+      <c r="AI21" s="145"/>
+      <c r="AJ21" s="145"/>
+      <c r="AK21" s="145"/>
+      <c r="AL21" s="145"/>
+      <c r="AM21" s="145"/>
+      <c r="AN21" s="145"/>
+      <c r="AO21" s="145"/>
+      <c r="AP21" s="145"/>
+      <c r="AQ21" s="128"/>
+      <c r="AR21" s="128"/>
+      <c r="AS21" s="128"/>
+      <c r="AT21" s="128"/>
+      <c r="AU21" s="128"/>
+      <c r="AV21" s="128"/>
+      <c r="AW21" s="128"/>
+      <c r="AX21" s="128"/>
+      <c r="AY21" s="128"/>
+      <c r="AZ21" s="128"/>
+      <c r="BA21" s="128"/>
+      <c r="BB21" s="128"/>
+      <c r="BC21" s="128"/>
+      <c r="BD21" s="128"/>
+      <c r="BE21" s="128"/>
+      <c r="BF21" s="128"/>
+      <c r="BG21" s="128"/>
+      <c r="BH21" s="128"/>
     </row>
     <row r="22" spans="1:60" ht="13">
       <c r="A22" s="32"/>
@@ -43381,48 +43319,48 @@
       <c r="Q22" s="32"/>
       <c r="R22" s="32"/>
       <c r="S22" s="32"/>
-      <c r="U22" s="148"/>
-      <c r="V22" s="176" t="s">
+      <c r="U22" s="128"/>
+      <c r="V22" s="146" t="s">
         <v>288</v>
       </c>
-      <c r="W22" s="148"/>
-      <c r="X22" s="176"/>
-      <c r="Y22" s="148"/>
-      <c r="Z22" s="148"/>
-      <c r="AA22" s="148"/>
-      <c r="AB22" s="148"/>
-      <c r="AC22" s="148"/>
-      <c r="AD22" s="148"/>
-      <c r="AE22" s="148"/>
-      <c r="AF22" s="148"/>
-      <c r="AG22" s="148"/>
-      <c r="AH22" s="148"/>
-      <c r="AI22" s="148"/>
-      <c r="AJ22" s="148"/>
-      <c r="AK22" s="148"/>
-      <c r="AL22" s="148"/>
-      <c r="AM22" s="148"/>
-      <c r="AN22" s="148"/>
-      <c r="AO22" s="148"/>
-      <c r="AP22" s="148"/>
-      <c r="AQ22" s="148"/>
-      <c r="AR22" s="148"/>
-      <c r="AS22" s="148"/>
-      <c r="AT22" s="148"/>
-      <c r="AU22" s="148"/>
-      <c r="AV22" s="148"/>
-      <c r="AW22" s="148"/>
-      <c r="AX22" s="148"/>
-      <c r="AY22" s="148"/>
-      <c r="AZ22" s="148"/>
-      <c r="BA22" s="148"/>
-      <c r="BB22" s="148"/>
-      <c r="BC22" s="148"/>
-      <c r="BD22" s="148"/>
-      <c r="BE22" s="148"/>
-      <c r="BF22" s="148"/>
-      <c r="BG22" s="148"/>
-      <c r="BH22" s="148"/>
+      <c r="W22" s="128"/>
+      <c r="X22" s="146"/>
+      <c r="Y22" s="128"/>
+      <c r="Z22" s="128"/>
+      <c r="AA22" s="128"/>
+      <c r="AB22" s="128"/>
+      <c r="AC22" s="128"/>
+      <c r="AD22" s="128"/>
+      <c r="AE22" s="128"/>
+      <c r="AF22" s="128"/>
+      <c r="AG22" s="128"/>
+      <c r="AH22" s="128"/>
+      <c r="AI22" s="128"/>
+      <c r="AJ22" s="128"/>
+      <c r="AK22" s="128"/>
+      <c r="AL22" s="128"/>
+      <c r="AM22" s="128"/>
+      <c r="AN22" s="128"/>
+      <c r="AO22" s="128"/>
+      <c r="AP22" s="128"/>
+      <c r="AQ22" s="128"/>
+      <c r="AR22" s="128"/>
+      <c r="AS22" s="128"/>
+      <c r="AT22" s="128"/>
+      <c r="AU22" s="128"/>
+      <c r="AV22" s="128"/>
+      <c r="AW22" s="128"/>
+      <c r="AX22" s="128"/>
+      <c r="AY22" s="128"/>
+      <c r="AZ22" s="128"/>
+      <c r="BA22" s="128"/>
+      <c r="BB22" s="128"/>
+      <c r="BC22" s="128"/>
+      <c r="BD22" s="128"/>
+      <c r="BE22" s="128"/>
+      <c r="BF22" s="128"/>
+      <c r="BG22" s="128"/>
+      <c r="BH22" s="128"/>
     </row>
     <row r="23" spans="1:60" ht="13">
       <c r="A23" s="33" t="s">
@@ -43446,46 +43384,46 @@
       <c r="Q23" s="25"/>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
-      <c r="U23" s="148"/>
-      <c r="V23" s="148"/>
-      <c r="W23" s="148"/>
-      <c r="X23" s="148"/>
-      <c r="Y23" s="148"/>
-      <c r="Z23" s="148"/>
-      <c r="AA23" s="148"/>
-      <c r="AB23" s="148"/>
-      <c r="AC23" s="148"/>
-      <c r="AD23" s="148"/>
-      <c r="AE23" s="148"/>
-      <c r="AF23" s="148"/>
-      <c r="AG23" s="148"/>
-      <c r="AH23" s="148"/>
-      <c r="AI23" s="148"/>
-      <c r="AJ23" s="148"/>
-      <c r="AK23" s="148"/>
-      <c r="AL23" s="148"/>
-      <c r="AM23" s="148"/>
-      <c r="AN23" s="148"/>
-      <c r="AO23" s="148"/>
-      <c r="AP23" s="148"/>
-      <c r="AQ23" s="148"/>
-      <c r="AR23" s="148"/>
-      <c r="AS23" s="148"/>
-      <c r="AT23" s="148"/>
-      <c r="AU23" s="148"/>
-      <c r="AV23" s="148"/>
-      <c r="AW23" s="148"/>
-      <c r="AX23" s="148"/>
-      <c r="AY23" s="148"/>
-      <c r="AZ23" s="148"/>
-      <c r="BA23" s="148"/>
-      <c r="BB23" s="148"/>
-      <c r="BC23" s="148"/>
-      <c r="BD23" s="148"/>
-      <c r="BE23" s="148"/>
-      <c r="BF23" s="148"/>
-      <c r="BG23" s="148"/>
-      <c r="BH23" s="148"/>
+      <c r="U23" s="128"/>
+      <c r="V23" s="128"/>
+      <c r="W23" s="128"/>
+      <c r="X23" s="128"/>
+      <c r="Y23" s="128"/>
+      <c r="Z23" s="128"/>
+      <c r="AA23" s="128"/>
+      <c r="AB23" s="128"/>
+      <c r="AC23" s="128"/>
+      <c r="AD23" s="128"/>
+      <c r="AE23" s="128"/>
+      <c r="AF23" s="128"/>
+      <c r="AG23" s="128"/>
+      <c r="AH23" s="128"/>
+      <c r="AI23" s="128"/>
+      <c r="AJ23" s="128"/>
+      <c r="AK23" s="128"/>
+      <c r="AL23" s="128"/>
+      <c r="AM23" s="128"/>
+      <c r="AN23" s="128"/>
+      <c r="AO23" s="128"/>
+      <c r="AP23" s="128"/>
+      <c r="AQ23" s="128"/>
+      <c r="AR23" s="128"/>
+      <c r="AS23" s="128"/>
+      <c r="AT23" s="128"/>
+      <c r="AU23" s="128"/>
+      <c r="AV23" s="128"/>
+      <c r="AW23" s="128"/>
+      <c r="AX23" s="128"/>
+      <c r="AY23" s="128"/>
+      <c r="AZ23" s="128"/>
+      <c r="BA23" s="128"/>
+      <c r="BB23" s="128"/>
+      <c r="BC23" s="128"/>
+      <c r="BD23" s="128"/>
+      <c r="BE23" s="128"/>
+      <c r="BF23" s="128"/>
+      <c r="BG23" s="128"/>
+      <c r="BH23" s="128"/>
     </row>
     <row r="24" spans="1:60" ht="12.75" customHeight="1">
       <c r="A24" s="25"/>
@@ -45001,16 +44939,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="M6:N7"/>
-    <mergeCell ref="P6:Q7"/>
-    <mergeCell ref="U3:V6"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="AF5:AG6"/>
-    <mergeCell ref="AI5:AJ6"/>
-    <mergeCell ref="AL5:AM6"/>
-    <mergeCell ref="AO5:AO6"/>
-    <mergeCell ref="P4:S5"/>
     <mergeCell ref="AP1:BH1"/>
     <mergeCell ref="AP3:AS4"/>
     <mergeCell ref="AP5:AQ6"/>
@@ -45026,6 +44954,16 @@
     <mergeCell ref="AC3:AD6"/>
     <mergeCell ref="AF3:AJ4"/>
     <mergeCell ref="AL3:AO4"/>
+    <mergeCell ref="AF5:AG6"/>
+    <mergeCell ref="AI5:AJ6"/>
+    <mergeCell ref="AL5:AM6"/>
+    <mergeCell ref="AO5:AO6"/>
+    <mergeCell ref="P4:S5"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="M6:N7"/>
+    <mergeCell ref="P6:Q7"/>
+    <mergeCell ref="U3:V6"/>
+    <mergeCell ref="S6:S7"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <conditionalFormatting sqref="AA8:AA20">
@@ -45114,7 +45052,6 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -46123,35 +46060,35 @@
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="137" t="s">
+      <c r="B40" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="138"/>
-      <c r="D40" s="138"/>
-      <c r="E40" s="138"/>
-      <c r="F40" s="138"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="138"/>
-      <c r="I40" s="138"/>
-      <c r="J40" s="138"/>
-      <c r="K40" s="138"/>
+      <c r="C40" s="171"/>
+      <c r="D40" s="171"/>
+      <c r="E40" s="171"/>
+      <c r="F40" s="171"/>
+      <c r="G40" s="171"/>
+      <c r="H40" s="171"/>
+      <c r="I40" s="171"/>
+      <c r="J40" s="171"/>
+      <c r="K40" s="171"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="139" t="s">
+      <c r="B41" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="139"/>
-      <c r="D41" s="139"/>
-      <c r="E41" s="139"/>
-      <c r="F41" s="139"/>
-      <c r="G41" s="139"/>
-      <c r="H41" s="139"/>
-      <c r="I41" s="139"/>
-      <c r="J41" s="139"/>
-      <c r="K41" s="139"/>
+      <c r="C41" s="172"/>
+      <c r="D41" s="172"/>
+      <c r="E41" s="172"/>
+      <c r="F41" s="172"/>
+      <c r="G41" s="172"/>
+      <c r="H41" s="172"/>
+      <c r="I41" s="172"/>
+      <c r="J41" s="172"/>
+      <c r="K41" s="172"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="9"/>
@@ -46811,24 +46748,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="173" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="140"/>
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
+      <c r="A2" s="173"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="36" t="s">
@@ -47299,15 +47236,15 @@
         <v>18.600000000000001</v>
       </c>
       <c r="G29" s="40"/>
-      <c r="I29" s="141" t="s">
+      <c r="I29" s="174" t="s">
         <v>85</v>
       </c>
-      <c r="J29" s="142"/>
-      <c r="K29" s="142"/>
-      <c r="L29" s="142"/>
-      <c r="M29" s="142"/>
-      <c r="N29" s="142"/>
-      <c r="O29" s="142"/>
+      <c r="J29" s="175"/>
+      <c r="K29" s="175"/>
+      <c r="L29" s="175"/>
+      <c r="M29" s="175"/>
+      <c r="N29" s="175"/>
+      <c r="O29" s="175"/>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="37">
@@ -47331,13 +47268,13 @@
       <c r="G30" s="41">
         <v>1980</v>
       </c>
-      <c r="I30" s="142"/>
-      <c r="J30" s="142"/>
-      <c r="K30" s="142"/>
-      <c r="L30" s="142"/>
-      <c r="M30" s="142"/>
-      <c r="N30" s="142"/>
-      <c r="O30" s="142"/>
+      <c r="I30" s="175"/>
+      <c r="J30" s="175"/>
+      <c r="K30" s="175"/>
+      <c r="L30" s="175"/>
+      <c r="M30" s="175"/>
+      <c r="N30" s="175"/>
+      <c r="O30" s="175"/>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="37">
@@ -47359,13 +47296,13 @@
         <v>19.3</v>
       </c>
       <c r="G31" s="40"/>
-      <c r="I31" s="142"/>
-      <c r="J31" s="142"/>
-      <c r="K31" s="142"/>
-      <c r="L31" s="142"/>
-      <c r="M31" s="142"/>
-      <c r="N31" s="142"/>
-      <c r="O31" s="142"/>
+      <c r="I31" s="175"/>
+      <c r="J31" s="175"/>
+      <c r="K31" s="175"/>
+      <c r="L31" s="175"/>
+      <c r="M31" s="175"/>
+      <c r="N31" s="175"/>
+      <c r="O31" s="175"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="37">
@@ -48868,7 +48805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="U87" sqref="U87"/>
     </sheetView>
   </sheetViews>
@@ -50801,7 +50738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed tick marks from chart-styles chart
</commit_message>
<xml_diff>
--- a/chart-styles.xlsx
+++ b/chart-styles.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhou/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhou/Documents/graphics-styleguide/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="33700" windowHeight="23860" tabRatio="913" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="33700" windowHeight="23860" tabRatio="913" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="17" r:id="rId1"/>
@@ -997,7 +997,7 @@
     <t>Capital gains</t>
   </si>
   <si>
-    <t>*REMOVE TICK MARKS FROM X-AXIS FOR CONTINUOUS DATA (except for histogram)</t>
+    <t>*TICK MARKS ON X-AXIS ARE NOT USED FOR CATEGORICAL DATA</t>
   </si>
 </sst>
 </file>
@@ -1886,16 +1886,19 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="3" fontId="57" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="58" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1907,34 +1910,7 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1949,7 +1925,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1971,12 +1977,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="57" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="58" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -2151,11 +2151,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-2095986496"/>
-        <c:axId val="-2067621440"/>
+        <c:axId val="541210528"/>
+        <c:axId val="541294016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095986496"/>
+        <c:axId val="541210528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2172,7 +2172,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2067621440"/>
+        <c:crossAx val="541294016"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2180,7 +2180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2067621440"/>
+        <c:axId val="541294016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2207,7 +2207,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2095986496"/>
+        <c:crossAx val="541210528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -4303,11 +4303,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132574064"/>
-        <c:axId val="-2074051584"/>
+        <c:axId val="507467104"/>
+        <c:axId val="507460832"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2132574064"/>
+        <c:axId val="507467104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4317,7 +4317,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074051584"/>
+        <c:crossAx val="507460832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4326,7 +4326,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074051584"/>
+        <c:axId val="507460832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4337,7 +4337,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132574064"/>
+        <c:crossAx val="507467104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4962,18 +4962,18 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="-2067460000"/>
-        <c:axId val="-2067028688"/>
+        <c:axId val="470143712"/>
+        <c:axId val="470129328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2067460000"/>
+        <c:axId val="470143712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -4994,7 +4994,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2067028688"/>
+        <c:crossAx val="470129328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5002,7 +5002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2067028688"/>
+        <c:axId val="470129328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5039,7 +5039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2067460000"/>
+        <c:crossAx val="470143712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5676,11 +5676,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2132327280"/>
-        <c:axId val="-2074014272"/>
+        <c:axId val="513861296"/>
+        <c:axId val="514326304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2132327280"/>
+        <c:axId val="513861296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5690,7 +5690,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2074014272"/>
+        <c:crossAx val="514326304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5698,7 +5698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074014272"/>
+        <c:axId val="514326304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5724,7 +5724,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2132327280"/>
+        <c:crossAx val="513861296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7042,11 +7042,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2073667632"/>
-        <c:axId val="-2112112016"/>
+        <c:axId val="504283504"/>
+        <c:axId val="504261648"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2073667632"/>
+        <c:axId val="504283504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7056,7 +7056,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112112016"/>
+        <c:crossAx val="504261648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7064,7 +7064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112112016"/>
+        <c:axId val="504261648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7098,7 +7098,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2073667632"/>
+        <c:crossAx val="504283504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7219,9 +7219,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7410,9 +7408,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7518,11 +7514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2078328208"/>
-        <c:axId val="-2078327168"/>
+        <c:axId val="469843328"/>
+        <c:axId val="504146784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2078328208"/>
+        <c:axId val="469843328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7550,7 +7546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078327168"/>
+        <c:crossAx val="504146784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7558,7 +7554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2078327168"/>
+        <c:axId val="504146784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.3E7"/>
@@ -7597,7 +7593,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078328208"/>
+        <c:crossAx val="469843328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7971,11 +7967,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2079120592"/>
-        <c:axId val="-2073838784"/>
+        <c:axId val="433497568"/>
+        <c:axId val="392499216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2079120592"/>
+        <c:axId val="433497568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7985,7 +7981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073838784"/>
+        <c:crossAx val="392499216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7993,7 +7989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2073838784"/>
+        <c:axId val="392499216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8019,7 +8015,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2079120592"/>
+        <c:crossAx val="433497568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8126,14 +8122,11 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -8142,9 +8135,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8163,9 +8154,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8343,9 +8332,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8364,9 +8351,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8385,7 +8370,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -8435,11 +8419,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2076253072"/>
-        <c:axId val="-2076264384"/>
+        <c:axId val="514082944"/>
+        <c:axId val="514080496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2076253072"/>
+        <c:axId val="514082944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8449,7 +8433,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076264384"/>
+        <c:crossAx val="514080496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8457,7 +8441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076264384"/>
+        <c:axId val="514080496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8467,7 +8451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076253072"/>
+        <c:crossAx val="514082944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8589,9 +8573,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8609,9 +8591,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8629,9 +8609,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8649,9 +8627,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8669,9 +8645,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8689,9 +8663,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8932,20 +8904,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2076556000"/>
-        <c:axId val="-2076602480"/>
+        <c:axId val="507287600"/>
+        <c:axId val="507268912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2076556000"/>
+        <c:axId val="507287600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076602480"/>
+        <c:crossAx val="507268912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8953,7 +8926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076602480"/>
+        <c:axId val="507268912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8979,7 +8952,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2076556000"/>
+        <c:crossAx val="507287600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9078,7 +9051,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -9146,11 +9118,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-2065337840"/>
-        <c:axId val="-2064868208"/>
+        <c:axId val="433201712"/>
+        <c:axId val="433182048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2065337840"/>
+        <c:axId val="433201712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9167,7 +9139,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2064868208"/>
+        <c:crossAx val="433182048"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9175,7 +9147,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2064868208"/>
+        <c:axId val="433182048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -9187,7 +9159,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2065337840"/>
+        <c:crossAx val="433201712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -9418,11 +9390,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-2112653376"/>
-        <c:axId val="-2112729328"/>
+        <c:axId val="541826352"/>
+        <c:axId val="514795600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112653376"/>
+        <c:axId val="541826352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9439,7 +9411,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2112729328"/>
+        <c:crossAx val="514795600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9447,7 +9419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112729328"/>
+        <c:axId val="514795600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-20.0"/>
@@ -9474,7 +9446,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2112653376"/>
+        <c:crossAx val="541826352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -9773,16 +9745,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2112155952"/>
-        <c:axId val="-2112316240"/>
+        <c:axId val="514766800"/>
+        <c:axId val="514745328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112155952"/>
+        <c:axId val="514766800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -9796,7 +9769,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2112316240"/>
+        <c:crossAx val="514745328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9804,7 +9777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112316240"/>
+        <c:axId val="514745328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9830,7 +9803,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2112155952"/>
+        <c:crossAx val="514766800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9977,7 +9950,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="17"/>
-              <c:layout/>
               <c:spPr/>
               <c:txPr>
                 <a:bodyPr/>
@@ -9996,14 +9968,11 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
-              <c:layout/>
               <c:spPr/>
               <c:txPr>
                 <a:bodyPr/>
@@ -10022,9 +9991,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -10277,11 +10244,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="30"/>
-        <c:axId val="-2095649632"/>
-        <c:axId val="-2067317888"/>
+        <c:axId val="470612816"/>
+        <c:axId val="470585600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095649632"/>
+        <c:axId val="470612816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10309,7 +10276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2067317888"/>
+        <c:crossAx val="470585600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10319,7 +10286,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2067317888"/>
+        <c:axId val="470585600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -10356,7 +10323,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095649632"/>
+        <c:crossAx val="470612816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -10510,7 +10477,7 @@
                   <c:v>5.0718</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.154199999999991</c:v>
+                  <c:v>6.15419999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7.2366</c:v>
@@ -11442,11 +11409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2065439760"/>
-        <c:axId val="-2065044000"/>
+        <c:axId val="426367232"/>
+        <c:axId val="426353344"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2065439760"/>
+        <c:axId val="426367232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11474,7 +11441,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065044000"/>
+        <c:crossAx val="426353344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11484,7 +11451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2065044000"/>
+        <c:axId val="426353344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11564,7 +11531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065439760"/>
+        <c:crossAx val="426367232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
@@ -12613,11 +12580,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2065630384"/>
-        <c:axId val="-2065354864"/>
+        <c:axId val="429032304"/>
+        <c:axId val="429031216"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2065630384"/>
+        <c:axId val="429032304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12645,7 +12612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065354864"/>
+        <c:crossAx val="429031216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12655,7 +12622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2065354864"/>
+        <c:axId val="429031216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12691,7 +12658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065630384"/>
+        <c:crossAx val="429032304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -13660,8 +13627,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2065077552"/>
-        <c:axId val="-2064742512"/>
+        <c:axId val="507302672"/>
+        <c:axId val="507234288"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13934,17 +13901,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2065077552"/>
-        <c:axId val="-2064742512"/>
+        <c:axId val="507302672"/>
+        <c:axId val="507234288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2065077552"/>
+        <c:axId val="507302672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -13966,7 +13933,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064742512"/>
+        <c:crossAx val="507234288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13976,7 +13943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2064742512"/>
+        <c:axId val="507234288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14014,7 +13981,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065077552"/>
+        <c:crossAx val="507302672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -14990,8 +14957,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112484784"/>
-        <c:axId val="-2112055440"/>
+        <c:axId val="506604816"/>
+        <c:axId val="506869232"/>
       </c:areaChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -15063,11 +15030,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2112484784"/>
-        <c:axId val="-2112055440"/>
+        <c:axId val="506604816"/>
+        <c:axId val="506869232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112484784"/>
+        <c:axId val="506604816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15077,7 +15044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112055440"/>
+        <c:crossAx val="506869232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15087,7 +15054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112055440"/>
+        <c:axId val="506869232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -15114,7 +15081,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2112484784"/>
+        <c:crossAx val="506604816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17191,14 +17158,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17261,14 +17228,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17331,14 +17298,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17455,14 +17422,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17528,14 +17495,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17609,7 +17576,7 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:noFill/>
             </a14:hiddenFill>
           </a:ext>
@@ -29626,8 +29593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX272"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="11" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -31671,9 +31638,9 @@
       <c r="F24" s="46"/>
       <c r="G24" s="46"/>
       <c r="H24" s="46"/>
-      <c r="I24" s="178"/>
+      <c r="I24" s="148"/>
       <c r="J24" s="46"/>
-      <c r="K24" s="179" t="s">
+      <c r="K24" s="149" t="s">
         <v>293</v>
       </c>
       <c r="L24" s="46"/>
@@ -41058,7 +41025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+    <sheetView topLeftCell="B6" workbookViewId="0">
       <selection activeCell="V68" sqref="V68"/>
     </sheetView>
   </sheetViews>
@@ -41259,20 +41226,20 @@
     </row>
     <row r="4" spans="1:11" s="60" customFormat="1" ht="14" x14ac:dyDescent="0.15"/>
     <row r="5" spans="1:11" s="60" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="178" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="176"/>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="176"/>
+      <c r="B5" s="178"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
     </row>
     <row r="6" spans="1:11" s="60" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="177"/>
-      <c r="B6" s="177"/>
-      <c r="C6" s="177"/>
-      <c r="D6" s="177"/>
-      <c r="E6" s="177"/>
+      <c r="A6" s="179"/>
+      <c r="B6" s="179"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -41809,27 +41776,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" s="14" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="169" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
-      <c r="L1" s="155"/>
-      <c r="M1" s="155"/>
-      <c r="N1" s="155"/>
-      <c r="O1" s="155"/>
-      <c r="P1" s="155"/>
-      <c r="Q1" s="155"/>
-      <c r="R1" s="155"/>
-      <c r="S1" s="155"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
+      <c r="K1" s="169"/>
+      <c r="L1" s="169"/>
+      <c r="M1" s="169"/>
+      <c r="N1" s="169"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
+      <c r="Q1" s="169"/>
+      <c r="R1" s="169"/>
+      <c r="S1" s="169"/>
       <c r="U1" s="126"/>
       <c r="V1" s="147" t="s">
         <v>42</v>
@@ -41853,48 +41820,48 @@
       <c r="AM1" s="127"/>
       <c r="AN1" s="127"/>
       <c r="AO1" s="126"/>
-      <c r="AP1" s="148"/>
-      <c r="AQ1" s="148"/>
-      <c r="AR1" s="148"/>
-      <c r="AS1" s="148"/>
-      <c r="AT1" s="148"/>
-      <c r="AU1" s="148"/>
-      <c r="AV1" s="148"/>
-      <c r="AW1" s="148"/>
-      <c r="AX1" s="148"/>
-      <c r="AY1" s="148"/>
-      <c r="AZ1" s="148"/>
-      <c r="BA1" s="148"/>
-      <c r="BB1" s="148"/>
-      <c r="BC1" s="148"/>
-      <c r="BD1" s="148"/>
-      <c r="BE1" s="148"/>
-      <c r="BF1" s="148"/>
-      <c r="BG1" s="148"/>
-      <c r="BH1" s="148"/>
+      <c r="AP1" s="166"/>
+      <c r="AQ1" s="166"/>
+      <c r="AR1" s="166"/>
+      <c r="AS1" s="166"/>
+      <c r="AT1" s="166"/>
+      <c r="AU1" s="166"/>
+      <c r="AV1" s="166"/>
+      <c r="AW1" s="166"/>
+      <c r="AX1" s="166"/>
+      <c r="AY1" s="166"/>
+      <c r="AZ1" s="166"/>
+      <c r="BA1" s="166"/>
+      <c r="BB1" s="166"/>
+      <c r="BC1" s="166"/>
+      <c r="BD1" s="166"/>
+      <c r="BE1" s="166"/>
+      <c r="BF1" s="166"/>
+      <c r="BG1" s="166"/>
+      <c r="BH1" s="166"/>
     </row>
     <row r="2" spans="1:60" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="169" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
-      <c r="L2" s="155"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="155"/>
-      <c r="O2" s="155"/>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="155"/>
-      <c r="S2" s="155"/>
+      <c r="B2" s="169"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
       <c r="U2" s="128"/>
       <c r="V2" s="129"/>
       <c r="W2" s="129"/>
@@ -41956,41 +41923,41 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
-      <c r="U3" s="149"/>
-      <c r="V3" s="149"/>
-      <c r="W3" s="149" t="s">
+      <c r="U3" s="164"/>
+      <c r="V3" s="164"/>
+      <c r="W3" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="149"/>
+      <c r="X3" s="164"/>
       <c r="Y3" s="130"/>
-      <c r="Z3" s="149" t="s">
+      <c r="Z3" s="164" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="149"/>
+      <c r="AA3" s="164"/>
       <c r="AB3" s="131"/>
-      <c r="AC3" s="149" t="s">
+      <c r="AC3" s="164" t="s">
         <v>45</v>
       </c>
-      <c r="AD3" s="149"/>
+      <c r="AD3" s="164"/>
       <c r="AE3" s="130"/>
-      <c r="AF3" s="149" t="s">
+      <c r="AF3" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="AG3" s="161"/>
-      <c r="AH3" s="161"/>
-      <c r="AI3" s="161"/>
-      <c r="AJ3" s="161"/>
+      <c r="AG3" s="171"/>
+      <c r="AH3" s="171"/>
+      <c r="AI3" s="171"/>
+      <c r="AJ3" s="171"/>
       <c r="AK3" s="132"/>
-      <c r="AL3" s="149" t="s">
+      <c r="AL3" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="AM3" s="150"/>
-      <c r="AN3" s="150"/>
-      <c r="AO3" s="150"/>
-      <c r="AP3" s="149"/>
-      <c r="AQ3" s="150"/>
-      <c r="AR3" s="150"/>
-      <c r="AS3" s="150"/>
+      <c r="AM3" s="167"/>
+      <c r="AN3" s="167"/>
+      <c r="AO3" s="167"/>
+      <c r="AP3" s="164"/>
+      <c r="AQ3" s="167"/>
+      <c r="AR3" s="167"/>
+      <c r="AS3" s="167"/>
       <c r="AT3" s="128"/>
       <c r="AU3" s="128"/>
       <c r="AV3" s="128"/>
@@ -42026,42 +41993,42 @@
       <c r="J4" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="159"/>
-      <c r="L4" s="159"/>
-      <c r="M4" s="159"/>
-      <c r="N4" s="159"/>
+      <c r="K4" s="170"/>
+      <c r="L4" s="170"/>
+      <c r="M4" s="170"/>
+      <c r="N4" s="170"/>
       <c r="O4" s="19"/>
       <c r="P4" s="156" t="s">
         <v>47</v>
       </c>
-      <c r="Q4" s="165"/>
-      <c r="R4" s="165"/>
-      <c r="S4" s="165"/>
-      <c r="U4" s="152"/>
-      <c r="V4" s="152"/>
-      <c r="W4" s="152"/>
-      <c r="X4" s="152"/>
+      <c r="Q4" s="157"/>
+      <c r="R4" s="157"/>
+      <c r="S4" s="157"/>
+      <c r="U4" s="153"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
       <c r="Y4" s="133"/>
-      <c r="Z4" s="152"/>
-      <c r="AA4" s="152"/>
+      <c r="Z4" s="153"/>
+      <c r="AA4" s="153"/>
       <c r="AB4" s="134"/>
-      <c r="AC4" s="152"/>
-      <c r="AD4" s="152"/>
+      <c r="AC4" s="153"/>
+      <c r="AD4" s="153"/>
       <c r="AE4" s="133"/>
-      <c r="AF4" s="162"/>
-      <c r="AG4" s="162"/>
-      <c r="AH4" s="162"/>
-      <c r="AI4" s="162"/>
-      <c r="AJ4" s="162"/>
+      <c r="AF4" s="152"/>
+      <c r="AG4" s="152"/>
+      <c r="AH4" s="152"/>
+      <c r="AI4" s="152"/>
+      <c r="AJ4" s="152"/>
       <c r="AK4" s="135"/>
-      <c r="AL4" s="151"/>
-      <c r="AM4" s="151"/>
-      <c r="AN4" s="151"/>
-      <c r="AO4" s="151"/>
-      <c r="AP4" s="151"/>
-      <c r="AQ4" s="151"/>
-      <c r="AR4" s="151"/>
-      <c r="AS4" s="151"/>
+      <c r="AL4" s="168"/>
+      <c r="AM4" s="168"/>
+      <c r="AN4" s="168"/>
+      <c r="AO4" s="168"/>
+      <c r="AP4" s="168"/>
+      <c r="AQ4" s="168"/>
+      <c r="AR4" s="168"/>
+      <c r="AS4" s="168"/>
       <c r="AT4" s="128"/>
       <c r="AU4" s="128"/>
       <c r="AV4" s="128"/>
@@ -42079,58 +42046,58 @@
       <c r="BH4" s="128"/>
     </row>
     <row r="5" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="157"/>
-      <c r="B5" s="157"/>
+      <c r="A5" s="162"/>
+      <c r="B5" s="162"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
       <c r="F5" s="21"/>
-      <c r="G5" s="157"/>
-      <c r="H5" s="157"/>
+      <c r="G5" s="162"/>
+      <c r="H5" s="162"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="160"/>
-      <c r="L5" s="160"/>
-      <c r="M5" s="160"/>
-      <c r="N5" s="160"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="161"/>
+      <c r="M5" s="161"/>
+      <c r="N5" s="161"/>
       <c r="O5" s="22"/>
-      <c r="P5" s="166"/>
-      <c r="Q5" s="166"/>
-      <c r="R5" s="166"/>
-      <c r="S5" s="166"/>
-      <c r="U5" s="152"/>
-      <c r="V5" s="152"/>
-      <c r="W5" s="152"/>
-      <c r="X5" s="152"/>
+      <c r="P5" s="158"/>
+      <c r="Q5" s="158"/>
+      <c r="R5" s="158"/>
+      <c r="S5" s="158"/>
+      <c r="U5" s="153"/>
+      <c r="V5" s="153"/>
+      <c r="W5" s="153"/>
+      <c r="X5" s="153"/>
       <c r="Y5" s="133"/>
-      <c r="Z5" s="152"/>
-      <c r="AA5" s="152"/>
+      <c r="Z5" s="153"/>
+      <c r="AA5" s="153"/>
       <c r="AB5" s="134"/>
-      <c r="AC5" s="152"/>
-      <c r="AD5" s="152"/>
+      <c r="AC5" s="153"/>
+      <c r="AD5" s="153"/>
       <c r="AE5" s="133"/>
-      <c r="AF5" s="163" t="s">
+      <c r="AF5" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="AG5" s="164"/>
+      <c r="AG5" s="151"/>
       <c r="AH5" s="136"/>
-      <c r="AI5" s="163" t="s">
+      <c r="AI5" s="150" t="s">
         <v>49</v>
       </c>
-      <c r="AJ5" s="164"/>
+      <c r="AJ5" s="151"/>
       <c r="AK5" s="136"/>
-      <c r="AL5" s="152" t="s">
+      <c r="AL5" s="153" t="s">
         <v>50</v>
       </c>
-      <c r="AM5" s="152"/>
+      <c r="AM5" s="153"/>
       <c r="AN5" s="136"/>
-      <c r="AO5" s="152" t="s">
+      <c r="AO5" s="153" t="s">
         <v>51</v>
       </c>
-      <c r="AP5" s="152"/>
-      <c r="AQ5" s="152"/>
+      <c r="AP5" s="153"/>
+      <c r="AQ5" s="153"/>
       <c r="AR5" s="136"/>
-      <c r="AS5" s="152"/>
+      <c r="AS5" s="153"/>
       <c r="AT5" s="128"/>
       <c r="AU5" s="128"/>
       <c r="AV5" s="128"/>
@@ -42148,58 +42115,58 @@
       <c r="BH5" s="128"/>
     </row>
     <row r="6" spans="1:60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="157"/>
-      <c r="B6" s="157"/>
+      <c r="A6" s="162"/>
+      <c r="B6" s="162"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="157"/>
-      <c r="E6" s="157"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
+      <c r="G6" s="162"/>
+      <c r="H6" s="162"/>
       <c r="I6" s="20"/>
-      <c r="J6" s="167" t="s">
+      <c r="J6" s="159" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="168"/>
+      <c r="K6" s="160"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="167" t="s">
+      <c r="M6" s="159" t="s">
         <v>49</v>
       </c>
-      <c r="N6" s="168"/>
+      <c r="N6" s="160"/>
       <c r="O6" s="23"/>
-      <c r="P6" s="157" t="s">
+      <c r="P6" s="162" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="157"/>
+      <c r="Q6" s="162"/>
       <c r="R6" s="23"/>
-      <c r="S6" s="157" t="s">
+      <c r="S6" s="162" t="s">
         <v>51</v>
       </c>
-      <c r="U6" s="153"/>
-      <c r="V6" s="153"/>
-      <c r="W6" s="153"/>
-      <c r="X6" s="153"/>
+      <c r="U6" s="154"/>
+      <c r="V6" s="154"/>
+      <c r="W6" s="154"/>
+      <c r="X6" s="154"/>
       <c r="Y6" s="133"/>
-      <c r="Z6" s="153"/>
-      <c r="AA6" s="153"/>
+      <c r="Z6" s="154"/>
+      <c r="AA6" s="154"/>
       <c r="AB6" s="134"/>
-      <c r="AC6" s="153"/>
-      <c r="AD6" s="153"/>
+      <c r="AC6" s="154"/>
+      <c r="AD6" s="154"/>
       <c r="AE6" s="133"/>
-      <c r="AF6" s="162"/>
-      <c r="AG6" s="162"/>
+      <c r="AF6" s="152"/>
+      <c r="AG6" s="152"/>
       <c r="AH6" s="137"/>
-      <c r="AI6" s="162"/>
-      <c r="AJ6" s="162"/>
+      <c r="AI6" s="152"/>
+      <c r="AJ6" s="152"/>
       <c r="AK6" s="136"/>
-      <c r="AL6" s="153"/>
-      <c r="AM6" s="153"/>
+      <c r="AL6" s="154"/>
+      <c r="AM6" s="154"/>
       <c r="AN6" s="137"/>
-      <c r="AO6" s="154"/>
-      <c r="AP6" s="153"/>
-      <c r="AQ6" s="153"/>
+      <c r="AO6" s="155"/>
+      <c r="AP6" s="154"/>
+      <c r="AQ6" s="154"/>
       <c r="AR6" s="137"/>
-      <c r="AS6" s="154"/>
+      <c r="AS6" s="155"/>
       <c r="AT6" s="128"/>
       <c r="AU6" s="128"/>
       <c r="AV6" s="128"/>
@@ -42217,25 +42184,25 @@
       <c r="BH6" s="128"/>
     </row>
     <row r="7" spans="1:60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="158"/>
-      <c r="B7" s="158"/>
+      <c r="A7" s="163"/>
+      <c r="B7" s="163"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
+      <c r="G7" s="163"/>
+      <c r="H7" s="163"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="160"/>
-      <c r="K7" s="160"/>
+      <c r="J7" s="161"/>
+      <c r="K7" s="161"/>
       <c r="L7" s="24"/>
-      <c r="M7" s="160"/>
-      <c r="N7" s="160"/>
+      <c r="M7" s="161"/>
+      <c r="N7" s="161"/>
       <c r="O7" s="23"/>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="158"/>
+      <c r="P7" s="163"/>
+      <c r="Q7" s="163"/>
       <c r="R7" s="24"/>
-      <c r="S7" s="169"/>
+      <c r="S7" s="165"/>
       <c r="U7" s="128"/>
       <c r="V7" s="128"/>
       <c r="W7" s="128"/>
@@ -45279,15 +45246,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="AI5:AJ6"/>
-    <mergeCell ref="AL5:AM6"/>
-    <mergeCell ref="AO5:AO6"/>
-    <mergeCell ref="P4:S5"/>
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="M6:N7"/>
-    <mergeCell ref="P6:Q7"/>
-    <mergeCell ref="U3:V6"/>
-    <mergeCell ref="S6:S7"/>
     <mergeCell ref="AP1:BH1"/>
     <mergeCell ref="AP3:AS4"/>
     <mergeCell ref="AP5:AQ6"/>
@@ -45304,6 +45262,15 @@
     <mergeCell ref="AF3:AJ4"/>
     <mergeCell ref="AL3:AO4"/>
     <mergeCell ref="AF5:AG6"/>
+    <mergeCell ref="AI5:AJ6"/>
+    <mergeCell ref="AL5:AM6"/>
+    <mergeCell ref="AO5:AO6"/>
+    <mergeCell ref="P4:S5"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="M6:N7"/>
+    <mergeCell ref="P6:Q7"/>
+    <mergeCell ref="U3:V6"/>
+    <mergeCell ref="S6:S7"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <conditionalFormatting sqref="AA8:AA20">
@@ -46392,35 +46359,35 @@
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="170" t="s">
+      <c r="B40" s="172" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="171"/>
-      <c r="D40" s="171"/>
-      <c r="E40" s="171"/>
-      <c r="F40" s="171"/>
-      <c r="G40" s="171"/>
-      <c r="H40" s="171"/>
-      <c r="I40" s="171"/>
-      <c r="J40" s="171"/>
-      <c r="K40" s="171"/>
+      <c r="C40" s="173"/>
+      <c r="D40" s="173"/>
+      <c r="E40" s="173"/>
+      <c r="F40" s="173"/>
+      <c r="G40" s="173"/>
+      <c r="H40" s="173"/>
+      <c r="I40" s="173"/>
+      <c r="J40" s="173"/>
+      <c r="K40" s="173"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="172" t="s">
+      <c r="B41" s="174" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="172"/>
-      <c r="D41" s="172"/>
-      <c r="E41" s="172"/>
-      <c r="F41" s="172"/>
-      <c r="G41" s="172"/>
-      <c r="H41" s="172"/>
-      <c r="I41" s="172"/>
-      <c r="J41" s="172"/>
-      <c r="K41" s="172"/>
+      <c r="C41" s="174"/>
+      <c r="D41" s="174"/>
+      <c r="E41" s="174"/>
+      <c r="F41" s="174"/>
+      <c r="G41" s="174"/>
+      <c r="H41" s="174"/>
+      <c r="I41" s="174"/>
+      <c r="J41" s="174"/>
+      <c r="K41" s="174"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42" s="9"/>
@@ -47070,24 +47037,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="175" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="173"/>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
+      <c r="A2" s="175"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="36" t="s">
@@ -47558,15 +47525,15 @@
         <v>18.600000000000001</v>
       </c>
       <c r="G29" s="40"/>
-      <c r="I29" s="174" t="s">
+      <c r="I29" s="176" t="s">
         <v>85</v>
       </c>
-      <c r="J29" s="175"/>
-      <c r="K29" s="175"/>
-      <c r="L29" s="175"/>
-      <c r="M29" s="175"/>
-      <c r="N29" s="175"/>
-      <c r="O29" s="175"/>
+      <c r="J29" s="177"/>
+      <c r="K29" s="177"/>
+      <c r="L29" s="177"/>
+      <c r="M29" s="177"/>
+      <c r="N29" s="177"/>
+      <c r="O29" s="177"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="37">
@@ -47590,13 +47557,13 @@
       <c r="G30" s="41">
         <v>1980</v>
       </c>
-      <c r="I30" s="175"/>
-      <c r="J30" s="175"/>
-      <c r="K30" s="175"/>
-      <c r="L30" s="175"/>
-      <c r="M30" s="175"/>
-      <c r="N30" s="175"/>
-      <c r="O30" s="175"/>
+      <c r="I30" s="177"/>
+      <c r="J30" s="177"/>
+      <c r="K30" s="177"/>
+      <c r="L30" s="177"/>
+      <c r="M30" s="177"/>
+      <c r="N30" s="177"/>
+      <c r="O30" s="177"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="37">
@@ -47618,13 +47585,13 @@
         <v>19.3</v>
       </c>
       <c r="G31" s="40"/>
-      <c r="I31" s="175"/>
-      <c r="J31" s="175"/>
-      <c r="K31" s="175"/>
-      <c r="L31" s="175"/>
-      <c r="M31" s="175"/>
-      <c r="N31" s="175"/>
-      <c r="O31" s="175"/>
+      <c r="I31" s="177"/>
+      <c r="J31" s="177"/>
+      <c r="K31" s="177"/>
+      <c r="L31" s="177"/>
+      <c r="M31" s="177"/>
+      <c r="N31" s="177"/>
+      <c r="O31" s="177"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="37">

</xml_diff>

<commit_message>
added more changes to graphs in excel file
</commit_message>
<xml_diff>
--- a/chart-styles.xlsx
+++ b/chart-styles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="1940" windowWidth="29860" windowHeight="23860" tabRatio="913" firstSheet="5" activeTab="14"/>
+    <workbookView xWindow="2020" yWindow="1940" windowWidth="29860" windowHeight="23860" tabRatio="913" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="17" r:id="rId1"/>
@@ -1903,13 +1903,16 @@
     </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1921,7 +1924,34 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1936,37 +1966,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -2042,16 +2042,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FF0A4B69"/>
+      <color rgb="FFDC2B26"/>
+      <color rgb="FF1796D3"/>
       <color rgb="FF0095D4"/>
+      <color rgb="FF696969"/>
       <color rgb="FFA1D4EE"/>
       <color rgb="FF6FBFE4"/>
       <color rgb="FF024B6B"/>
       <color rgb="FF000000"/>
       <color rgb="FF322C2E"/>
-      <color rgb="FFD3D3D3"/>
-      <color rgb="FFEF2B8C"/>
-      <color rgb="FFFFC100"/>
-      <color rgb="FF1882C8"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2171,11 +2171,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1594592720"/>
-        <c:axId val="1268965840"/>
+        <c:axId val="1358358048"/>
+        <c:axId val="1659982512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1594592720"/>
+        <c:axId val="1358358048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,7 +2192,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1268965840"/>
+        <c:crossAx val="1659982512"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2200,7 +2200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1268965840"/>
+        <c:axId val="1659982512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2227,7 +2227,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1594592720"/>
+        <c:crossAx val="1358358048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -4323,11 +4323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1647038288"/>
-        <c:axId val="1651311920"/>
+        <c:axId val="1670535904"/>
+        <c:axId val="1613348352"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1647038288"/>
+        <c:axId val="1670535904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4337,7 +4337,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1651311920"/>
+        <c:crossAx val="1613348352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4346,7 +4346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1651311920"/>
+        <c:axId val="1613348352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4357,7 +4357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1647038288"/>
+        <c:crossAx val="1670535904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4982,11 +4982,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="1648865264"/>
-        <c:axId val="1692299456"/>
+        <c:axId val="1670824608"/>
+        <c:axId val="1363754272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1648865264"/>
+        <c:axId val="1670824608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5014,7 +5014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1692299456"/>
+        <c:crossAx val="1363754272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5022,7 +5022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1692299456"/>
+        <c:axId val="1363754272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5059,7 +5059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1648865264"/>
+        <c:crossAx val="1670824608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5696,11 +5696,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1646593824"/>
-        <c:axId val="1720723776"/>
+        <c:axId val="1364364432"/>
+        <c:axId val="1364368416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1646593824"/>
+        <c:axId val="1364364432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5710,7 +5710,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1720723776"/>
+        <c:crossAx val="1364368416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5718,7 +5718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1720723776"/>
+        <c:axId val="1364368416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5744,7 +5744,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1646593824"/>
+        <c:crossAx val="1364364432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7062,11 +7062,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1720950560"/>
-        <c:axId val="1721214176"/>
+        <c:axId val="1611348032"/>
+        <c:axId val="1358623312"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1720950560"/>
+        <c:axId val="1611348032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7076,7 +7076,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1721214176"/>
+        <c:crossAx val="1358623312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7084,7 +7084,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1721214176"/>
+        <c:axId val="1358623312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7118,7 +7118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1720950560"/>
+        <c:crossAx val="1611348032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7534,11 +7534,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1720738752"/>
-        <c:axId val="1651472800"/>
+        <c:axId val="1357947136"/>
+        <c:axId val="1358141072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1720738752"/>
+        <c:axId val="1357947136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7566,7 +7566,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1651472800"/>
+        <c:crossAx val="1358141072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7574,7 +7574,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1651472800"/>
+        <c:axId val="1358141072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.3E7"/>
@@ -7613,7 +7613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1720738752"/>
+        <c:crossAx val="1357947136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7987,11 +7987,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1596913536"/>
-        <c:axId val="1704250928"/>
+        <c:axId val="1358463120"/>
+        <c:axId val="1361701152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1596913536"/>
+        <c:axId val="1358463120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8001,7 +8001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1704250928"/>
+        <c:crossAx val="1361701152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8009,7 +8009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1704250928"/>
+        <c:axId val="1361701152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8035,7 +8035,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1596913536"/>
+        <c:crossAx val="1358463120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8160,8 +8160,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0281721430390821"/>
-                  <c:y val="-0.0679486703313029"/>
+                  <c:x val="0.0190205307988589"/>
+                  <c:y val="-0.0477359126124826"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -8190,12 +8190,14 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.146441631504923"/>
-                      <c:h val="0.102358490566038"/>
+                      <c:w val="0.128138423611843"/>
+                      <c:h val="0.142783824718666"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -8205,8 +8207,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.00284887648537598"/>
-                  <c:y val="0.0346725969395335"/>
+                  <c:x val="0.00988858073049609"/>
+                  <c:y val="0.0608301282393356"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -8235,6 +8237,8 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
@@ -8250,10 +8254,29 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0307540671340133"/>
-                  <c:y val="-0.0174485589065518"/>
+                  <c:x val="-0.0328659850228148"/>
+                  <c:y val="0.0158428166105787"/>
                 </c:manualLayout>
               </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="1"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -8261,12 +8284,14 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.153220815752461"/>
-                      <c:h val="0.075"/>
+                      <c:w val="0.112390528292277"/>
+                      <c:h val="0.127315115180228"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -8297,6 +8322,8 @@
             <c:showSerName val="0"/>
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
+            <c:separator>
+</c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
@@ -8492,11 +8519,31 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0141074365975641"/>
-                  <c:y val="0.000447428317437308"/>
+                  <c:x val="0.00565981907602813"/>
+                  <c:y val="0.00756655230730797"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00140794277056309"/>
+                  <c:y val="0.00711904291661765"/>
+                </c:manualLayout>
+              </c:layout>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -8544,7 +8591,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1"/>
+                  <a:defRPr sz="1100" b="0"/>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -8608,11 +8655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1694184272"/>
-        <c:axId val="1673969776"/>
+        <c:axId val="1359639056"/>
+        <c:axId val="1693591664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1694184272"/>
+        <c:axId val="1359639056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8622,7 +8669,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1673969776"/>
+        <c:crossAx val="1693591664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8630,7 +8677,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1673969776"/>
+        <c:axId val="1693591664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8640,7 +8687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1694184272"/>
+        <c:crossAx val="1359639056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9175,11 +9222,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1612017072"/>
-        <c:axId val="1594955152"/>
+        <c:axId val="1694317760"/>
+        <c:axId val="1324289968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1612017072"/>
+        <c:axId val="1694317760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9203,7 +9250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1594955152"/>
+        <c:crossAx val="1324289968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9211,7 +9258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1594955152"/>
+        <c:axId val="1324289968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9237,7 +9284,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1612017072"/>
+        <c:crossAx val="1694317760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9403,11 +9450,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1763196480"/>
-        <c:axId val="1691607488"/>
+        <c:axId val="1613408976"/>
+        <c:axId val="1617353472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1763196480"/>
+        <c:axId val="1613408976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9424,7 +9471,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1691607488"/>
+        <c:crossAx val="1617353472"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9432,7 +9479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1691607488"/>
+        <c:axId val="1617353472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -9444,7 +9491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1763196480"/>
+        <c:crossAx val="1613408976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -9725,11 +9772,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1709877344"/>
-        <c:axId val="1677590560"/>
+        <c:axId val="1323860672"/>
+        <c:axId val="1764026640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1709877344"/>
+        <c:axId val="1323860672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9746,7 +9793,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1677590560"/>
+        <c:crossAx val="1764026640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9754,7 +9801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1677590560"/>
+        <c:axId val="1764026640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-20.0"/>
@@ -9781,7 +9828,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1709877344"/>
+        <c:crossAx val="1323860672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -9939,7 +9986,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFC100"/>
+              <a:srgbClr val="DC2B26"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -10080,11 +10127,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1704241856"/>
-        <c:axId val="1688720720"/>
+        <c:axId val="1723777040"/>
+        <c:axId val="1359676128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1704241856"/>
+        <c:axId val="1723777040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10104,7 +10151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1688720720"/>
+        <c:crossAx val="1359676128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10112,7 +10159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1688720720"/>
+        <c:axId val="1359676128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10138,7 +10185,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1704241856"/>
+        <c:crossAx val="1723777040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10252,7 +10299,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="0A4B69"/>
               </a:solidFill>
               <a:ln w="25400">
                 <a:noFill/>
@@ -10285,6 +10332,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="17"/>
+              <c:layout/>
               <c:spPr/>
               <c:txPr>
                 <a:bodyPr/>
@@ -10303,11 +10351,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:spPr/>
               <c:txPr>
                 <a:bodyPr/>
@@ -10326,7 +10377,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -10591,11 +10644,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="30"/>
-        <c:axId val="1647688432"/>
-        <c:axId val="1721131184"/>
+        <c:axId val="1270714336"/>
+        <c:axId val="1270780720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1647688432"/>
+        <c:axId val="1270714336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10623,7 +10676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1721131184"/>
+        <c:crossAx val="1270780720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10633,7 +10686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1721131184"/>
+        <c:axId val="1270780720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -10670,7 +10723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1647688432"/>
+        <c:crossAx val="1270714336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -10824,7 +10877,7 @@
                   <c:v>5.0718</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.154199999999986</c:v>
+                  <c:v>6.154199999999985</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7.2366</c:v>
@@ -11756,11 +11809,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1677650800"/>
-        <c:axId val="1594540880"/>
+        <c:axId val="1727971024"/>
+        <c:axId val="1704356128"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1677650800"/>
+        <c:axId val="1727971024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11788,7 +11841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1594540880"/>
+        <c:crossAx val="1704356128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11798,7 +11851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1594540880"/>
+        <c:axId val="1704356128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11878,7 +11931,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1677650800"/>
+        <c:crossAx val="1727971024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
@@ -12927,11 +12980,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1659153120"/>
-        <c:axId val="1597434560"/>
+        <c:axId val="1694283232"/>
+        <c:axId val="1323388992"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1659153120"/>
+        <c:axId val="1694283232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12959,7 +13012,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1597434560"/>
+        <c:crossAx val="1323388992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12969,7 +13022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1597434560"/>
+        <c:axId val="1323388992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13005,7 +13058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1659153120"/>
+        <c:crossAx val="1694283232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -13102,7 +13155,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx2"/>
+              <a:srgbClr val="1796D3"/>
             </a:solidFill>
             <a:ln w="25400">
               <a:noFill/>
@@ -13974,8 +14027,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1704154592"/>
-        <c:axId val="1652746592"/>
+        <c:axId val="1670663680"/>
+        <c:axId val="1671006688"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14248,11 +14301,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1704154592"/>
-        <c:axId val="1652746592"/>
+        <c:axId val="1670663680"/>
+        <c:axId val="1671006688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1704154592"/>
+        <c:axId val="1670663680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14280,7 +14333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1652746592"/>
+        <c:crossAx val="1671006688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14290,7 +14343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1652746592"/>
+        <c:axId val="1671006688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14328,7 +14381,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1704154592"/>
+        <c:crossAx val="1670663680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -15304,8 +15357,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1764703120"/>
-        <c:axId val="1763992864"/>
+        <c:axId val="1670554336"/>
+        <c:axId val="1671337616"/>
       </c:areaChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -15377,11 +15430,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1764703120"/>
-        <c:axId val="1763992864"/>
+        <c:axId val="1670554336"/>
+        <c:axId val="1671337616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1764703120"/>
+        <c:axId val="1670554336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15391,7 +15444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1763992864"/>
+        <c:crossAx val="1671337616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15401,7 +15454,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1763992864"/>
+        <c:axId val="1671337616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -15428,7 +15481,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1764703120"/>
+        <c:crossAx val="1670554336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16018,7 +16071,7 @@
         </cdr:nvSpPr>
         <cdr:spPr>
           <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:off x="7486650" y="6850202"/>
+            <a:off x="7355320" y="6833693"/>
             <a:ext cx="1483360" cy="236398"/>
           </a:xfrm>
           <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
@@ -17502,14 +17555,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17572,14 +17625,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17642,14 +17695,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17766,14 +17819,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17794,16 +17847,13 @@
           <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" b="1" i="1" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
+                <a:srgbClr val="696969"/>
               </a:solidFill>
               <a:latin typeface="Lato" charset="0"/>
               <a:ea typeface="Lato" charset="0"/>
               <a:cs typeface="Lato" charset="0"/>
             </a:rPr>
-            <a:t>Actual</a:t>
+            <a:t>ACTUAL</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -17839,14 +17889,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17867,16 +17917,13 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="1" i="1" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
+                <a:srgbClr val="696969"/>
               </a:solidFill>
               <a:latin typeface="Lato" charset="0"/>
               <a:ea typeface="Lato" charset="0"/>
               <a:cs typeface="Lato" charset="0"/>
             </a:rPr>
-            <a:t>Projected</a:t>
+            <a:t>PROJECTED</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -17918,7 +17965,7 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:noFill/>
             </a14:hiddenFill>
           </a:ext>
@@ -25795,12 +25842,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.83526</cdr:x>
-      <cdr:y>0.95335</cdr:y>
+      <cdr:x>0.82184</cdr:x>
+      <cdr:y>0.92518</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>1</cdr:x>
-      <cdr:y>1</cdr:y>
+      <cdr:x>0.98658</cdr:x>
+      <cdr:y>0.97183</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -25809,8 +25856,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="7537450" y="7066102"/>
-          <a:ext cx="1483360" cy="236398"/>
+          <a:off x="7409240" y="4965111"/>
+          <a:ext cx="1485195" cy="250355"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -41809,8 +41856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView topLeftCell="A4" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41907,8 +41954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="A13" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42429,27 +42476,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" s="14" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
-      <c r="P1" s="170"/>
-      <c r="Q1" s="170"/>
-      <c r="R1" s="170"/>
-      <c r="S1" s="170"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
+      <c r="K1" s="158"/>
+      <c r="L1" s="158"/>
+      <c r="M1" s="158"/>
+      <c r="N1" s="158"/>
+      <c r="O1" s="158"/>
+      <c r="P1" s="158"/>
+      <c r="Q1" s="158"/>
+      <c r="R1" s="158"/>
+      <c r="S1" s="158"/>
       <c r="U1" s="125"/>
       <c r="V1" s="146" t="s">
         <v>42</v>
@@ -42473,48 +42520,48 @@
       <c r="AM1" s="126"/>
       <c r="AN1" s="126"/>
       <c r="AO1" s="125"/>
-      <c r="AP1" s="167"/>
-      <c r="AQ1" s="167"/>
-      <c r="AR1" s="167"/>
-      <c r="AS1" s="167"/>
-      <c r="AT1" s="167"/>
-      <c r="AU1" s="167"/>
-      <c r="AV1" s="167"/>
-      <c r="AW1" s="167"/>
-      <c r="AX1" s="167"/>
-      <c r="AY1" s="167"/>
-      <c r="AZ1" s="167"/>
-      <c r="BA1" s="167"/>
-      <c r="BB1" s="167"/>
-      <c r="BC1" s="167"/>
-      <c r="BD1" s="167"/>
-      <c r="BE1" s="167"/>
-      <c r="BF1" s="167"/>
-      <c r="BG1" s="167"/>
-      <c r="BH1" s="167"/>
+      <c r="AP1" s="151"/>
+      <c r="AQ1" s="151"/>
+      <c r="AR1" s="151"/>
+      <c r="AS1" s="151"/>
+      <c r="AT1" s="151"/>
+      <c r="AU1" s="151"/>
+      <c r="AV1" s="151"/>
+      <c r="AW1" s="151"/>
+      <c r="AX1" s="151"/>
+      <c r="AY1" s="151"/>
+      <c r="AZ1" s="151"/>
+      <c r="BA1" s="151"/>
+      <c r="BB1" s="151"/>
+      <c r="BC1" s="151"/>
+      <c r="BD1" s="151"/>
+      <c r="BE1" s="151"/>
+      <c r="BF1" s="151"/>
+      <c r="BG1" s="151"/>
+      <c r="BH1" s="151"/>
     </row>
     <row r="2" spans="1:60" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="158" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
-      <c r="P2" s="170"/>
-      <c r="Q2" s="170"/>
-      <c r="R2" s="170"/>
-      <c r="S2" s="170"/>
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="158"/>
+      <c r="M2" s="158"/>
+      <c r="N2" s="158"/>
+      <c r="O2" s="158"/>
+      <c r="P2" s="158"/>
+      <c r="Q2" s="158"/>
+      <c r="R2" s="158"/>
+      <c r="S2" s="158"/>
       <c r="U2" s="127"/>
       <c r="V2" s="128"/>
       <c r="W2" s="128"/>
@@ -42576,41 +42623,41 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
-      <c r="U3" s="165"/>
-      <c r="V3" s="165"/>
-      <c r="W3" s="165" t="s">
+      <c r="U3" s="152"/>
+      <c r="V3" s="152"/>
+      <c r="W3" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="165"/>
+      <c r="X3" s="152"/>
       <c r="Y3" s="129"/>
-      <c r="Z3" s="165" t="s">
+      <c r="Z3" s="152" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="165"/>
+      <c r="AA3" s="152"/>
       <c r="AB3" s="130"/>
-      <c r="AC3" s="165" t="s">
+      <c r="AC3" s="152" t="s">
         <v>45</v>
       </c>
-      <c r="AD3" s="165"/>
+      <c r="AD3" s="152"/>
       <c r="AE3" s="129"/>
-      <c r="AF3" s="165" t="s">
+      <c r="AF3" s="152" t="s">
         <v>46</v>
       </c>
-      <c r="AG3" s="172"/>
-      <c r="AH3" s="172"/>
-      <c r="AI3" s="172"/>
-      <c r="AJ3" s="172"/>
+      <c r="AG3" s="164"/>
+      <c r="AH3" s="164"/>
+      <c r="AI3" s="164"/>
+      <c r="AJ3" s="164"/>
       <c r="AK3" s="131"/>
-      <c r="AL3" s="165" t="s">
+      <c r="AL3" s="152" t="s">
         <v>47</v>
       </c>
-      <c r="AM3" s="168"/>
-      <c r="AN3" s="168"/>
-      <c r="AO3" s="168"/>
-      <c r="AP3" s="165"/>
-      <c r="AQ3" s="168"/>
-      <c r="AR3" s="168"/>
-      <c r="AS3" s="168"/>
+      <c r="AM3" s="153"/>
+      <c r="AN3" s="153"/>
+      <c r="AO3" s="153"/>
+      <c r="AP3" s="152"/>
+      <c r="AQ3" s="153"/>
+      <c r="AR3" s="153"/>
+      <c r="AS3" s="153"/>
       <c r="AT3" s="127"/>
       <c r="AU3" s="127"/>
       <c r="AV3" s="127"/>
@@ -42628,60 +42675,60 @@
       <c r="BH3" s="127"/>
     </row>
     <row r="4" spans="1:60" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="157" t="s">
+      <c r="A4" s="159" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="157"/>
+      <c r="B4" s="159"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="157" t="s">
+      <c r="D4" s="159" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="157"/>
+      <c r="E4" s="159"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="157" t="s">
+      <c r="G4" s="159" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="157"/>
+      <c r="H4" s="159"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="157" t="s">
+      <c r="J4" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="171"/>
-      <c r="L4" s="171"/>
-      <c r="M4" s="171"/>
-      <c r="N4" s="171"/>
+      <c r="K4" s="162"/>
+      <c r="L4" s="162"/>
+      <c r="M4" s="162"/>
+      <c r="N4" s="162"/>
       <c r="O4" s="19"/>
-      <c r="P4" s="157" t="s">
+      <c r="P4" s="159" t="s">
         <v>47</v>
       </c>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="158"/>
-      <c r="S4" s="158"/>
-      <c r="U4" s="154"/>
-      <c r="V4" s="154"/>
-      <c r="W4" s="154"/>
-      <c r="X4" s="154"/>
+      <c r="Q4" s="168"/>
+      <c r="R4" s="168"/>
+      <c r="S4" s="168"/>
+      <c r="U4" s="155"/>
+      <c r="V4" s="155"/>
+      <c r="W4" s="155"/>
+      <c r="X4" s="155"/>
       <c r="Y4" s="132"/>
-      <c r="Z4" s="154"/>
-      <c r="AA4" s="154"/>
+      <c r="Z4" s="155"/>
+      <c r="AA4" s="155"/>
       <c r="AB4" s="133"/>
-      <c r="AC4" s="154"/>
-      <c r="AD4" s="154"/>
+      <c r="AC4" s="155"/>
+      <c r="AD4" s="155"/>
       <c r="AE4" s="132"/>
-      <c r="AF4" s="153"/>
-      <c r="AG4" s="153"/>
-      <c r="AH4" s="153"/>
-      <c r="AI4" s="153"/>
-      <c r="AJ4" s="153"/>
+      <c r="AF4" s="165"/>
+      <c r="AG4" s="165"/>
+      <c r="AH4" s="165"/>
+      <c r="AI4" s="165"/>
+      <c r="AJ4" s="165"/>
       <c r="AK4" s="134"/>
-      <c r="AL4" s="169"/>
-      <c r="AM4" s="169"/>
-      <c r="AN4" s="169"/>
-      <c r="AO4" s="169"/>
-      <c r="AP4" s="169"/>
-      <c r="AQ4" s="169"/>
-      <c r="AR4" s="169"/>
-      <c r="AS4" s="169"/>
+      <c r="AL4" s="154"/>
+      <c r="AM4" s="154"/>
+      <c r="AN4" s="154"/>
+      <c r="AO4" s="154"/>
+      <c r="AP4" s="154"/>
+      <c r="AQ4" s="154"/>
+      <c r="AR4" s="154"/>
+      <c r="AS4" s="154"/>
       <c r="AT4" s="127"/>
       <c r="AU4" s="127"/>
       <c r="AV4" s="127"/>
@@ -42699,58 +42746,58 @@
       <c r="BH4" s="127"/>
     </row>
     <row r="5" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="163"/>
-      <c r="B5" s="163"/>
+      <c r="A5" s="160"/>
+      <c r="B5" s="160"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
       <c r="F5" s="21"/>
-      <c r="G5" s="163"/>
-      <c r="H5" s="163"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="160"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="162"/>
-      <c r="K5" s="162"/>
-      <c r="L5" s="162"/>
-      <c r="M5" s="162"/>
-      <c r="N5" s="162"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="163"/>
       <c r="O5" s="22"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="159"/>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="U5" s="154"/>
-      <c r="V5" s="154"/>
-      <c r="W5" s="154"/>
-      <c r="X5" s="154"/>
+      <c r="P5" s="169"/>
+      <c r="Q5" s="169"/>
+      <c r="R5" s="169"/>
+      <c r="S5" s="169"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="155"/>
+      <c r="W5" s="155"/>
+      <c r="X5" s="155"/>
       <c r="Y5" s="132"/>
-      <c r="Z5" s="154"/>
-      <c r="AA5" s="154"/>
+      <c r="Z5" s="155"/>
+      <c r="AA5" s="155"/>
       <c r="AB5" s="133"/>
-      <c r="AC5" s="154"/>
-      <c r="AD5" s="154"/>
+      <c r="AC5" s="155"/>
+      <c r="AD5" s="155"/>
       <c r="AE5" s="132"/>
-      <c r="AF5" s="151" t="s">
+      <c r="AF5" s="166" t="s">
         <v>48</v>
       </c>
-      <c r="AG5" s="152"/>
+      <c r="AG5" s="167"/>
       <c r="AH5" s="135"/>
-      <c r="AI5" s="151" t="s">
+      <c r="AI5" s="166" t="s">
         <v>49</v>
       </c>
-      <c r="AJ5" s="152"/>
+      <c r="AJ5" s="167"/>
       <c r="AK5" s="135"/>
-      <c r="AL5" s="154" t="s">
+      <c r="AL5" s="155" t="s">
         <v>50</v>
       </c>
-      <c r="AM5" s="154"/>
+      <c r="AM5" s="155"/>
       <c r="AN5" s="135"/>
-      <c r="AO5" s="154" t="s">
+      <c r="AO5" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="AP5" s="154"/>
-      <c r="AQ5" s="154"/>
+      <c r="AP5" s="155"/>
+      <c r="AQ5" s="155"/>
       <c r="AR5" s="135"/>
-      <c r="AS5" s="154"/>
+      <c r="AS5" s="155"/>
       <c r="AT5" s="127"/>
       <c r="AU5" s="127"/>
       <c r="AV5" s="127"/>
@@ -42768,58 +42815,58 @@
       <c r="BH5" s="127"/>
     </row>
     <row r="6" spans="1:60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="163"/>
-      <c r="B6" s="163"/>
+      <c r="A6" s="160"/>
+      <c r="B6" s="160"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="160"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
+      <c r="G6" s="160"/>
+      <c r="H6" s="160"/>
       <c r="I6" s="20"/>
-      <c r="J6" s="160" t="s">
+      <c r="J6" s="170" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="161"/>
+      <c r="K6" s="171"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="160" t="s">
+      <c r="M6" s="170" t="s">
         <v>49</v>
       </c>
-      <c r="N6" s="161"/>
+      <c r="N6" s="171"/>
       <c r="O6" s="23"/>
-      <c r="P6" s="163" t="s">
+      <c r="P6" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="163"/>
+      <c r="Q6" s="160"/>
       <c r="R6" s="23"/>
-      <c r="S6" s="163" t="s">
+      <c r="S6" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="U6" s="155"/>
-      <c r="V6" s="155"/>
-      <c r="W6" s="155"/>
-      <c r="X6" s="155"/>
+      <c r="U6" s="156"/>
+      <c r="V6" s="156"/>
+      <c r="W6" s="156"/>
+      <c r="X6" s="156"/>
       <c r="Y6" s="132"/>
-      <c r="Z6" s="155"/>
-      <c r="AA6" s="155"/>
+      <c r="Z6" s="156"/>
+      <c r="AA6" s="156"/>
       <c r="AB6" s="133"/>
-      <c r="AC6" s="155"/>
-      <c r="AD6" s="155"/>
+      <c r="AC6" s="156"/>
+      <c r="AD6" s="156"/>
       <c r="AE6" s="132"/>
-      <c r="AF6" s="153"/>
-      <c r="AG6" s="153"/>
+      <c r="AF6" s="165"/>
+      <c r="AG6" s="165"/>
       <c r="AH6" s="136"/>
-      <c r="AI6" s="153"/>
-      <c r="AJ6" s="153"/>
+      <c r="AI6" s="165"/>
+      <c r="AJ6" s="165"/>
       <c r="AK6" s="135"/>
-      <c r="AL6" s="155"/>
-      <c r="AM6" s="155"/>
+      <c r="AL6" s="156"/>
+      <c r="AM6" s="156"/>
       <c r="AN6" s="136"/>
-      <c r="AO6" s="156"/>
-      <c r="AP6" s="155"/>
-      <c r="AQ6" s="155"/>
+      <c r="AO6" s="157"/>
+      <c r="AP6" s="156"/>
+      <c r="AQ6" s="156"/>
       <c r="AR6" s="136"/>
-      <c r="AS6" s="156"/>
+      <c r="AS6" s="157"/>
       <c r="AT6" s="127"/>
       <c r="AU6" s="127"/>
       <c r="AV6" s="127"/>
@@ -42837,25 +42884,25 @@
       <c r="BH6" s="127"/>
     </row>
     <row r="7" spans="1:60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="164"/>
-      <c r="B7" s="164"/>
+      <c r="A7" s="161"/>
+      <c r="B7" s="161"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="164"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="164"/>
-      <c r="H7" s="164"/>
+      <c r="G7" s="161"/>
+      <c r="H7" s="161"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="162"/>
-      <c r="K7" s="162"/>
+      <c r="J7" s="163"/>
+      <c r="K7" s="163"/>
       <c r="L7" s="24"/>
-      <c r="M7" s="162"/>
-      <c r="N7" s="162"/>
+      <c r="M7" s="163"/>
+      <c r="N7" s="163"/>
       <c r="O7" s="23"/>
-      <c r="P7" s="164"/>
-      <c r="Q7" s="164"/>
+      <c r="P7" s="161"/>
+      <c r="Q7" s="161"/>
       <c r="R7" s="24"/>
-      <c r="S7" s="166"/>
+      <c r="S7" s="172"/>
       <c r="U7" s="127"/>
       <c r="V7" s="127"/>
       <c r="W7" s="127"/>
@@ -45899,6 +45946,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="AI5:AJ6"/>
+    <mergeCell ref="AL5:AM6"/>
+    <mergeCell ref="AO5:AO6"/>
+    <mergeCell ref="P4:S5"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="M6:N7"/>
+    <mergeCell ref="P6:Q7"/>
+    <mergeCell ref="U3:V6"/>
+    <mergeCell ref="S6:S7"/>
     <mergeCell ref="AP1:BH1"/>
     <mergeCell ref="AP3:AS4"/>
     <mergeCell ref="AP5:AQ6"/>
@@ -45915,15 +45971,6 @@
     <mergeCell ref="AF3:AJ4"/>
     <mergeCell ref="AL3:AO4"/>
     <mergeCell ref="AF5:AG6"/>
-    <mergeCell ref="AI5:AJ6"/>
-    <mergeCell ref="AL5:AM6"/>
-    <mergeCell ref="AO5:AO6"/>
-    <mergeCell ref="P4:S5"/>
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="M6:N7"/>
-    <mergeCell ref="P6:Q7"/>
-    <mergeCell ref="U3:V6"/>
-    <mergeCell ref="S6:S7"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <conditionalFormatting sqref="AA8:AA20">
@@ -46093,7 +46140,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46213,8 +46260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
-      <selection activeCell="Y50" sqref="Y50"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
+      <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -47676,7 +47723,7 @@
   <dimension ref="A1:O144"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="156" zoomScaleNormal="156" zoomScalePageLayoutView="156" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
added text and graph changes based on web and print rules
</commit_message>
<xml_diff>
--- a/chart-styles.xlsx
+++ b/chart-styles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="1940" windowWidth="29860" windowHeight="23860" tabRatio="913" activeTab="4"/>
+    <workbookView xWindow="8400" yWindow="1700" windowWidth="29860" windowHeight="23860" tabRatio="913"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="17" r:id="rId1"/>
@@ -1903,16 +1903,13 @@
     </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1924,34 +1921,7 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1966,7 +1936,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -2042,16 +2042,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FFA3D5EC"/>
+      <color rgb="FFD3D3D3"/>
+      <color rgb="FF1796D3"/>
       <color rgb="FF0A4B69"/>
       <color rgb="FFDC2B26"/>
-      <color rgb="FF1796D3"/>
       <color rgb="FF0095D4"/>
       <color rgb="FF696969"/>
       <color rgb="FFA1D4EE"/>
       <color rgb="FF6FBFE4"/>
       <color rgb="FF024B6B"/>
-      <color rgb="FF000000"/>
-      <color rgb="FF322C2E"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2171,11 +2171,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1358358048"/>
-        <c:axId val="1659982512"/>
+        <c:axId val="1323944192"/>
+        <c:axId val="1323957504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1358358048"/>
+        <c:axId val="1323944192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,7 +2192,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1659982512"/>
+        <c:crossAx val="1323957504"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2200,7 +2200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1659982512"/>
+        <c:axId val="1323957504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2227,7 +2227,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1358358048"/>
+        <c:crossAx val="1323944192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -4323,11 +4323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1670535904"/>
-        <c:axId val="1613348352"/>
+        <c:axId val="1676036544"/>
+        <c:axId val="1675771936"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1670535904"/>
+        <c:axId val="1676036544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4337,7 +4337,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1613348352"/>
+        <c:crossAx val="1675771936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4346,7 +4346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1613348352"/>
+        <c:axId val="1675771936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4357,7 +4357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1670535904"/>
+        <c:crossAx val="1676036544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4982,11 +4982,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="1670824608"/>
-        <c:axId val="1363754272"/>
+        <c:axId val="1675574880"/>
+        <c:axId val="1675220912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1670824608"/>
+        <c:axId val="1675574880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5014,7 +5014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1363754272"/>
+        <c:crossAx val="1675220912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5022,7 +5022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1363754272"/>
+        <c:axId val="1675220912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5059,7 +5059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1670824608"/>
+        <c:crossAx val="1675574880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5696,11 +5696,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1364364432"/>
-        <c:axId val="1364368416"/>
+        <c:axId val="1689657904"/>
+        <c:axId val="1689865664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1364364432"/>
+        <c:axId val="1689657904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5710,7 +5710,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1364368416"/>
+        <c:crossAx val="1689865664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5718,7 +5718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1364368416"/>
+        <c:axId val="1689865664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5744,7 +5744,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1364364432"/>
+        <c:crossAx val="1689657904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7062,11 +7062,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1611348032"/>
-        <c:axId val="1358623312"/>
+        <c:axId val="1675383280"/>
+        <c:axId val="1674702272"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1611348032"/>
+        <c:axId val="1675383280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7076,7 +7076,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1358623312"/>
+        <c:crossAx val="1674702272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7084,7 +7084,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1358623312"/>
+        <c:axId val="1674702272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7118,7 +7118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1611348032"/>
+        <c:crossAx val="1675383280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7239,7 +7239,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7428,7 +7430,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7534,11 +7538,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1357947136"/>
-        <c:axId val="1358141072"/>
+        <c:axId val="1323579424"/>
+        <c:axId val="1323583792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1357947136"/>
+        <c:axId val="1323579424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7566,7 +7570,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1358141072"/>
+        <c:crossAx val="1323583792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7574,7 +7578,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1358141072"/>
+        <c:axId val="1323583792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.3E7"/>
@@ -7613,7 +7617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1357947136"/>
+        <c:crossAx val="1323579424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7987,11 +7991,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1358463120"/>
-        <c:axId val="1361701152"/>
+        <c:axId val="1323338688"/>
+        <c:axId val="1323342608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1358463120"/>
+        <c:axId val="1323338688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8001,7 +8005,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1361701152"/>
+        <c:crossAx val="1323342608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8009,7 +8013,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1361701152"/>
+        <c:axId val="1323342608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8035,7 +8039,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1358463120"/>
+        <c:crossAx val="1323338688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8605,7 +8609,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -8656,7 +8659,7 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:axId val="1359639056"/>
-        <c:axId val="1693591664"/>
+        <c:axId val="1359627696"/>
       </c:barChart>
       <c:catAx>
         <c:axId val="1359639056"/>
@@ -8669,7 +8672,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1693591664"/>
+        <c:crossAx val="1359627696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8677,7 +8680,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1693591664"/>
+        <c:axId val="1359627696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9222,11 +9225,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1694317760"/>
-        <c:axId val="1324289968"/>
+        <c:axId val="1708948416"/>
+        <c:axId val="1708648048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1694317760"/>
+        <c:axId val="1708948416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9250,7 +9253,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1324289968"/>
+        <c:crossAx val="1708648048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9258,7 +9261,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1324289968"/>
+        <c:axId val="1708648048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9284,7 +9287,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1694317760"/>
+        <c:crossAx val="1708948416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9383,6 +9386,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -9450,11 +9454,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1613408976"/>
-        <c:axId val="1617353472"/>
+        <c:axId val="1323889472"/>
+        <c:axId val="1323883456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1613408976"/>
+        <c:axId val="1323889472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9471,7 +9475,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1617353472"/>
+        <c:crossAx val="1323883456"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9479,7 +9483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1617353472"/>
+        <c:axId val="1323883456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -9491,7 +9495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1613408976"/>
+        <c:crossAx val="1323889472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -9565,7 +9569,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="tx2"/>
+              <a:srgbClr val="1796D3"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -9575,7 +9579,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0095D4"/>
+                <a:srgbClr val="1796D3"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9585,7 +9589,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0095D4"/>
+                <a:srgbClr val="1796D3"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9595,7 +9599,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0095D4"/>
+                <a:srgbClr val="1796D3"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9605,7 +9609,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0095D4"/>
+                <a:srgbClr val="1796D3"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9615,7 +9619,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0095D4"/>
+                <a:srgbClr val="1796D3"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9625,7 +9629,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC100"/>
+                <a:srgbClr val="D3D3D3"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9635,7 +9639,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="A3D5EC"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9645,7 +9649,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="A3D5EC"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9655,7 +9659,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="A3D5EC"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9665,7 +9669,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="A3D5EC"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9675,7 +9679,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="A3D5EC"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -9772,11 +9776,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="1323860672"/>
-        <c:axId val="1764026640"/>
+        <c:axId val="1351199504"/>
+        <c:axId val="1351179936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1323860672"/>
+        <c:axId val="1351199504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9793,7 +9797,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1764026640"/>
+        <c:crossAx val="1351179936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9801,7 +9805,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1764026640"/>
+        <c:axId val="1351179936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-20.0"/>
@@ -9828,7 +9832,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1323860672"/>
+        <c:crossAx val="1351199504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -10127,11 +10131,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1723777040"/>
-        <c:axId val="1359676128"/>
+        <c:axId val="1350738208"/>
+        <c:axId val="1350742464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1723777040"/>
+        <c:axId val="1350738208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10151,7 +10155,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1359676128"/>
+        <c:crossAx val="1350742464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10159,7 +10163,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1359676128"/>
+        <c:axId val="1350742464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10185,7 +10189,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1723777040"/>
+        <c:crossAx val="1350738208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10644,11 +10648,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="30"/>
-        <c:axId val="1270714336"/>
-        <c:axId val="1270780720"/>
+        <c:axId val="1711082512"/>
+        <c:axId val="1711057408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1270714336"/>
+        <c:axId val="1711082512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10676,7 +10680,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1270780720"/>
+        <c:crossAx val="1711057408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10686,7 +10690,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1270780720"/>
+        <c:axId val="1711057408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -10723,7 +10727,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1270714336"/>
+        <c:crossAx val="1711082512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -10877,7 +10881,7 @@
                   <c:v>5.0718</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.154199999999985</c:v>
+                  <c:v>6.154199999999984</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7.2366</c:v>
@@ -11809,11 +11813,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1727971024"/>
-        <c:axId val="1704356128"/>
+        <c:axId val="1710267552"/>
+        <c:axId val="1710250528"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1727971024"/>
+        <c:axId val="1710267552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11841,7 +11845,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1704356128"/>
+        <c:crossAx val="1710250528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11851,7 +11855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1704356128"/>
+        <c:axId val="1710250528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11931,7 +11935,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1727971024"/>
+        <c:crossAx val="1710267552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
@@ -12980,11 +12984,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1694283232"/>
-        <c:axId val="1323388992"/>
+        <c:axId val="1676562896"/>
+        <c:axId val="1676366032"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="1694283232"/>
+        <c:axId val="1676562896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13012,7 +13016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1323388992"/>
+        <c:crossAx val="1676366032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13022,7 +13026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1323388992"/>
+        <c:axId val="1676366032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13058,7 +13062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1694283232"/>
+        <c:crossAx val="1676562896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -14027,8 +14031,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1670663680"/>
-        <c:axId val="1671006688"/>
+        <c:axId val="1689783696"/>
+        <c:axId val="1689705248"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14301,11 +14305,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1670663680"/>
-        <c:axId val="1671006688"/>
+        <c:axId val="1689783696"/>
+        <c:axId val="1689705248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1670663680"/>
+        <c:axId val="1689783696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14333,7 +14337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1671006688"/>
+        <c:crossAx val="1689705248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14343,7 +14347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1671006688"/>
+        <c:axId val="1689705248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14381,7 +14385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1670663680"/>
+        <c:crossAx val="1689783696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -15357,8 +15361,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1670554336"/>
-        <c:axId val="1671337616"/>
+        <c:axId val="1323723008"/>
+        <c:axId val="1323715296"/>
       </c:areaChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -15430,11 +15434,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1670554336"/>
-        <c:axId val="1671337616"/>
+        <c:axId val="1323723008"/>
+        <c:axId val="1323715296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1670554336"/>
+        <c:axId val="1323723008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15444,7 +15448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1671337616"/>
+        <c:crossAx val="1323715296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15454,7 +15458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1671337616"/>
+        <c:axId val="1323715296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -15481,7 +15485,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1670554336"/>
+        <c:crossAx val="1323723008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15816,7 +15820,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Title in 18pt Title Case</a:t>
+              <a:t>Title in 18px Title Case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -15832,7 +15836,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Subtitle in 14pt sentence case</a:t>
+              <a:t>Subtitle in 14px sentence case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -17050,7 +17054,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -17066,7 +17070,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -17555,14 +17559,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17625,14 +17629,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17695,14 +17699,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17819,14 +17823,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17889,14 +17893,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -17965,7 +17969,7 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:noFill/>
             </a14:hiddenFill>
           </a:ext>
@@ -18083,7 +18087,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -18099,7 +18103,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -19507,7 +19511,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -19523,7 +19527,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -20779,7 +20783,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -20795,7 +20799,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -21383,7 +21387,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -21399,7 +21403,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -21974,7 +21978,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -21990,7 +21994,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -22550,7 +22554,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -22566,7 +22570,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -23173,7 +23177,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Title in 18pt Title Case</a:t>
+              <a:t>Title in 18px Title Case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -23189,7 +23193,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Subtitle in 14pt sentence case</a:t>
+              <a:t>Subtitle in 14px sentence case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -23729,7 +23733,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -23745,7 +23749,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -24434,7 +24438,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -24450,7 +24454,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -25040,7 +25044,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case </a:t>
+            <a:t>Title in 18px Title Case </a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -25056,7 +25060,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -25581,7 +25585,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Title in 18pt Title Case</a:t>
+            <a:t>Title in 18px Title Case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -25597,7 +25601,7 @@
               <a:ea typeface="Avenir Medium"/>
               <a:cs typeface="Lato Regular"/>
             </a:rPr>
-            <a:t>Subtitle in 14pt sentence case</a:t>
+            <a:t>Subtitle in 14px sentence case</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -26071,7 +26075,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Title in 18pt Title Case</a:t>
+              <a:t>Title in 18px Title Case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -26087,7 +26091,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Subtitle in 14pt sentence case</a:t>
+              <a:t>Subtitle in 14px sentence case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -26495,13 +26499,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>186266</xdr:colOff>
+      <xdr:colOff>186265</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>414866</xdr:colOff>
+      <xdr:colOff>493380</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -26724,8 +26728,8 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="54888"/>
-          <a:ext cx="8954140" cy="4569377"/>
+          <a:off x="0" y="55105"/>
+          <a:ext cx="8993915" cy="4587377"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="8970010" cy="4229913"/>
         </a:xfrm>
@@ -26824,7 +26828,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Title in 18pt Title Case</a:t>
+              <a:t>Title in 18px Title Case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -26840,7 +26844,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Subtitle in 14pt sentence case</a:t>
+              <a:t>Subtitle in 14px sentence case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -27398,7 +27402,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Title in 18pt Title Case</a:t>
+              <a:t>Title in 18px Title Case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -27414,7 +27418,7 @@
                 <a:ea typeface="Avenir Medium"/>
                 <a:cs typeface="Lato Regular"/>
               </a:rPr>
-              <a:t>Subtitle in 14pt sentence case</a:t>
+              <a:t>Subtitle in 14px sentence case</a:t>
             </a:r>
           </a:p>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -29746,7 +29750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -30294,7 +30298,7 @@
   <dimension ref="A1:BX272"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScale="163" zoomScaleNormal="163" zoomScalePageLayoutView="163" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="11" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35593,7 +35597,7 @@
   <dimension ref="A1:BX276"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="11" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -41725,7 +41729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" zoomScale="163" zoomScaleNormal="163" zoomScalePageLayoutView="163" workbookViewId="0">
+    <sheetView topLeftCell="C7" zoomScale="163" zoomScaleNormal="163" zoomScalePageLayoutView="163" workbookViewId="0">
       <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
@@ -41856,7 +41860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
       <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
@@ -41954,7 +41958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
+    <sheetView zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
       <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
@@ -42067,7 +42071,7 @@
   <dimension ref="B3:D40"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AA65" sqref="AA65"/>
+      <selection activeCell="T56" sqref="T56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -42429,8 +42433,8 @@
   </sheetPr>
   <dimension ref="A1:BH95"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="S1" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="AF25" sqref="AF25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="AD42" sqref="AD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -42476,27 +42480,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" s="14" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
-      <c r="K1" s="158"/>
-      <c r="L1" s="158"/>
-      <c r="M1" s="158"/>
-      <c r="N1" s="158"/>
-      <c r="O1" s="158"/>
-      <c r="P1" s="158"/>
-      <c r="Q1" s="158"/>
-      <c r="R1" s="158"/>
-      <c r="S1" s="158"/>
+      <c r="B1" s="170"/>
+      <c r="C1" s="170"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="170"/>
+      <c r="I1" s="170"/>
+      <c r="J1" s="170"/>
+      <c r="K1" s="170"/>
+      <c r="L1" s="170"/>
+      <c r="M1" s="170"/>
+      <c r="N1" s="170"/>
+      <c r="O1" s="170"/>
+      <c r="P1" s="170"/>
+      <c r="Q1" s="170"/>
+      <c r="R1" s="170"/>
+      <c r="S1" s="170"/>
       <c r="U1" s="125"/>
       <c r="V1" s="146" t="s">
         <v>42</v>
@@ -42520,48 +42524,48 @@
       <c r="AM1" s="126"/>
       <c r="AN1" s="126"/>
       <c r="AO1" s="125"/>
-      <c r="AP1" s="151"/>
-      <c r="AQ1" s="151"/>
-      <c r="AR1" s="151"/>
-      <c r="AS1" s="151"/>
-      <c r="AT1" s="151"/>
-      <c r="AU1" s="151"/>
-      <c r="AV1" s="151"/>
-      <c r="AW1" s="151"/>
-      <c r="AX1" s="151"/>
-      <c r="AY1" s="151"/>
-      <c r="AZ1" s="151"/>
-      <c r="BA1" s="151"/>
-      <c r="BB1" s="151"/>
-      <c r="BC1" s="151"/>
-      <c r="BD1" s="151"/>
-      <c r="BE1" s="151"/>
-      <c r="BF1" s="151"/>
-      <c r="BG1" s="151"/>
-      <c r="BH1" s="151"/>
+      <c r="AP1" s="167"/>
+      <c r="AQ1" s="167"/>
+      <c r="AR1" s="167"/>
+      <c r="AS1" s="167"/>
+      <c r="AT1" s="167"/>
+      <c r="AU1" s="167"/>
+      <c r="AV1" s="167"/>
+      <c r="AW1" s="167"/>
+      <c r="AX1" s="167"/>
+      <c r="AY1" s="167"/>
+      <c r="AZ1" s="167"/>
+      <c r="BA1" s="167"/>
+      <c r="BB1" s="167"/>
+      <c r="BC1" s="167"/>
+      <c r="BD1" s="167"/>
+      <c r="BE1" s="167"/>
+      <c r="BF1" s="167"/>
+      <c r="BG1" s="167"/>
+      <c r="BH1" s="167"/>
     </row>
     <row r="2" spans="1:60" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="170" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-      <c r="G2" s="158"/>
-      <c r="H2" s="158"/>
-      <c r="I2" s="158"/>
-      <c r="J2" s="158"/>
-      <c r="K2" s="158"/>
-      <c r="L2" s="158"/>
-      <c r="M2" s="158"/>
-      <c r="N2" s="158"/>
-      <c r="O2" s="158"/>
-      <c r="P2" s="158"/>
-      <c r="Q2" s="158"/>
-      <c r="R2" s="158"/>
-      <c r="S2" s="158"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
+      <c r="L2" s="170"/>
+      <c r="M2" s="170"/>
+      <c r="N2" s="170"/>
+      <c r="O2" s="170"/>
+      <c r="P2" s="170"/>
+      <c r="Q2" s="170"/>
+      <c r="R2" s="170"/>
+      <c r="S2" s="170"/>
       <c r="U2" s="127"/>
       <c r="V2" s="128"/>
       <c r="W2" s="128"/>
@@ -42623,41 +42627,41 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
-      <c r="U3" s="152"/>
-      <c r="V3" s="152"/>
-      <c r="W3" s="152" t="s">
+      <c r="U3" s="165"/>
+      <c r="V3" s="165"/>
+      <c r="W3" s="165" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="152"/>
+      <c r="X3" s="165"/>
       <c r="Y3" s="129"/>
-      <c r="Z3" s="152" t="s">
+      <c r="Z3" s="165" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="152"/>
+      <c r="AA3" s="165"/>
       <c r="AB3" s="130"/>
-      <c r="AC3" s="152" t="s">
+      <c r="AC3" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="AD3" s="152"/>
+      <c r="AD3" s="165"/>
       <c r="AE3" s="129"/>
-      <c r="AF3" s="152" t="s">
+      <c r="AF3" s="165" t="s">
         <v>46</v>
       </c>
-      <c r="AG3" s="164"/>
-      <c r="AH3" s="164"/>
-      <c r="AI3" s="164"/>
-      <c r="AJ3" s="164"/>
+      <c r="AG3" s="172"/>
+      <c r="AH3" s="172"/>
+      <c r="AI3" s="172"/>
+      <c r="AJ3" s="172"/>
       <c r="AK3" s="131"/>
-      <c r="AL3" s="152" t="s">
+      <c r="AL3" s="165" t="s">
         <v>47</v>
       </c>
-      <c r="AM3" s="153"/>
-      <c r="AN3" s="153"/>
-      <c r="AO3" s="153"/>
-      <c r="AP3" s="152"/>
-      <c r="AQ3" s="153"/>
-      <c r="AR3" s="153"/>
-      <c r="AS3" s="153"/>
+      <c r="AM3" s="168"/>
+      <c r="AN3" s="168"/>
+      <c r="AO3" s="168"/>
+      <c r="AP3" s="165"/>
+      <c r="AQ3" s="168"/>
+      <c r="AR3" s="168"/>
+      <c r="AS3" s="168"/>
       <c r="AT3" s="127"/>
       <c r="AU3" s="127"/>
       <c r="AV3" s="127"/>
@@ -42675,60 +42679,60 @@
       <c r="BH3" s="127"/>
     </row>
     <row r="4" spans="1:60" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="159" t="s">
+      <c r="A4" s="157" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="159"/>
+      <c r="B4" s="157"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="159" t="s">
+      <c r="D4" s="157" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="159"/>
+      <c r="E4" s="157"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="159" t="s">
+      <c r="G4" s="157" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="159"/>
+      <c r="H4" s="157"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="159" t="s">
+      <c r="J4" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="162"/>
-      <c r="L4" s="162"/>
-      <c r="M4" s="162"/>
-      <c r="N4" s="162"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="171"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="171"/>
       <c r="O4" s="19"/>
-      <c r="P4" s="159" t="s">
+      <c r="P4" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="Q4" s="168"/>
-      <c r="R4" s="168"/>
-      <c r="S4" s="168"/>
-      <c r="U4" s="155"/>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
+      <c r="S4" s="158"/>
+      <c r="U4" s="154"/>
+      <c r="V4" s="154"/>
+      <c r="W4" s="154"/>
+      <c r="X4" s="154"/>
       <c r="Y4" s="132"/>
-      <c r="Z4" s="155"/>
-      <c r="AA4" s="155"/>
+      <c r="Z4" s="154"/>
+      <c r="AA4" s="154"/>
       <c r="AB4" s="133"/>
-      <c r="AC4" s="155"/>
-      <c r="AD4" s="155"/>
+      <c r="AC4" s="154"/>
+      <c r="AD4" s="154"/>
       <c r="AE4" s="132"/>
-      <c r="AF4" s="165"/>
-      <c r="AG4" s="165"/>
-      <c r="AH4" s="165"/>
-      <c r="AI4" s="165"/>
-      <c r="AJ4" s="165"/>
+      <c r="AF4" s="153"/>
+      <c r="AG4" s="153"/>
+      <c r="AH4" s="153"/>
+      <c r="AI4" s="153"/>
+      <c r="AJ4" s="153"/>
       <c r="AK4" s="134"/>
-      <c r="AL4" s="154"/>
-      <c r="AM4" s="154"/>
-      <c r="AN4" s="154"/>
-      <c r="AO4" s="154"/>
-      <c r="AP4" s="154"/>
-      <c r="AQ4" s="154"/>
-      <c r="AR4" s="154"/>
-      <c r="AS4" s="154"/>
+      <c r="AL4" s="169"/>
+      <c r="AM4" s="169"/>
+      <c r="AN4" s="169"/>
+      <c r="AO4" s="169"/>
+      <c r="AP4" s="169"/>
+      <c r="AQ4" s="169"/>
+      <c r="AR4" s="169"/>
+      <c r="AS4" s="169"/>
       <c r="AT4" s="127"/>
       <c r="AU4" s="127"/>
       <c r="AV4" s="127"/>
@@ -42746,58 +42750,58 @@
       <c r="BH4" s="127"/>
     </row>
     <row r="5" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="160"/>
-      <c r="B5" s="160"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="163"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
       <c r="F5" s="21"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="163"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="163"/>
-      <c r="K5" s="163"/>
-      <c r="L5" s="163"/>
-      <c r="M5" s="163"/>
-      <c r="N5" s="163"/>
+      <c r="J5" s="162"/>
+      <c r="K5" s="162"/>
+      <c r="L5" s="162"/>
+      <c r="M5" s="162"/>
+      <c r="N5" s="162"/>
       <c r="O5" s="22"/>
-      <c r="P5" s="169"/>
-      <c r="Q5" s="169"/>
-      <c r="R5" s="169"/>
-      <c r="S5" s="169"/>
-      <c r="U5" s="155"/>
-      <c r="V5" s="155"/>
-      <c r="W5" s="155"/>
-      <c r="X5" s="155"/>
+      <c r="P5" s="159"/>
+      <c r="Q5" s="159"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
+      <c r="U5" s="154"/>
+      <c r="V5" s="154"/>
+      <c r="W5" s="154"/>
+      <c r="X5" s="154"/>
       <c r="Y5" s="132"/>
-      <c r="Z5" s="155"/>
-      <c r="AA5" s="155"/>
+      <c r="Z5" s="154"/>
+      <c r="AA5" s="154"/>
       <c r="AB5" s="133"/>
-      <c r="AC5" s="155"/>
-      <c r="AD5" s="155"/>
+      <c r="AC5" s="154"/>
+      <c r="AD5" s="154"/>
       <c r="AE5" s="132"/>
-      <c r="AF5" s="166" t="s">
+      <c r="AF5" s="151" t="s">
         <v>48</v>
       </c>
-      <c r="AG5" s="167"/>
+      <c r="AG5" s="152"/>
       <c r="AH5" s="135"/>
-      <c r="AI5" s="166" t="s">
+      <c r="AI5" s="151" t="s">
         <v>49</v>
       </c>
-      <c r="AJ5" s="167"/>
+      <c r="AJ5" s="152"/>
       <c r="AK5" s="135"/>
-      <c r="AL5" s="155" t="s">
+      <c r="AL5" s="154" t="s">
         <v>50</v>
       </c>
-      <c r="AM5" s="155"/>
+      <c r="AM5" s="154"/>
       <c r="AN5" s="135"/>
-      <c r="AO5" s="155" t="s">
+      <c r="AO5" s="154" t="s">
         <v>51</v>
       </c>
-      <c r="AP5" s="155"/>
-      <c r="AQ5" s="155"/>
+      <c r="AP5" s="154"/>
+      <c r="AQ5" s="154"/>
       <c r="AR5" s="135"/>
-      <c r="AS5" s="155"/>
+      <c r="AS5" s="154"/>
       <c r="AT5" s="127"/>
       <c r="AU5" s="127"/>
       <c r="AV5" s="127"/>
@@ -42815,58 +42819,58 @@
       <c r="BH5" s="127"/>
     </row>
     <row r="6" spans="1:60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="160"/>
-      <c r="B6" s="160"/>
+      <c r="A6" s="163"/>
+      <c r="B6" s="163"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="160"/>
-      <c r="E6" s="160"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="160"/>
-      <c r="H6" s="160"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
       <c r="I6" s="20"/>
-      <c r="J6" s="170" t="s">
+      <c r="J6" s="160" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="171"/>
+      <c r="K6" s="161"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="170" t="s">
+      <c r="M6" s="160" t="s">
         <v>49</v>
       </c>
-      <c r="N6" s="171"/>
+      <c r="N6" s="161"/>
       <c r="O6" s="23"/>
-      <c r="P6" s="160" t="s">
+      <c r="P6" s="163" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="160"/>
+      <c r="Q6" s="163"/>
       <c r="R6" s="23"/>
-      <c r="S6" s="160" t="s">
+      <c r="S6" s="163" t="s">
         <v>51</v>
       </c>
-      <c r="U6" s="156"/>
-      <c r="V6" s="156"/>
-      <c r="W6" s="156"/>
-      <c r="X6" s="156"/>
+      <c r="U6" s="155"/>
+      <c r="V6" s="155"/>
+      <c r="W6" s="155"/>
+      <c r="X6" s="155"/>
       <c r="Y6" s="132"/>
-      <c r="Z6" s="156"/>
-      <c r="AA6" s="156"/>
+      <c r="Z6" s="155"/>
+      <c r="AA6" s="155"/>
       <c r="AB6" s="133"/>
-      <c r="AC6" s="156"/>
-      <c r="AD6" s="156"/>
+      <c r="AC6" s="155"/>
+      <c r="AD6" s="155"/>
       <c r="AE6" s="132"/>
-      <c r="AF6" s="165"/>
-      <c r="AG6" s="165"/>
+      <c r="AF6" s="153"/>
+      <c r="AG6" s="153"/>
       <c r="AH6" s="136"/>
-      <c r="AI6" s="165"/>
-      <c r="AJ6" s="165"/>
+      <c r="AI6" s="153"/>
+      <c r="AJ6" s="153"/>
       <c r="AK6" s="135"/>
-      <c r="AL6" s="156"/>
-      <c r="AM6" s="156"/>
+      <c r="AL6" s="155"/>
+      <c r="AM6" s="155"/>
       <c r="AN6" s="136"/>
-      <c r="AO6" s="157"/>
-      <c r="AP6" s="156"/>
-      <c r="AQ6" s="156"/>
+      <c r="AO6" s="156"/>
+      <c r="AP6" s="155"/>
+      <c r="AQ6" s="155"/>
       <c r="AR6" s="136"/>
-      <c r="AS6" s="157"/>
+      <c r="AS6" s="156"/>
       <c r="AT6" s="127"/>
       <c r="AU6" s="127"/>
       <c r="AV6" s="127"/>
@@ -42884,25 +42888,25 @@
       <c r="BH6" s="127"/>
     </row>
     <row r="7" spans="1:60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="161"/>
-      <c r="B7" s="161"/>
+      <c r="A7" s="164"/>
+      <c r="B7" s="164"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="164"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="161"/>
-      <c r="H7" s="161"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="164"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="163"/>
-      <c r="K7" s="163"/>
+      <c r="J7" s="162"/>
+      <c r="K7" s="162"/>
       <c r="L7" s="24"/>
-      <c r="M7" s="163"/>
-      <c r="N7" s="163"/>
+      <c r="M7" s="162"/>
+      <c r="N7" s="162"/>
       <c r="O7" s="23"/>
-      <c r="P7" s="161"/>
-      <c r="Q7" s="161"/>
+      <c r="P7" s="164"/>
+      <c r="Q7" s="164"/>
       <c r="R7" s="24"/>
-      <c r="S7" s="172"/>
+      <c r="S7" s="166"/>
       <c r="U7" s="127"/>
       <c r="V7" s="127"/>
       <c r="W7" s="127"/>
@@ -45946,15 +45950,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="AI5:AJ6"/>
-    <mergeCell ref="AL5:AM6"/>
-    <mergeCell ref="AO5:AO6"/>
-    <mergeCell ref="P4:S5"/>
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="M6:N7"/>
-    <mergeCell ref="P6:Q7"/>
-    <mergeCell ref="U3:V6"/>
-    <mergeCell ref="S6:S7"/>
     <mergeCell ref="AP1:BH1"/>
     <mergeCell ref="AP3:AS4"/>
     <mergeCell ref="AP5:AQ6"/>
@@ -45971,6 +45966,15 @@
     <mergeCell ref="AF3:AJ4"/>
     <mergeCell ref="AL3:AO4"/>
     <mergeCell ref="AF5:AG6"/>
+    <mergeCell ref="AI5:AJ6"/>
+    <mergeCell ref="AL5:AM6"/>
+    <mergeCell ref="AO5:AO6"/>
+    <mergeCell ref="P4:S5"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="M6:N7"/>
+    <mergeCell ref="P6:Q7"/>
+    <mergeCell ref="U3:V6"/>
+    <mergeCell ref="S6:S7"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <conditionalFormatting sqref="AA8:AA20">
@@ -46260,7 +46264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
       <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
revised language and graphs
</commit_message>
<xml_diff>
--- a/chart-styles.xlsx
+++ b/chart-styles.xlsx
@@ -932,9 +932,6 @@
     <t>Legend labels</t>
   </si>
   <si>
-    <t>The main point of the chart. Try to keep shorter than two lines and avoid qualifiers. Titles can be 24px for the web. See example in "Maps" section.</t>
-  </si>
-  <si>
     <t>Always horizontal, above the top axis label. If needed, include units or multipliers in parenthesis. For example: Price (2014 dollars)</t>
   </si>
   <si>
@@ -978,6 +975,9 @@
       </rPr>
       <t>” as well as any statistical significance indicators.</t>
     </r>
+  </si>
+  <si>
+    <t>The main point of the chart. Try to keep shorter than two lines and avoid qualifiers. For maps, titles can be 24px for the web. See example in "Maps" section.</t>
   </si>
 </sst>
 </file>
@@ -1914,54 +1914,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1983,7 +1935,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2004,7 +1971,40 @@
     <xf numFmtId="0" fontId="61" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -2209,11 +2209,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-1649448880"/>
-        <c:axId val="-1649444480"/>
+        <c:axId val="1324758288"/>
+        <c:axId val="1324762688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1649448880"/>
+        <c:axId val="1324758288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,7 +2240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1649444480"/>
+        <c:crossAx val="1324762688"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2248,7 +2248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1649444480"/>
+        <c:axId val="1324762688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2285,7 +2285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1649448880"/>
+        <c:crossAx val="1324758288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -3241,8 +3241,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1647152496"/>
-        <c:axId val="-1647147808"/>
+        <c:axId val="1326951280"/>
+        <c:axId val="1326955968"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3515,11 +3515,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1647152496"/>
-        <c:axId val="-1647147808"/>
+        <c:axId val="1326951280"/>
+        <c:axId val="1326955968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1647152496"/>
+        <c:axId val="1326951280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3547,7 +3547,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1647147808"/>
+        <c:crossAx val="1326955968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3557,7 +3557,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1647147808"/>
+        <c:axId val="1326955968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3595,7 +3595,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1647152496"/>
+        <c:crossAx val="1326951280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -4571,8 +4571,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1649174560"/>
-        <c:axId val="-1649169920"/>
+        <c:axId val="1327108496"/>
+        <c:axId val="1327113136"/>
       </c:areaChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -4644,11 +4644,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-1649174560"/>
-        <c:axId val="-1649169920"/>
+        <c:axId val="1327108496"/>
+        <c:axId val="1327113136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1649174560"/>
+        <c:axId val="1327108496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4658,7 +4658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1649169920"/>
+        <c:crossAx val="1327113136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4668,7 +4668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1649169920"/>
+        <c:axId val="1327113136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -4695,7 +4695,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-1649174560"/>
+        <c:crossAx val="1327108496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6788,11 +6788,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1649026720"/>
-        <c:axId val="-1649022800"/>
+        <c:axId val="1327254688"/>
+        <c:axId val="1327258608"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1649026720"/>
+        <c:axId val="1327254688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6802,7 +6802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1649022800"/>
+        <c:crossAx val="1327258608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6811,7 +6811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1649022800"/>
+        <c:axId val="1327258608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6822,7 +6822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1649026720"/>
+        <c:crossAx val="1327254688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7500,11 +7500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1650876848"/>
-        <c:axId val="-1650872480"/>
+        <c:axId val="1327419088"/>
+        <c:axId val="1327423456"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1650876848"/>
+        <c:axId val="1327419088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7527,7 +7527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1650872480"/>
+        <c:crossAx val="1327423456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7537,7 +7537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1650872480"/>
+        <c:axId val="1327423456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7571,7 +7571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1650876848"/>
+        <c:crossAx val="1327419088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7928,8 +7928,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1648901440"/>
-        <c:axId val="-1648896464"/>
+        <c:axId val="1327582400"/>
+        <c:axId val="1327587376"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -8020,11 +8020,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1648887728"/>
-        <c:axId val="-1648891856"/>
+        <c:axId val="1327596112"/>
+        <c:axId val="1327591984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1648901440"/>
+        <c:axId val="1327582400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8055,7 +8055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648896464"/>
+        <c:crossAx val="1327587376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8063,7 +8063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1648896464"/>
+        <c:axId val="1327587376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.3E7"/>
@@ -8102,12 +8102,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648901440"/>
+        <c:crossAx val="1327582400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1648891856"/>
+        <c:axId val="1327591984"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -8134,12 +8134,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648887728"/>
+        <c:crossAx val="1327596112"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1648887728"/>
+        <c:axId val="1327596112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8168,7 +8168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648891856"/>
+        <c:crossAx val="1327591984"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8539,11 +8539,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1648734624"/>
-        <c:axId val="-1648730528"/>
+        <c:axId val="1327749136"/>
+        <c:axId val="1327753232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1648734624"/>
+        <c:axId val="1327749136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8556,7 +8556,7 @@
         <c:spPr>
           <a:ln/>
         </c:spPr>
-        <c:crossAx val="-1648730528"/>
+        <c:crossAx val="1327753232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8566,7 +8566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1648730528"/>
+        <c:axId val="1327753232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8592,7 +8592,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-1648734624"/>
+        <c:crossAx val="1327749136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8955,11 +8955,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1647506368"/>
-        <c:axId val="-1647502448"/>
+        <c:axId val="1327902000"/>
+        <c:axId val="1327905920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1647506368"/>
+        <c:axId val="1327902000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8969,7 +8969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1647502448"/>
+        <c:crossAx val="1327905920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8977,7 +8977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1647502448"/>
+        <c:axId val="1327905920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9003,7 +9003,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-1647506368"/>
+        <c:crossAx val="1327902000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9616,11 +9616,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-1650733600"/>
-        <c:axId val="-1650729648"/>
+        <c:axId val="1281049504"/>
+        <c:axId val="1281053408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1650733600"/>
+        <c:axId val="1281049504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9630,7 +9630,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1650729648"/>
+        <c:crossAx val="1281053408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9638,7 +9638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1650729648"/>
+        <c:axId val="1281053408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9648,7 +9648,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1650733600"/>
+        <c:crossAx val="1281049504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10128,7 +10128,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -10197,11 +10196,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-1649305056"/>
-        <c:axId val="-1649300768"/>
+        <c:axId val="1324876384"/>
+        <c:axId val="1324880672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1649305056"/>
+        <c:axId val="1324876384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10228,7 +10227,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1649300768"/>
+        <c:crossAx val="1324880672"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10236,7 +10235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1649300768"/>
+        <c:axId val="1324880672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-0.08"/>
@@ -10271,7 +10270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1649305056"/>
+        <c:crossAx val="1324876384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.05"/>
@@ -10427,11 +10426,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-1650672800"/>
-        <c:axId val="-1650668944"/>
+        <c:axId val="1328085376"/>
+        <c:axId val="1328089536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1650672800"/>
+        <c:axId val="1328085376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10455,7 +10454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1650668944"/>
+        <c:crossAx val="1328089536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10463,7 +10462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1650668944"/>
+        <c:axId val="1328089536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10489,7 +10488,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-1650672800"/>
+        <c:crossAx val="1328085376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10940,11 +10939,11 @@
         </c:dLbls>
         <c:bubbleScale val="20"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="-1648591712"/>
-        <c:axId val="-1648586976"/>
+        <c:axId val="1328219056"/>
+        <c:axId val="1328223792"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="-1648591712"/>
+        <c:axId val="1328219056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
@@ -10996,12 +10995,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648586976"/>
+        <c:crossAx val="1328223792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1648586976"/>
+        <c:axId val="1328223792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
@@ -11062,7 +11061,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648591712"/>
+        <c:crossAx val="1328219056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11249,11 +11248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="-1648189456"/>
-        <c:axId val="-1648185024"/>
+        <c:axId val="1324968368"/>
+        <c:axId val="1324972672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1648189456"/>
+        <c:axId val="1324968368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11280,7 +11279,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648185024"/>
+        <c:crossAx val="1324972672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11288,7 +11287,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1648185024"/>
+        <c:axId val="1324972672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-20.0"/>
@@ -11315,7 +11314,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-1648189456"/>
+        <c:crossAx val="1324968368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -11819,11 +11818,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="-1651145808"/>
-        <c:axId val="-1651071152"/>
+        <c:axId val="1325128704"/>
+        <c:axId val="1325133040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1651145808"/>
+        <c:axId val="1325128704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11851,7 +11850,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1651071152"/>
+        <c:crossAx val="1325133040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11859,7 +11858,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1651071152"/>
+        <c:axId val="1325133040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11896,7 +11895,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1651145808"/>
+        <c:crossAx val="1325128704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12203,11 +12202,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1648065216"/>
-        <c:axId val="-1648061040"/>
+        <c:axId val="1325239200"/>
+        <c:axId val="1325243376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1648065216"/>
+        <c:axId val="1325239200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12227,7 +12226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648061040"/>
+        <c:crossAx val="1325243376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12235,7 +12234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1648061040"/>
+        <c:axId val="1325243376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12271,7 +12270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1648065216"/>
+        <c:crossAx val="1325239200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12887,11 +12886,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1647938304"/>
-        <c:axId val="-1647934304"/>
+        <c:axId val="1325366176"/>
+        <c:axId val="1325370176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1647938304"/>
+        <c:axId val="1325366176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12901,7 +12900,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1647934304"/>
+        <c:crossAx val="1325370176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12909,7 +12908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1647934304"/>
+        <c:axId val="1325370176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12935,7 +12934,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-1647938304"/>
+        <c:crossAx val="1325366176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13378,11 +13377,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="30"/>
-        <c:axId val="-1647311424"/>
-        <c:axId val="-1647307744"/>
+        <c:axId val="1326559744"/>
+        <c:axId val="1326563424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1647311424"/>
+        <c:axId val="1326559744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13410,7 +13409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1647307744"/>
+        <c:crossAx val="1326563424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13420,7 +13419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1647307744"/>
+        <c:axId val="1326563424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -13457,7 +13456,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1647311424"/>
+        <c:crossAx val="1326559744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -13611,7 +13610,7 @@
                   <c:v>5.0718</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.154199999999982</c:v>
+                  <c:v>6.154199999999981</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7.2366</c:v>
@@ -14543,11 +14542,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1651084528"/>
-        <c:axId val="-1651079936"/>
+        <c:axId val="1326702320"/>
+        <c:axId val="1326706912"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1651084528"/>
+        <c:axId val="1326702320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14575,7 +14574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1651079936"/>
+        <c:crossAx val="1326706912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14585,7 +14584,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1651079936"/>
+        <c:axId val="1326706912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14665,7 +14664,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1651084528"/>
+        <c:crossAx val="1326702320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
@@ -15714,11 +15713,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1647810080"/>
-        <c:axId val="-1647805520"/>
+        <c:axId val="1326798592"/>
+        <c:axId val="1326803152"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1647810080"/>
+        <c:axId val="1326798592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15746,7 +15745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1647805520"/>
+        <c:crossAx val="1326803152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15756,7 +15755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1647805520"/>
+        <c:axId val="1326803152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15792,7 +15791,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1647810080"/>
+        <c:crossAx val="1326798592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
@@ -19507,14 +19506,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -19577,14 +19576,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -19647,14 +19646,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -19771,14 +19770,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -19841,14 +19840,14 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -19917,7 +19916,7 @@
         </a:ln>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:noFill/>
             </a14:hiddenFill>
           </a:ext>
@@ -29001,7 +29000,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29039,7 +29038,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29165,7 +29164,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29351,7 +29350,7 @@
         <cdr:cNvPr id="2" name="XAxisBox">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C44B43-1FA3-4338-AEAF-B20BF5470C27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1C44B43-1FA3-4338-AEAF-B20BF5470C27}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -33917,8 +33916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33990,7 +33989,7 @@
         <v>135</v>
       </c>
       <c r="G7" s="104" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -34036,7 +34035,7 @@
         <v>135</v>
       </c>
       <c r="G9" s="104" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -34082,7 +34081,7 @@
         <v>135</v>
       </c>
       <c r="G11" s="104" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -34151,7 +34150,7 @@
         <v>135</v>
       </c>
       <c r="G14" s="104" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="32" x14ac:dyDescent="0.2">
@@ -40731,27 +40730,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:59" s="14" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="183"/>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="183"/>
-      <c r="M2" s="183"/>
-      <c r="N2" s="183"/>
-      <c r="O2" s="183"/>
-      <c r="P2" s="183"/>
-      <c r="Q2" s="183"/>
-      <c r="R2" s="183"/>
-      <c r="S2" s="183"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
+      <c r="P2" s="167"/>
+      <c r="Q2" s="167"/>
+      <c r="R2" s="167"/>
+      <c r="S2" s="167"/>
       <c r="U2" s="141" t="s">
         <v>42</v>
       </c>
@@ -40774,48 +40773,48 @@
       <c r="AL2" s="126"/>
       <c r="AM2" s="126"/>
       <c r="AN2" s="125"/>
-      <c r="AO2" s="177"/>
-      <c r="AP2" s="177"/>
-      <c r="AQ2" s="177"/>
-      <c r="AR2" s="177"/>
-      <c r="AS2" s="177"/>
-      <c r="AT2" s="177"/>
-      <c r="AU2" s="177"/>
-      <c r="AV2" s="177"/>
-      <c r="AW2" s="177"/>
-      <c r="AX2" s="177"/>
-      <c r="AY2" s="177"/>
-      <c r="AZ2" s="177"/>
-      <c r="BA2" s="177"/>
-      <c r="BB2" s="177"/>
-      <c r="BC2" s="177"/>
-      <c r="BD2" s="177"/>
-      <c r="BE2" s="177"/>
-      <c r="BF2" s="177"/>
-      <c r="BG2" s="177"/>
+      <c r="AO2" s="161"/>
+      <c r="AP2" s="161"/>
+      <c r="AQ2" s="161"/>
+      <c r="AR2" s="161"/>
+      <c r="AS2" s="161"/>
+      <c r="AT2" s="161"/>
+      <c r="AU2" s="161"/>
+      <c r="AV2" s="161"/>
+      <c r="AW2" s="161"/>
+      <c r="AX2" s="161"/>
+      <c r="AY2" s="161"/>
+      <c r="AZ2" s="161"/>
+      <c r="BA2" s="161"/>
+      <c r="BB2" s="161"/>
+      <c r="BC2" s="161"/>
+      <c r="BD2" s="161"/>
+      <c r="BE2" s="161"/>
+      <c r="BF2" s="161"/>
+      <c r="BG2" s="161"/>
     </row>
     <row r="3" spans="1:59" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="183" t="s">
+      <c r="A3" s="167" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="183"/>
-      <c r="H3" s="183"/>
-      <c r="I3" s="183"/>
-      <c r="J3" s="183"/>
-      <c r="K3" s="183"/>
-      <c r="L3" s="183"/>
-      <c r="M3" s="183"/>
-      <c r="N3" s="183"/>
-      <c r="O3" s="183"/>
-      <c r="P3" s="183"/>
-      <c r="Q3" s="183"/>
-      <c r="R3" s="183"/>
-      <c r="S3" s="183"/>
+      <c r="B3" s="167"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="167"/>
+      <c r="K3" s="167"/>
+      <c r="L3" s="167"/>
+      <c r="M3" s="167"/>
+      <c r="N3" s="167"/>
+      <c r="O3" s="167"/>
+      <c r="P3" s="167"/>
+      <c r="Q3" s="167"/>
+      <c r="R3" s="167"/>
+      <c r="S3" s="167"/>
       <c r="U3" s="127"/>
       <c r="V3" s="128"/>
       <c r="W3" s="128"/>
@@ -40876,40 +40875,40 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
       <c r="S4" s="16"/>
-      <c r="U4" s="161" t="s">
+      <c r="U4" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="V4" s="162"/>
-      <c r="W4" s="162"/>
+      <c r="V4" s="182"/>
+      <c r="W4" s="182"/>
       <c r="X4" s="142"/>
-      <c r="Y4" s="161" t="s">
+      <c r="Y4" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="Z4" s="161"/>
+      <c r="Z4" s="173"/>
       <c r="AA4" s="143"/>
-      <c r="AB4" s="161" t="s">
+      <c r="AB4" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="AC4" s="161"/>
+      <c r="AC4" s="173"/>
       <c r="AD4" s="142"/>
-      <c r="AE4" s="161" t="s">
+      <c r="AE4" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="AF4" s="187"/>
-      <c r="AG4" s="187"/>
-      <c r="AH4" s="187"/>
-      <c r="AI4" s="187"/>
+      <c r="AF4" s="176"/>
+      <c r="AG4" s="176"/>
+      <c r="AH4" s="176"/>
+      <c r="AI4" s="176"/>
       <c r="AJ4" s="144"/>
-      <c r="AK4" s="161" t="s">
+      <c r="AK4" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="AL4" s="189"/>
-      <c r="AM4" s="189"/>
-      <c r="AN4" s="189"/>
-      <c r="AO4" s="178"/>
-      <c r="AP4" s="179"/>
-      <c r="AQ4" s="179"/>
-      <c r="AR4" s="179"/>
+      <c r="AL4" s="178"/>
+      <c r="AM4" s="178"/>
+      <c r="AN4" s="178"/>
+      <c r="AO4" s="162"/>
+      <c r="AP4" s="163"/>
+      <c r="AQ4" s="163"/>
+      <c r="AR4" s="163"/>
       <c r="AS4" s="127"/>
       <c r="AT4" s="127"/>
       <c r="AU4" s="127"/>
@@ -40945,41 +40944,41 @@
       <c r="J5" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="184"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="184"/>
+      <c r="K5" s="171"/>
+      <c r="L5" s="171"/>
+      <c r="M5" s="171"/>
+      <c r="N5" s="171"/>
       <c r="O5" s="19"/>
       <c r="P5" s="168" t="s">
         <v>47</v>
       </c>
-      <c r="Q5" s="169"/>
-      <c r="R5" s="169"/>
-      <c r="S5" s="169"/>
-      <c r="U5" s="163"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="U5" s="183"/>
+      <c r="V5" s="183"/>
+      <c r="W5" s="183"/>
       <c r="X5" s="145"/>
-      <c r="Y5" s="185"/>
-      <c r="Z5" s="185"/>
+      <c r="Y5" s="174"/>
+      <c r="Z5" s="174"/>
       <c r="AA5" s="146"/>
-      <c r="AB5" s="185"/>
-      <c r="AC5" s="185"/>
+      <c r="AB5" s="174"/>
+      <c r="AC5" s="174"/>
       <c r="AD5" s="145"/>
-      <c r="AE5" s="188"/>
-      <c r="AF5" s="188"/>
-      <c r="AG5" s="188"/>
-      <c r="AH5" s="188"/>
-      <c r="AI5" s="188"/>
+      <c r="AE5" s="177"/>
+      <c r="AF5" s="177"/>
+      <c r="AG5" s="177"/>
+      <c r="AH5" s="177"/>
+      <c r="AI5" s="177"/>
       <c r="AJ5" s="147"/>
-      <c r="AK5" s="190"/>
-      <c r="AL5" s="190"/>
-      <c r="AM5" s="190"/>
-      <c r="AN5" s="190"/>
-      <c r="AO5" s="180"/>
-      <c r="AP5" s="180"/>
-      <c r="AQ5" s="180"/>
-      <c r="AR5" s="180"/>
+      <c r="AK5" s="179"/>
+      <c r="AL5" s="179"/>
+      <c r="AM5" s="179"/>
+      <c r="AN5" s="179"/>
+      <c r="AO5" s="164"/>
+      <c r="AP5" s="164"/>
+      <c r="AQ5" s="164"/>
+      <c r="AR5" s="164"/>
       <c r="AS5" s="127"/>
       <c r="AT5" s="127"/>
       <c r="AU5" s="127"/>
@@ -40997,57 +40996,57 @@
       <c r="BG5" s="127"/>
     </row>
     <row r="6" spans="1:59" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="174"/>
-      <c r="B6" s="174"/>
+      <c r="A6" s="169"/>
+      <c r="B6" s="169"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="174"/>
-      <c r="E6" s="174"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="174"/>
-      <c r="H6" s="174"/>
+      <c r="G6" s="169"/>
+      <c r="H6" s="169"/>
       <c r="I6" s="20"/>
-      <c r="J6" s="173"/>
-      <c r="K6" s="173"/>
-      <c r="L6" s="173"/>
-      <c r="M6" s="173"/>
-      <c r="N6" s="173"/>
+      <c r="J6" s="172"/>
+      <c r="K6" s="172"/>
+      <c r="L6" s="172"/>
+      <c r="M6" s="172"/>
+      <c r="N6" s="172"/>
       <c r="O6" s="22"/>
-      <c r="P6" s="170"/>
-      <c r="Q6" s="170"/>
-      <c r="R6" s="170"/>
-      <c r="S6" s="170"/>
-      <c r="U6" s="163"/>
-      <c r="V6" s="163"/>
-      <c r="W6" s="163"/>
+      <c r="P6" s="188"/>
+      <c r="Q6" s="188"/>
+      <c r="R6" s="188"/>
+      <c r="S6" s="188"/>
+      <c r="U6" s="183"/>
+      <c r="V6" s="183"/>
+      <c r="W6" s="183"/>
       <c r="X6" s="145"/>
-      <c r="Y6" s="185"/>
-      <c r="Z6" s="185"/>
+      <c r="Y6" s="174"/>
+      <c r="Z6" s="174"/>
       <c r="AA6" s="146"/>
-      <c r="AB6" s="185"/>
-      <c r="AC6" s="185"/>
+      <c r="AB6" s="174"/>
+      <c r="AC6" s="174"/>
       <c r="AD6" s="145"/>
-      <c r="AE6" s="165" t="s">
+      <c r="AE6" s="180" t="s">
         <v>48</v>
       </c>
-      <c r="AF6" s="191"/>
+      <c r="AF6" s="181"/>
       <c r="AG6" s="148"/>
-      <c r="AH6" s="165" t="s">
+      <c r="AH6" s="180" t="s">
         <v>49</v>
       </c>
-      <c r="AI6" s="191"/>
+      <c r="AI6" s="181"/>
       <c r="AJ6" s="148"/>
-      <c r="AK6" s="185" t="s">
+      <c r="AK6" s="174" t="s">
         <v>50</v>
       </c>
-      <c r="AL6" s="185"/>
+      <c r="AL6" s="174"/>
       <c r="AM6" s="148"/>
-      <c r="AN6" s="165" t="s">
+      <c r="AN6" s="180" t="s">
         <v>51</v>
       </c>
-      <c r="AO6" s="166"/>
+      <c r="AO6" s="185"/>
       <c r="AP6" s="139"/>
       <c r="AQ6" s="129"/>
-      <c r="AR6" s="181"/>
+      <c r="AR6" s="165"/>
       <c r="AS6" s="127"/>
       <c r="AT6" s="127"/>
       <c r="AU6" s="127"/>
@@ -41065,57 +41064,57 @@
       <c r="BG6" s="127"/>
     </row>
     <row r="7" spans="1:59" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="174"/>
-      <c r="B7" s="174"/>
+      <c r="A7" s="169"/>
+      <c r="B7" s="169"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="174"/>
-      <c r="E7" s="174"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="174"/>
-      <c r="H7" s="174"/>
+      <c r="G7" s="169"/>
+      <c r="H7" s="169"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="171" t="s">
+      <c r="J7" s="189" t="s">
         <v>48</v>
       </c>
-      <c r="K7" s="172"/>
+      <c r="K7" s="190"/>
       <c r="L7" s="23"/>
-      <c r="M7" s="171" t="s">
+      <c r="M7" s="189" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="172"/>
+      <c r="N7" s="190"/>
       <c r="O7" s="23"/>
-      <c r="P7" s="174" t="s">
+      <c r="P7" s="169" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="174"/>
+      <c r="Q7" s="169"/>
       <c r="R7" s="23"/>
-      <c r="S7" s="174" t="s">
+      <c r="S7" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="U7" s="164"/>
-      <c r="V7" s="164"/>
-      <c r="W7" s="164"/>
+      <c r="U7" s="184"/>
+      <c r="V7" s="184"/>
+      <c r="W7" s="184"/>
       <c r="X7" s="145"/>
-      <c r="Y7" s="186"/>
-      <c r="Z7" s="186"/>
+      <c r="Y7" s="175"/>
+      <c r="Z7" s="175"/>
       <c r="AA7" s="146"/>
-      <c r="AB7" s="186"/>
-      <c r="AC7" s="186"/>
+      <c r="AB7" s="175"/>
+      <c r="AC7" s="175"/>
       <c r="AD7" s="145"/>
-      <c r="AE7" s="188"/>
-      <c r="AF7" s="188"/>
+      <c r="AE7" s="177"/>
+      <c r="AF7" s="177"/>
       <c r="AG7" s="149"/>
-      <c r="AH7" s="188"/>
-      <c r="AI7" s="188"/>
+      <c r="AH7" s="177"/>
+      <c r="AI7" s="177"/>
       <c r="AJ7" s="148"/>
-      <c r="AK7" s="186"/>
-      <c r="AL7" s="186"/>
+      <c r="AK7" s="175"/>
+      <c r="AL7" s="175"/>
       <c r="AM7" s="149"/>
-      <c r="AN7" s="167"/>
-      <c r="AO7" s="164"/>
+      <c r="AN7" s="186"/>
+      <c r="AO7" s="184"/>
       <c r="AP7" s="140"/>
       <c r="AQ7" s="130"/>
-      <c r="AR7" s="182"/>
+      <c r="AR7" s="166"/>
       <c r="AS7" s="127"/>
       <c r="AT7" s="127"/>
       <c r="AU7" s="127"/>
@@ -41133,25 +41132,25 @@
       <c r="BG7" s="127"/>
     </row>
     <row r="8" spans="1:59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="175"/>
-      <c r="B8" s="175"/>
+      <c r="A8" s="170"/>
+      <c r="B8" s="170"/>
       <c r="C8" s="20"/>
-      <c r="D8" s="175"/>
-      <c r="E8" s="175"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="170"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="175"/>
-      <c r="H8" s="175"/>
+      <c r="G8" s="170"/>
+      <c r="H8" s="170"/>
       <c r="I8" s="20"/>
-      <c r="J8" s="173"/>
-      <c r="K8" s="173"/>
+      <c r="J8" s="172"/>
+      <c r="K8" s="172"/>
       <c r="L8" s="24"/>
-      <c r="M8" s="173"/>
-      <c r="N8" s="173"/>
+      <c r="M8" s="172"/>
+      <c r="N8" s="172"/>
       <c r="O8" s="23"/>
-      <c r="P8" s="175"/>
-      <c r="Q8" s="175"/>
+      <c r="P8" s="170"/>
+      <c r="Q8" s="170"/>
       <c r="R8" s="24"/>
-      <c r="S8" s="176"/>
+      <c r="S8" s="191"/>
       <c r="U8" s="127"/>
       <c r="V8" s="127"/>
       <c r="W8" s="127"/>
@@ -44178,6 +44177,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="U4:W7"/>
+    <mergeCell ref="AN6:AO7"/>
+    <mergeCell ref="P5:S6"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="S7:S8"/>
     <mergeCell ref="AO2:BG2"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AR6:AR7"/>
@@ -44194,13 +44200,6 @@
     <mergeCell ref="AE6:AF7"/>
     <mergeCell ref="AH6:AI7"/>
     <mergeCell ref="AK6:AL7"/>
-    <mergeCell ref="U4:W7"/>
-    <mergeCell ref="AN6:AO7"/>
-    <mergeCell ref="P5:S6"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="S7:S8"/>
   </mergeCells>
   <phoneticPr fontId="30" type="noConversion"/>
   <conditionalFormatting sqref="Z9:Z21">

</xml_diff>